<commit_message>
update the report for determinism
</commit_message>
<xml_diff>
--- a/tests/traces/h100/google_owlv2-large-patch14-ensemble__1016001_perf_report.xlsx
+++ b/tests/traces/h100/google_owlv2-large-patch14-ensemble__1016001_perf_report.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="gpu_timeline" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ops_summary_by_category" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="ops_summary" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="ops_unique_args" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="GEMM" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="CONV_fwd" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="UnaryElementwise" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="BinaryElementwise" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gpu_timeline" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ops_summary_by_category" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ops_summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ops_unique_args" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GEMM" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CONV_fwd" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UnaryElementwise" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BinaryElementwise" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1527,12 +1527,12 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::cunn_SoftMaxForward&lt;8, c10::BFloat16, float, c10::BFloat16, at::native::(anonymous namespace)::SoftMaxForwardEpilogue&gt;(c10::BFloat16*, c10::BFloat16 const*, int)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(262422.467), 'mean_duration_us': np.float64(2186.8538916666666), 'median_duration_us': np.float64(2170.955), 'std_dev_duration_us': np.float64(52.45910857528236), 'min_duration_us': np.float64(2146.764), 'max_duration_us': np.float64(2395.817)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::cunn_SoftMaxForward&lt;8, c10::BFloat16, float, c10::BFloat16, at::native::(anonymous namespace)::SoftMaxForwardEpilogue&gt;(c10::BFloat16*, c10::BFloat16 const*, int)', 'stream': 7, 'count': 120, 'total_duration_us': 262422.467, 'mean_duration_us': 2186.8538916666666, 'median_duration_us': 2170.955, 'std_dev_duration_us': 52.45910857528236, 'min_duration_us': 2146.764, 'max_duration_us': 2395.817}]</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::cunn_SoftMaxForward&lt;8, c...', 'stream': 7, 'mean_duration_us': np.float64(2186.85)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::cunn_SoftMaxForward&lt;8, c...', 'stream': 7, 'mean_duration_us': 2186.85}]</t>
         </is>
       </c>
       <c r="P2" t="n">
@@ -1594,12 +1594,12 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(130015.7), 'mean_duration_us': np.float64(1083.4641666666666), 'median_duration_us': np.float64(1082.965), 'std_dev_duration_us': np.float64(3.932529614919927), 'min_duration_us': np.float64(1075.574), 'max_duration_us': np.float64(1096.694)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': 130015.7, 'mean_duration_us': 1083.4641666666666, 'median_duration_us': 1082.965, 'std_dev_duration_us': 3.932529614919927, 'min_duration_us': 1075.574, 'max_duration_us': 1096.694}]</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_25...', 'stream': 7, 'mean_duration_us': np.float64(1083.46)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_25...', 'stream': 7, 'mean_duration_us': 1083.46}]</t>
         </is>
       </c>
       <c r="P3" t="n">
@@ -1661,12 +1661,12 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(99311.41), 'mean_duration_us': np.float64(827.5950833333334), 'median_duration_us': np.float64(826.9205), 'std_dev_duration_us': np.float64(2.9474507419783706), 'min_duration_us': np.float64(825.432), 'max_duration_us': np.float64(851.8)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': 99311.41, 'mean_duration_us': 827.5950833333334, 'median_duration_us': 826.9205, 'std_dev_duration_us': 2.9474507419783706, 'min_duration_us': 825.432, 'max_duration_us': 851.8}]</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_12...', 'stream': 7, 'mean_duration_us': np.float64(827.6)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_12...', 'stream': 7, 'mean_duration_us': 827.6}]</t>
         </is>
       </c>
       <c r="P4" t="n">
@@ -1728,12 +1728,12 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 480, 'total_duration_us': np.float64(449.6640000000001), 'mean_duration_us': np.float64(0.9368000000000002), 'median_duration_us': np.float64(0.96), 'std_dev_duration_us': np.float64(0.14700191892171566), 'min_duration_us': np.float64(0.767), 'max_duration_us': np.float64(1.408)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 480, 'total_duration_us': np.float64(10035.521), 'mean_duration_us': np.float64(20.90733541666667), 'median_duration_us': np.float64(20.912), 'std_dev_duration_us': np.float64(0.2994497001373127), 'min_duration_us': np.float64(20.256), 'max_duration_us': np.float64(22.015)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 480, 'total_duration_us': 449.6640000000001, 'mean_duration_us': 0.9368000000000002, 'median_duration_us': 0.96, 'std_dev_duration_us': 0.14700191892171566, 'min_duration_us': 0.767, 'max_duration_us': 1.408}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 480, 'total_duration_us': 10035.521, 'mean_duration_us': 20.90733541666667, 'median_duration_us': 20.912, 'std_dev_duration_us': 0.2994497001373127, 'min_duration_us': 20.256, 'max_duration_us': 22.015}]</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.94)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(20.91)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.94}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 20.91}]</t>
         </is>
       </c>
       <c r="P5" t="n">
@@ -1795,12 +1795,12 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8133.554), 'mean_duration_us': np.float64(1626.7108), 'median_duration_us': np.float64(347.196), 'std_dev_duration_us': np.float64(1579.6924965375256), 'min_duration_us': np.float64(325.565), 'max_duration_us': np.float64(3620.445)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 8133.554, 'mean_duration_us': 1626.7108, 'median_duration_us': 347.196, 'std_dev_duration_us': 1579.6924965375256, 'min_duration_us': 325.565, 'max_duration_us': 3620.445}]</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(1626.71)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 1626.71}]</t>
         </is>
       </c>
       <c r="P6" t="n">
@@ -1862,12 +1862,12 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(115.61200000000002), 'mean_duration_us': np.float64(0.9634333333333335), 'median_duration_us': np.float64(0.96), 'std_dev_duration_us': np.float64(0.18370559478566667), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(1.6)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(7766.737), 'mean_duration_us': np.float64(64.72280833333333), 'median_duration_us': np.float64(64.639), 'std_dev_duration_us': np.float64(0.5570301951096441), 'min_duration_us': np.float64(63.711), 'max_duration_us': np.float64(65.951)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': 115.61200000000002, 'mean_duration_us': 0.9634333333333335, 'median_duration_us': 0.96, 'std_dev_duration_us': 0.18370559478566667, 'min_duration_us': 0.768, 'max_duration_us': 1.6}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': 7766.737, 'mean_duration_us': 64.72280833333333, 'median_duration_us': 64.639, 'std_dev_duration_us': 0.5570301951096441, 'min_duration_us': 63.711, 'max_duration_us': 65.951}]</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.96)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(64.72)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.96}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 64.72}]</t>
         </is>
       </c>
       <c r="P7" t="n">
@@ -1929,12 +1929,12 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(116.09), 'mean_duration_us': np.float64(0.9674166666666667), 'median_duration_us': np.float64(0.96), 'std_dev_duration_us': np.float64(0.15527371441711854), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(1.568)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(6884.5689999999995), 'mean_duration_us': np.float64(57.37140833333333), 'median_duration_us': np.float64(57.344), 'std_dev_duration_us': np.float64(0.31250691981227396), 'min_duration_us': np.float64(56.639), 'max_duration_us': np.float64(58.048)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': 116.09, 'mean_duration_us': 0.9674166666666667, 'median_duration_us': 0.96, 'std_dev_duration_us': 0.15527371441711854, 'min_duration_us': 0.768, 'max_duration_us': 1.568}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': 6884.5689999999995, 'mean_duration_us': 57.37140833333333, 'median_duration_us': 57.344, 'std_dev_duration_us': 0.31250691981227396, 'min_duration_us': 56.639, 'max_duration_us': 58.048}]</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.97)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(57.37)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.97}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 57.37}]</t>
         </is>
       </c>
       <c r="P8" t="n">
@@ -1996,12 +1996,12 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(5223.73), 'mean_duration_us': np.float64(43.53108333333333), 'median_duration_us': np.float64(43.3595), 'std_dev_duration_us': np.float64(0.6410638629566389), 'min_duration_us': np.float64(42.656), 'max_duration_us': np.float64(44.704)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 5223.73, 'mean_duration_us': 43.53108333333333, 'median_duration_us': 43.3595, 'std_dev_duration_us': 0.6410638629566389, 'min_duration_us': 42.656, 'max_duration_us': 44.704}]</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(43.53)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 43.53}]</t>
         </is>
       </c>
       <c r="P9" t="n">
@@ -2063,12 +2063,12 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 360, 'total_duration_us': np.float64(5038.033), 'mean_duration_us': np.float64(13.994536111111112), 'median_duration_us': np.float64(13.152), 'std_dev_duration_us': np.float64(1.3500063184322875), 'min_duration_us': np.float64(12.736), 'max_duration_us': np.float64(16.288)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 360, 'total_duration_us': 5038.033, 'mean_duration_us': 13.994536111111112, 'median_duration_us': 13.152, 'std_dev_duration_us': 1.3500063184322875, 'min_duration_us': 12.736, 'max_duration_us': 16.288}]</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(13.99)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 13.99}]</t>
         </is>
       </c>
       <c r="P10" t="n">
@@ -2130,12 +2130,12 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(3988.498), 'mean_duration_us': np.float64(33.23748333333334), 'median_duration_us': np.float64(33.055), 'std_dev_duration_us': np.float64(0.39268874407375365), 'min_duration_us': np.float64(32.8), 'max_duration_us': np.float64(34.272)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 3988.498, 'mean_duration_us': 33.23748333333334, 'median_duration_us': 33.055, 'std_dev_duration_us': 0.39268874407375365, 'min_duration_us': 32.8, 'max_duration_us': 34.272}]</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': np.float64(33.24)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': 33.24}]</t>
         </is>
       </c>
       <c r="P11" t="n">
@@ -2197,12 +2197,12 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 250, 'total_duration_us': np.float64(3701.084), 'mean_duration_us': np.float64(14.804336), 'median_duration_us': np.float64(14.56), 'std_dev_duration_us': np.float64(0.5479889406767253), 'min_duration_us': np.float64(13.952), 'max_duration_us': np.float64(15.807)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 250, 'total_duration_us': 3701.084, 'mean_duration_us': 14.804336, 'median_duration_us': 14.56, 'std_dev_duration_us': 0.5479889406767253, 'min_duration_us': 13.952, 'max_duration_us': 15.807}]</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': np.float64(14.8)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': 14.8}]</t>
         </is>
       </c>
       <c r="P12" t="n">
@@ -2264,12 +2264,12 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(3687.3240000000005), 'mean_duration_us': np.float64(30.727700000000006), 'median_duration_us': np.float64(30.591), 'std_dev_duration_us': np.float64(0.3214868737600341), 'min_duration_us': np.float64(30.336), 'max_duration_us': np.float64(31.711)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 3687.3240000000005, 'mean_duration_us': 30.727700000000006, 'median_duration_us': 30.591, 'std_dev_duration_us': 0.3214868737600341, 'min_duration_us': 30.336, 'max_duration_us': 31.711}]</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(30.73)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 30.73}]</t>
         </is>
       </c>
       <c r="P13" t="n">
@@ -2331,12 +2331,12 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(2338.761), 'mean_duration_us': np.float64(467.7522), 'median_duration_us': np.float64(464.252), 'std_dev_duration_us': np.float64(11.281809454161158), 'min_duration_us': np.float64(454.556), 'max_duration_us': np.float64(487.899)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 2338.761, 'mean_duration_us': 467.7522, 'median_duration_us': 464.252, 'std_dev_duration_us': 11.281809454161158, 'min_duration_us': 454.556, 'max_duration_us': 487.899}]</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(467.75)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 467.75}]</t>
         </is>
       </c>
       <c r="P14" t="n">
@@ -2398,12 +2398,12 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(2324.394), 'mean_duration_us': np.float64(464.87879999999996), 'median_duration_us': np.float64(472.188), 'std_dev_duration_us': np.float64(19.601893596282974), 'min_duration_us': np.float64(436.444), 'max_duration_us': np.float64(489.34)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 2324.394, 'mean_duration_us': 464.87879999999996, 'median_duration_us': 472.188, 'std_dev_duration_us': 19.601893596282974, 'min_duration_us': 436.444, 'max_duration_us': 489.34}]</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(464.88)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 464.88}]</t>
         </is>
       </c>
       <c r="P15" t="n">
@@ -2465,12 +2465,12 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 245, 'total_duration_us': np.float64(2317.353), 'mean_duration_us': np.float64(9.458583673469388), 'median_duration_us': np.float64(9.472), 'std_dev_duration_us': np.float64(0.3348456698101192), 'min_duration_us': np.float64(8.576), 'max_duration_us': np.float64(10.849)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 245, 'total_duration_us': 2317.353, 'mean_duration_us': 9.458583673469388, 'median_duration_us': 9.472, 'std_dev_duration_us': 0.3348456698101192, 'min_duration_us': 8.576, 'max_duration_us': 10.849}]</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(9.46)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 9.46}]</t>
         </is>
       </c>
       <c r="P16" t="n">
@@ -2532,12 +2532,12 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(1873.8329999999999), 'mean_duration_us': np.float64(15.615274999999999), 'median_duration_us': np.float64(15.584), 'std_dev_duration_us': np.float64(0.1854254999768552), 'min_duration_us': np.float64(15.264), 'max_duration_us': np.float64(16.384)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': 1873.8329999999999, 'mean_duration_us': 15.615274999999999, 'median_duration_us': 15.584, 'std_dev_duration_us': 0.1854254999768552, 'min_duration_us': 15.264, 'max_duration_us': 16.384}]</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(15.62)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 15.62}]</t>
         </is>
       </c>
       <c r="P17" t="n">
@@ -2599,12 +2599,12 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(1627.952), 'mean_duration_us': np.float64(325.5904), 'median_duration_us': np.float64(333.501), 'std_dev_duration_us': np.float64(11.368233417730304), 'min_duration_us': np.float64(304.989), 'max_duration_us': np.float64(334.205)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': 1627.952, 'mean_duration_us': 325.5904, 'median_duration_us': 333.501, 'std_dev_duration_us': 11.368233417730304, 'min_duration_us': 304.989, 'max_duration_us': 334.205}]</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(325.59)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 325.59}]</t>
         </is>
       </c>
       <c r="P18" t="n">
@@ -2666,12 +2666,12 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 240, 'total_duration_us': np.float64(1579.851), 'mean_duration_us': np.float64(6.5827125), 'median_duration_us': np.float64(6.592), 'std_dev_duration_us': np.float64(0.13116311667951205), 'min_duration_us': np.float64(6.303), 'max_duration_us': np.float64(6.975)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 240, 'total_duration_us': 1579.851, 'mean_duration_us': 6.5827125, 'median_duration_us': 6.592, 'std_dev_duration_us': 0.13116311667951205, 'min_duration_us': 6.303, 'max_duration_us': 6.975}]</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': np.float64(6.58)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': 6.58}]</t>
         </is>
       </c>
       <c r="P19" t="n">
@@ -2733,12 +2733,12 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(28.127000000000002), 'mean_duration_us': np.float64(5.625400000000001), 'median_duration_us': np.float64(5.664), 'std_dev_duration_us': np.float64(0.08941498755801505), 'min_duration_us': np.float64(5.503), 'max_duration_us': np.float64(5.728)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(222.207), 'mean_duration_us': np.float64(44.4414), 'median_duration_us': np.float64(44.384), 'std_dev_duration_us': np.float64(0.1792647204555328), 'min_duration_us': np.float64(44.224), 'max_duration_us': np.float64(44.768)}, {'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(10.85), 'mean_duration_us': np.float64(2.17), 'median_duration_us': np.float64(2.176), 'std_dev_duration_us': np.float64(0.013007690033207267), 'min_duration_us': np.float64(2.144), 'max_duration_us': np.float64(2.177)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(58.303000000000004), 'mean_duration_us': np.float64(11.6606), 'median_duration_us': np.float64(11.679), 'std_dev_duration_us': np.float64(0.15088485676170435), 'min_duration_us': np.float64(11.424), 'max_duration_us': np.float64(11.872)}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8&gt;(cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8::Params)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(982.9660000000001), 'mean_duration_us': np.float64(196.59320000000002), 'median_duration_us': np.float64(196.542), 'std_dev_duration_us': np.float64(0.4292092263686784), 'min_duration_us': np.float64(195.966), 'max_duration_us': np.float64(197.245)}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16, __nv_bfloat16, float, true, false, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nhwc2nchw_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(48.35), 'mean_duration_us': np.float64(9.67), 'median_duration_us': np.float64(9.663), 'std_dev_duration_us': np.float64(0.0547539952880155), 'min_duration_us': np.float64(9.6), 'max_duration_us': np.float64(9.759)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': 28.127000000000002, 'mean_duration_us': 5.625400000000001, 'median_duration_us': 5.664, 'std_dev_duration_us': 0.08941498755801505, 'min_duration_us': 5.503, 'max_duration_us': 5.728}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 222.207, 'mean_duration_us': 44.4414, 'median_duration_us': 44.384, 'std_dev_duration_us': 0.1792647204555328, 'min_duration_us': 44.224, 'max_duration_us': 44.768}, {'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': 10.85, 'mean_duration_us': 2.17, 'median_duration_us': 2.176, 'std_dev_duration_us': 0.013007690033207267, 'min_duration_us': 2.144, 'max_duration_us': 2.177}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 58.303000000000004, 'mean_duration_us': 11.6606, 'median_duration_us': 11.679, 'std_dev_duration_us': 0.15088485676170435, 'min_duration_us': 11.424, 'max_duration_us': 11.872}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8&gt;(cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8::Params)', 'stream': 7, 'count': 5, 'total_duration_us': 982.9660000000001, 'mean_duration_us': 196.59320000000002, 'median_duration_us': 196.542, 'std_dev_duration_us': 0.4292092263686784, 'min_duration_us': 195.966, 'max_duration_us': 197.245}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16, __nv_bfloat16, float, true, false, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nhwc2nchw_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 48.35, 'mean_duration_us': 9.67, 'median_duration_us': 9.663, 'std_dev_duration_us': 0.0547539952880155, 'min_duration_us': 9.6, 'max_duration_us': 9.759}]</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(5.63)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': np.float64(44.44)}, {'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(2.17)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': np.float64(11.66)}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop...', 'stream': 7, 'mean_duration_us': np.float64(196.59)}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': np.float64(9.67)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 5.63}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': 44.44}, {'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 2.17}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': 11.66}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop...', 'stream': 7, 'mean_duration_us': 196.59}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': 9.67}]</t>
         </is>
       </c>
       <c r="P20" t="n">
@@ -2800,12 +2800,12 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(934.809), 'mean_duration_us': np.float64(7.790075), 'median_duration_us': np.float64(7.776), 'std_dev_duration_us': np.float64(0.06863528763204346), 'min_duration_us': np.float64(7.711), 'max_duration_us': np.float64(8.032)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 934.809, 'mean_duration_us': 7.790075, 'median_duration_us': 7.776, 'std_dev_duration_us': 0.06863528763204346, 'min_duration_us': 7.711, 'max_duration_us': 8.032}]</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(7.79)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 7.79}]</t>
         </is>
       </c>
       <c r="P21" t="n">
@@ -2867,12 +2867,12 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(385.4959999999999), 'mean_duration_us': np.float64(6.424933333333332), 'median_duration_us': np.float64(6.336), 'std_dev_duration_us': np.float64(0.19279919317489072), 'min_duration_us': np.float64(6.239), 'max_duration_us': np.float64(6.912)}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, __nv_bfloat16, float, __nv_bfloat16, true, true, false&gt;(cublasLt::cublasSplitKParams&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, float const*, float const*, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, void*, long, float*, int*)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(140.35000000000002), 'mean_duration_us': np.float64(2.339166666666667), 'median_duration_us': np.float64(2.336), 'std_dev_duration_us': np.float64(0.037292164801142315), 'min_duration_us': np.float64(2.272), 'max_duration_us': np.float64(2.496)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 385.4959999999999, 'mean_duration_us': 6.424933333333332, 'median_duration_us': 6.336, 'std_dev_duration_us': 0.19279919317489072, 'min_duration_us': 6.239, 'max_duration_us': 6.912}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, __nv_bfloat16, float, __nv_bfloat16, true, true, false&gt;(cublasLt::cublasSplitKParams&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, float const*, float const*, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, void*, long, float*, int*)', 'stream': 7, 'count': 60, 'total_duration_us': 140.35000000000002, 'mean_duration_us': 2.339166666666667, 'median_duration_us': 2.336, 'std_dev_duration_us': 0.037292164801142315, 'min_duration_us': 2.272, 'max_duration_us': 2.496}]</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': np.float64(6.42)}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': np.float64(2.34)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': 6.42}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': 2.34}]</t>
         </is>
       </c>
       <c r="P22" t="n">
@@ -2934,12 +2934,12 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 180, 'total_duration_us': np.float64(457.9199999999999), 'mean_duration_us': np.float64(2.5439999999999996), 'median_duration_us': np.float64(2.4645), 'std_dev_duration_us': np.float64(0.22104903930525865), 'min_duration_us': np.float64(2.24), 'max_duration_us': np.float64(3.232)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 180, 'total_duration_us': 457.9199999999999, 'mean_duration_us': 2.5439999999999996, 'median_duration_us': 2.4645, 'std_dev_duration_us': 0.22104903930525865, 'min_duration_us': 2.24, 'max_duration_us': 3.232}]</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.54)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.54}]</t>
         </is>
       </c>
       <c r="P23" t="n">
@@ -3001,12 +3001,12 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 125, 'total_duration_us': np.float64(451.14099999999996), 'mean_duration_us': np.float64(3.6091279999999997), 'median_duration_us': np.float64(3.584), 'std_dev_duration_us': np.float64(0.16081094370719926), 'min_duration_us': np.float64(3.328), 'max_duration_us': np.float64(4.096)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 125, 'total_duration_us': 451.14099999999996, 'mean_duration_us': 3.6091279999999997, 'median_duration_us': 3.584, 'std_dev_duration_us': 0.16081094370719926, 'min_duration_us': 3.328, 'max_duration_us': 4.096}]</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': np.float64(3.61)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': 3.61}]</t>
         </is>
       </c>
       <c r="P24" t="n">
@@ -3068,12 +3068,12 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 20, 'total_duration_us': np.float64(17.248), 'mean_duration_us': np.float64(0.8624), 'median_duration_us': np.float64(0.8), 'std_dev_duration_us': np.float64(0.13365305832639968), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(1.248)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 20, 'total_duration_us': np.float64(414.7149999999999), 'mean_duration_us': np.float64(20.735749999999996), 'median_duration_us': np.float64(20.768), 'std_dev_duration_us': np.float64(0.42032010123238245), 'min_duration_us': np.float64(19.936), 'max_duration_us': np.float64(21.279)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 20, 'total_duration_us': 17.248, 'mean_duration_us': 0.8624, 'median_duration_us': 0.8, 'std_dev_duration_us': 0.13365305832639968, 'min_duration_us': 0.768, 'max_duration_us': 1.248}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 20, 'total_duration_us': 414.7149999999999, 'mean_duration_us': 20.735749999999996, 'median_duration_us': 20.768, 'std_dev_duration_us': 0.42032010123238245, 'min_duration_us': 19.936, 'max_duration_us': 21.279}]</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.86)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(20.74)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.86}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 20.74}]</t>
         </is>
       </c>
       <c r="P25" t="n">
@@ -3135,12 +3135,12 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(422.845), 'mean_duration_us': np.float64(7.047416666666667), 'median_duration_us': np.float64(6.976), 'std_dev_duration_us': np.float64(0.17790056133194818), 'min_duration_us': np.float64(6.752), 'max_duration_us': np.float64(7.52)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 422.845, 'mean_duration_us': 7.047416666666667, 'median_duration_us': 6.976, 'std_dev_duration_us': 0.17790056133194818, 'min_duration_us': 6.752, 'max_duration_us': 7.52}]</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': np.float64(7.05)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': 7.05}]</t>
         </is>
       </c>
       <c r="P26" t="n">
@@ -3202,12 +3202,12 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(287.13699999999994), 'mean_duration_us': np.float64(2.392808333333333), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.24387456802740948), 'min_duration_us': np.float64(1.984), 'max_duration_us': np.float64(2.913)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': 287.13699999999994, 'mean_duration_us': 2.392808333333333, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.24387456802740948, 'min_duration_us': 1.984, 'max_duration_us': 2.913}]</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.39)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.39}]</t>
         </is>
       </c>
       <c r="P27" t="n">
@@ -3269,12 +3269,12 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::CatArrayBatchedCopy&lt;at::native::(anonymous namespace)::OpaqueType&lt;2u&gt;, unsigned int, 3, 64, 64&gt;(at::native::(anonymous namespace)::OpaqueType&lt;2u&gt;*, at::native::(anonymous namespace)::CatArrInputTensorMetadata&lt;at::native::(anonymous namespace)::OpaqueType&lt;2u&gt;, unsigned int, 64, 64&gt;, at::native::(anonymous namespace)::TensorSizeStride&lt;unsigned int, 4u&gt;, int, unsigned int)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(219.806), 'mean_duration_us': np.float64(43.961200000000005), 'median_duration_us': np.float64(43.712), 'std_dev_duration_us': np.float64(0.48020553932665044), 'min_duration_us': np.float64(43.551), 'max_duration_us': np.float64(44.799)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::CatArrayBatchedCopy&lt;at::native::(anonymous namespace)::OpaqueType&lt;2u&gt;, unsigned int, 3, 64, 64&gt;(at::native::(anonymous namespace)::OpaqueType&lt;2u&gt;*, at::native::(anonymous namespace)::CatArrInputTensorMetadata&lt;at::native::(anonymous namespace)::OpaqueType&lt;2u&gt;, unsigned int, 64, 64&gt;, at::native::(anonymous namespace)::TensorSizeStride&lt;unsigned int, 4u&gt;, int, unsigned int)', 'stream': 7, 'count': 5, 'total_duration_us': 219.806, 'mean_duration_us': 43.961200000000005, 'median_duration_us': 43.712, 'std_dev_duration_us': 0.48020553932665044, 'min_duration_us': 43.551, 'max_duration_us': 44.799}]</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::CatArrayBatchedCopy&lt;at::...', 'stream': 7, 'mean_duration_us': np.float64(43.96)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::CatArrayBatchedCopy&lt;at::...', 'stream': 7, 'mean_duration_us': 43.96}]</t>
         </is>
       </c>
       <c r="P28" t="n">
@@ -3336,12 +3336,12 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectLargeIndex&lt;c10::BFloat16, long, unsigned int, 2, 2, -2, true&gt;(at::cuda::detail::TensorInfo&lt;c10::BFloat16, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;c10::BFloat16 const, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;long const, unsigned int&gt;, int, int, unsigned int, unsigned int, long)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(195.071), 'mean_duration_us': np.float64(39.0142), 'median_duration_us': np.float64(39.072), 'std_dev_duration_us': np.float64(0.2134070289376613), 'min_duration_us': np.float64(38.624), 'max_duration_us': np.float64(39.231)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectLargeIndex&lt;c10::BFloat16, long, unsigned int, 2, 2, -2, true&gt;(at::cuda::detail::TensorInfo&lt;c10::BFloat16, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;c10::BFloat16 const, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;long const, unsigned int&gt;, int, int, unsigned int, unsigned int, long)', 'stream': 7, 'count': 5, 'total_duration_us': 195.071, 'mean_duration_us': 39.0142, 'median_duration_us': 39.072, 'std_dev_duration_us': 0.2134070289376613, 'min_duration_us': 38.624, 'max_duration_us': 39.231}]</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectLargeIndex&lt;c1...', 'stream': 7, 'mean_duration_us': np.float64(39.01)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectLargeIndex&lt;c1...', 'stream': 7, 'mean_duration_us': 39.01}]</t>
         </is>
       </c>
       <c r="P29" t="n">
@@ -3403,12 +3403,12 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 125, 'total_duration_us': np.float64(187.747), 'mean_duration_us': np.float64(1.5019760000000002), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.09206636423797784), 'min_duration_us': np.float64(1.344), 'max_duration_us': np.float64(1.633)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 125, 'total_duration_us': 187.747, 'mean_duration_us': 1.5019760000000002, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.09206636423797784, 'min_duration_us': 1.344, 'max_duration_us': 1.633}]</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.5)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.5}]</t>
         </is>
       </c>
       <c r="P30" t="n">
@@ -3470,12 +3470,12 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(185.69699999999997), 'mean_duration_us': np.float64(3.0949499999999994), 'median_duration_us': np.float64(3.104), 'std_dev_duration_us': np.float64(0.04453478977159322), 'min_duration_us': np.float64(3.008), 'max_duration_us': np.float64(3.168)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 185.69699999999997, 'mean_duration_us': 3.0949499999999994, 'median_duration_us': 3.104, 'std_dev_duration_us': 0.04453478977159322, 'min_duration_us': 3.008, 'max_duration_us': 3.168}]</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': np.float64(3.09)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': 3.09}]</t>
         </is>
       </c>
       <c r="P31" t="n">
@@ -3537,12 +3537,12 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::GeluCUDAKernelImpl(at::TensorIteratorBase&amp;, at::native::GeluType)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::GeluCUDAKernelImpl(at::TensorIteratorBase&amp;, at::native::GeluType)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 20, 'total_duration_us': np.float64(176.76800000000006), 'mean_duration_us': np.float64(8.838400000000004), 'median_duration_us': np.float64(8.832), 'std_dev_duration_us': np.float64(0.06681796165702758), 'min_duration_us': np.float64(8.704), 'max_duration_us': np.float64(8.992)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::GeluCUDAKernelImpl(at::TensorIteratorBase&amp;, at::native::GeluType)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::GeluCUDAKernelImpl(at::TensorIteratorBase&amp;, at::native::GeluType)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 20, 'total_duration_us': 176.76800000000006, 'mean_duration_us': 8.838400000000004, 'median_duration_us': 8.832, 'std_dev_duration_us': 0.06681796165702758, 'min_duration_us': 8.704, 'max_duration_us': 8.992}]</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Ge...', 'stream': 7, 'mean_duration_us': np.float64(8.84)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Ge...', 'stream': 7, 'mean_duration_us': 8.84}]</t>
         </is>
       </c>
       <c r="P32" t="n">
@@ -3604,12 +3604,12 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(167.428), 'mean_duration_us': np.float64(2.7904666666666667), 'median_duration_us': np.float64(2.816), 'std_dev_duration_us': np.float64(0.037250264726874344), 'min_duration_us': np.float64(2.72), 'max_duration_us': np.float64(2.88)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 167.428, 'mean_duration_us': 2.7904666666666667, 'median_duration_us': 2.816, 'std_dev_duration_us': 0.037250264726874344, 'min_duration_us': 2.72, 'max_duration_us': 2.88}]</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': np.float64(2.79)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': 2.79}]</t>
         </is>
       </c>
       <c r="P33" t="n">
@@ -3671,12 +3671,12 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(163.17200000000005), 'mean_duration_us': np.float64(2.719533333333334), 'median_duration_us': np.float64(2.784), 'std_dev_duration_us': np.float64(0.14011381881250043), 'min_duration_us': np.float64(2.527), 'max_duration_us': np.float64(3.008)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 60, 'total_duration_us': 163.17200000000005, 'mean_duration_us': 2.719533333333334, 'median_duration_us': 2.784, 'std_dev_duration_us': 0.14011381881250043, 'min_duration_us': 2.527, 'max_duration_us': 3.008}]</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.72)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.72}]</t>
         </is>
       </c>
       <c r="P34" t="n">
@@ -3738,12 +3738,12 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 15, 'total_duration_us': np.float64(35.168), 'mean_duration_us': np.float64(2.344533333333333), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.10418372660300108), 'min_duration_us': np.float64(2.176), 'max_duration_us': np.float64(2.56)}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 15, 'total_duration_us': np.float64(83.104), 'mean_duration_us': np.float64(5.540266666666667), 'median_duration_us': np.float64(5.376), 'std_dev_duration_us': np.float64(0.32818683025916123), 'min_duration_us': np.float64(5.152), 'max_duration_us': np.float64(6.176)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 15, 'total_duration_us': 35.168, 'mean_duration_us': 2.344533333333333, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.10418372660300108, 'min_duration_us': 2.176, 'max_duration_us': 2.56}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 15, 'total_duration_us': 83.104, 'mean_duration_us': 5.540266666666667, 'median_duration_us': 5.376, 'std_dev_duration_us': 0.32818683025916123, 'min_duration_us': 5.152, 'max_duration_us': 6.176}]</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.34)}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': np.float64(5.54)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.34}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': 5.54}]</t>
         </is>
       </c>
       <c r="P35" t="n">
@@ -3805,12 +3805,12 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>[{'name': 'void (anonymous namespace)::softmax_warp_forward&lt;c10::BFloat16, c10::BFloat16, float, 3, false, false&gt;(c10::BFloat16*, c10::BFloat16 const*, int, int, int, bool const*, int, bool)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(115.74799999999999), 'mean_duration_us': np.float64(1.9291333333333331), 'median_duration_us': np.float64(1.857), 'std_dev_duration_us': np.float64(0.09073284349610612), 'min_duration_us': np.float64(1.824), 'max_duration_us': np.float64(2.049)}]</t>
+          <t>[{'name': 'void (anonymous namespace)::softmax_warp_forward&lt;c10::BFloat16, c10::BFloat16, float, 3, false, false&gt;(c10::BFloat16*, c10::BFloat16 const*, int, int, int, bool const*, int, bool)', 'stream': 7, 'count': 60, 'total_duration_us': 115.74799999999999, 'mean_duration_us': 1.9291333333333331, 'median_duration_us': 1.857, 'std_dev_duration_us': 0.09073284349610612, 'min_duration_us': 1.824, 'max_duration_us': 2.049}]</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>[{'name': 'void (anonymous namespace)::softmax_warp_forward&lt;c10::BFloat16, ...', 'stream': 7, 'mean_duration_us': np.float64(1.93)}]</t>
+          <t>[{'name': 'void (anonymous namespace)::softmax_warp_forward&lt;c10::BFloat16, ...', 'stream': 7, 'mean_duration_us': 1.93}]</t>
         </is>
       </c>
       <c r="P36" t="n">
@@ -3872,12 +3872,12 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(105.02100000000002), 'mean_duration_us': np.float64(1.7503500000000003), 'median_duration_us': np.float64(1.76), 'std_dev_duration_us': np.float64(0.021235838418422137), 'min_duration_us': np.float64(1.696), 'max_duration_us': np.float64(1.792)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 105.02100000000002, 'mean_duration_us': 1.7503500000000003, 'median_duration_us': 1.76, 'std_dev_duration_us': 0.021235838418422137, 'min_duration_us': 1.696, 'max_duration_us': 1.792}]</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': np.float64(1.75)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': 1.75}]</t>
         </is>
       </c>
       <c r="P37" t="n">
@@ -3939,12 +3939,12 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(94.07899999999998), 'mean_duration_us': np.float64(1.567983333333333), 'median_duration_us': np.float64(1.568), 'std_dev_duration_us': np.float64(0.02925092116308288), 'min_duration_us': np.float64(1.535), 'max_duration_us': np.float64(1.633)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 94.07899999999998, 'mean_duration_us': 1.567983333333333, 'median_duration_us': 1.568, 'std_dev_duration_us': 0.02925092116308288, 'min_duration_us': 1.535, 'max_duration_us': 1.633}]</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(1.57)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 1.57}]</t>
         </is>
       </c>
       <c r="P38" t="n">
@@ -4006,12 +4006,12 @@
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(89.14699999999999), 'mean_duration_us': np.float64(1.4857833333333332), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.016880058912482752), 'min_duration_us': np.float64(1.471), 'max_duration_us': np.float64(1.535)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 89.14699999999999, 'mean_duration_us': 1.4857833333333332, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.016880058912482752, 'min_duration_us': 1.471, 'max_duration_us': 1.535}]</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(1.49)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 1.49}]</t>
         </is>
       </c>
       <c r="P39" t="n">
@@ -4073,12 +4073,12 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warpgroupsize2x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(86.78200000000001), 'mean_duration_us': np.float64(17.3564), 'median_duration_us': np.float64(17.376), 'std_dev_duration_us': np.float64(0.07209049868047837), 'min_duration_us': np.float64(17.215), 'max_duration_us': np.float64(17.408)}]</t>
+          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warpgroupsize2x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 5, 'total_duration_us': 86.78200000000001, 'mean_duration_us': 17.3564, 'median_duration_us': 17.376, 'std_dev_duration_us': 0.07209049868047837, 'min_duration_us': 17.215, 'max_duration_us': 17.408}]</t>
         </is>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(17.36)}]</t>
+          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warp...', 'stream': 7, 'mean_duration_us': 17.36}]</t>
         </is>
       </c>
       <c r="P40" t="n">
@@ -4140,12 +4140,12 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(86.49500000000002), 'mean_duration_us': np.float64(1.4415833333333337), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.10003121040733015), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.568)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 86.49500000000002, 'mean_duration_us': 1.4415833333333337, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.10003121040733015, 'min_duration_us': 1.28, 'max_duration_us': 1.568}]</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(1.44)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 1.44}]</t>
         </is>
       </c>
       <c r="P41" t="n">
@@ -4207,12 +4207,12 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(70.463), 'mean_duration_us': np.float64(14.0926), 'median_duration_us': np.float64(14.079), 'std_dev_duration_us': np.float64(0.1321144957981524), 'min_duration_us': np.float64(13.92), 'max_duration_us': np.float64(14.272)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 70.463, 'mean_duration_us': 14.0926, 'median_duration_us': 14.079, 'std_dev_duration_us': 0.1321144957981524, 'min_duration_us': 13.92, 'max_duration_us': 14.272}]</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': np.float64(14.09)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': 14.09}]</t>
         </is>
       </c>
       <c r="P42" t="n">
@@ -4274,12 +4274,12 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(65.407), 'mean_duration_us': np.float64(13.081399999999999), 'median_duration_us': np.float64(13.088), 'std_dev_duration_us': np.float64(0.058854396607220374), 'min_duration_us': np.float64(13.023), 'max_duration_us': np.float64(13.184)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 65.407, 'mean_duration_us': 13.081399999999999, 'median_duration_us': 13.088, 'std_dev_duration_us': 0.058854396607220374, 'min_duration_us': 13.023, 'max_duration_us': 13.184}]</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(13.08)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 13.08}]</t>
         </is>
       </c>
       <c r="P43" t="n">
@@ -4341,12 +4341,12 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(57.631), 'mean_duration_us': np.float64(11.5262), 'median_duration_us': np.float64(11.552), 'std_dev_duration_us': np.float64(0.0889413289759043), 'min_duration_us': np.float64(11.392), 'max_duration_us': np.float64(11.616)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 57.631, 'mean_duration_us': 11.5262, 'median_duration_us': 11.552, 'std_dev_duration_us': 0.0889413289759043, 'min_duration_us': 11.392, 'max_duration_us': 11.616}]</t>
         </is>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(11.53)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 11.53}]</t>
         </is>
       </c>
       <c r="P44" t="n">
@@ -4408,12 +4408,12 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2&gt;(cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2::Params)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(56.54299999999999), 'mean_duration_us': np.float64(11.308599999999998), 'median_duration_us': np.float64(11.296), 'std_dev_duration_us': np.float64(0.10403768547983014), 'min_duration_us': np.float64(11.168), 'max_duration_us': np.float64(11.487)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2&gt;(cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2::Params)', 'stream': 7, 'count': 5, 'total_duration_us': 56.54299999999999, 'mean_duration_us': 11.308599999999998, 'median_duration_us': 11.296, 'std_dev_duration_us': 0.10403768547983014, 'min_duration_us': 11.168, 'max_duration_us': 11.487}]</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': np.float64(11.31)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': 11.31}]</t>
         </is>
       </c>
       <c r="P45" t="n">
@@ -4475,12 +4475,12 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt; &gt;(at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt;)', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(31.743), 'mean_duration_us': np.float64(3.1742999999999997), 'median_duration_us': np.float64(3.216), 'std_dev_duration_us': np.float64(0.22374005005809758), 'min_duration_us': np.float64(2.848), 'max_duration_us': np.float64(3.551)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt; &gt;(at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt;)', 'stream': 7, 'count': 10, 'total_duration_us': 31.743, 'mean_duration_us': 3.1742999999999997, 'median_duration_us': 3.216, 'std_dev_duration_us': 0.22374005005809758, 'min_duration_us': 2.848, 'max_duration_us': 3.551}]</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10:...', 'stream': 7, 'mean_duration_us': np.float64(3.17)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10:...', 'stream': 7, 'mean_duration_us': 3.17}]</t>
         </is>
       </c>
       <c r="P46" t="n">
@@ -4542,12 +4542,12 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c10::BFloat16, long, unsigned int, 2, 2, -2&gt;(at::cuda::detail::TensorInfo&lt;c10::BFloat16, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;c10::BFloat16 const, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;long const, unsigned int&gt;, int, int, unsigned int, long)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(28.159999999999997), 'mean_duration_us': np.float64(5.632), 'median_duration_us': np.float64(5.792), 'std_dev_duration_us': np.float64(0.2638787600395301), 'min_duration_us': np.float64(5.28), 'max_duration_us': np.float64(5.888)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c10::BFloat16, long, unsigned int, 2, 2, -2&gt;(at::cuda::detail::TensorInfo&lt;c10::BFloat16, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;c10::BFloat16 const, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;long const, unsigned int&gt;, int, int, unsigned int, long)', 'stream': 7, 'count': 5, 'total_duration_us': 28.159999999999997, 'mean_duration_us': 5.632, 'median_duration_us': 5.792, 'std_dev_duration_us': 0.2638787600395301, 'min_duration_us': 5.28, 'max_duration_us': 5.888}]</t>
         </is>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c1...', 'stream': 7, 'mean_duration_us': np.float64(5.63)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c1...', 'stream': 7, 'mean_duration_us': 5.63}]</t>
         </is>
       </c>
       <c r="P47" t="n">
@@ -4609,12 +4609,12 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(26.686999999999998), 'mean_duration_us': np.float64(2.6687), 'median_duration_us': np.float64(2.656), 'std_dev_duration_us': np.float64(0.20862696374150683), 'min_duration_us': np.float64(2.335), 'max_duration_us': np.float64(3.008)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 10, 'total_duration_us': 26.686999999999998, 'mean_duration_us': 2.6687, 'median_duration_us': 2.656, 'std_dev_duration_us': 0.20862696374150683, 'min_duration_us': 2.335, 'max_duration_us': 3.008}]</t>
         </is>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.67)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.67}]</t>
         </is>
       </c>
       <c r="P48" t="n">
@@ -4676,12 +4676,12 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c10::BFloat16, long, unsigned int, 2, 2, -2&gt;(at::cuda::detail::TensorInfo&lt;c10::BFloat16, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;c10::BFloat16 const, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;long const, unsigned int&gt;, int, int, unsigned int, long)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(26.463), 'mean_duration_us': np.float64(5.2926), 'median_duration_us': np.float64(5.216), 'std_dev_duration_us': np.float64(0.19653355947522047), 'min_duration_us': np.float64(5.088), 'max_duration_us': np.float64(5.599)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c10::BFloat16, long, unsigned int, 2, 2, -2&gt;(at::cuda::detail::TensorInfo&lt;c10::BFloat16, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;c10::BFloat16 const, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;long const, unsigned int&gt;, int, int, unsigned int, long)', 'stream': 7, 'count': 5, 'total_duration_us': 26.463, 'mean_duration_us': 5.2926, 'median_duration_us': 5.216, 'std_dev_duration_us': 0.19653355947522047, 'min_duration_us': 5.088, 'max_duration_us': 5.599}]</t>
         </is>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c1...', 'stream': 7, 'mean_duration_us': np.float64(5.29)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c1...', 'stream': 7, 'mean_duration_us': 5.29}]</t>
         </is>
       </c>
       <c r="P49" t="n">
@@ -4743,12 +4743,12 @@
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt; &gt;(at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(24.704), 'mean_duration_us': np.float64(4.9408), 'median_duration_us': np.float64(4.96), 'std_dev_duration_us': np.float64(0.05935115837117255), 'min_duration_us': np.float64(4.832), 'max_duration_us': np.float64(4.992)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt; &gt;(at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 24.704, 'mean_duration_us': 4.9408, 'median_duration_us': 4.96, 'std_dev_duration_us': 0.05935115837117255, 'min_duration_us': 4.832, 'max_duration_us': 4.992}]</t>
         </is>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10:...', 'stream': 7, 'mean_duration_us': np.float64(4.94)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10:...', 'stream': 7, 'mean_duration_us': 4.94}]</t>
         </is>
       </c>
       <c r="P50" t="n">
@@ -4810,12 +4810,12 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(23.615000000000002), 'mean_duration_us': np.float64(4.723000000000001), 'median_duration_us': np.float64(4.704), 'std_dev_duration_us': np.float64(0.06861486719363401), 'min_duration_us': np.float64(4.64), 'max_duration_us': np.float64(4.831)}]</t>
+          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 5, 'total_duration_us': 23.615000000000002, 'mean_duration_us': 4.723000000000001, 'median_duration_us': 4.704, 'std_dev_duration_us': 0.06861486719363401, 'min_duration_us': 4.64, 'max_duration_us': 4.831}]</t>
         </is>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': np.float64(4.72)}]</t>
+          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': 4.72}]</t>
         </is>
       </c>
       <c r="P51" t="n">
@@ -4877,12 +4877,12 @@
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt; &gt;(cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(10.143), 'mean_duration_us': np.float64(2.0286), 'median_duration_us': np.float64(2.047), 'std_dev_duration_us': np.float64(0.02545270123189289), 'min_duration_us': np.float64(1.984), 'max_duration_us': np.float64(2.048)}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStridedBatched&lt;float&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt; &gt;(float const*, float, cublasGemvTensorStridedBatched&lt;float&gt;, int, float const*, float, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, cublasPointerMode_t, cublasLtEpilogue_t, cublasGemvTensorStridedBatched&lt;biasType&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;::value_type, float&gt;::type const&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.183000000000002), 'mean_duration_us': np.float64(2.6366000000000005), 'median_duration_us': np.float64(2.688), 'std_dev_duration_us': np.float64(0.08984341934721768), 'min_duration_us': np.float64(2.527), 'max_duration_us': np.float64(2.72)}]</t>
+          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt; &gt;(cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 10.143, 'mean_duration_us': 2.0286, 'median_duration_us': 2.047, 'std_dev_duration_us': 0.02545270123189289, 'min_duration_us': 1.984, 'max_duration_us': 2.048}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStridedBatched&lt;float&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt; &gt;(float const*, float, cublasGemvTensorStridedBatched&lt;float&gt;, int, float const*, float, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, cublasPointerMode_t, cublasLtEpilogue_t, cublasGemvTensorStridedBatched&lt;biasType&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;::value_type, float&gt;::type const&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 13.183000000000002, 'mean_duration_us': 2.6366000000000005, 'median_duration_us': 2.688, 'std_dev_duration_us': 0.08984341934721768, 'min_duration_us': 2.527, 'max_duration_us': 2.72}]</t>
         </is>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorS...', 'stream': 7, 'mean_duration_us': np.float64(2.03)}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStrided...', 'stream': 7, 'mean_duration_us': np.float64(2.64)}]</t>
+          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorS...', 'stream': 7, 'mean_duration_us': 2.03}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStrided...', 'stream': 7, 'mean_duration_us': 2.64}]</t>
         </is>
       </c>
       <c r="P52" t="n">
@@ -4944,12 +4944,12 @@
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::index_elementwise_kernel&lt;128, 4, at::native::gpu_index_kernel&lt;at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1}&gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;, at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1} const&amp;)::{lambda(int)#1}&gt;(long, at::native::gpu_index_kernel&lt;at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1}&gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;, at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(22.176000000000002), 'mean_duration_us': np.float64(4.4352), 'median_duration_us': np.float64(4.256), 'std_dev_duration_us': np.float64(0.26400560600108475), 'min_duration_us': np.float64(4.192), 'max_duration_us': np.float64(4.832)}]</t>
+          <t>[{'name': 'void at::native::index_elementwise_kernel&lt;128, 4, at::native::gpu_index_kernel&lt;at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1}&gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;, at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1} const&amp;)::{lambda(int)#1}&gt;(long, at::native::gpu_index_kernel&lt;at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1}&gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;, at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 22.176000000000002, 'mean_duration_us': 4.4352, 'median_duration_us': 4.256, 'std_dev_duration_us': 0.26400560600108475, 'min_duration_us': 4.192, 'max_duration_us': 4.832}]</t>
         </is>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::index_elementwise_kernel&lt;128, 4, at::native::gp...', 'stream': 7, 'mean_duration_us': np.float64(4.44)}]</t>
+          <t>[{'name': 'void at::native::index_elementwise_kernel&lt;128, 4, at::native::gp...', 'stream': 7, 'mean_duration_us': 4.44}]</t>
         </is>
       </c>
       <c r="P53" t="n">
@@ -5011,12 +5011,12 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, 4, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(22.144000000000002), 'mean_duration_us': np.float64(4.428800000000001), 'median_duration_us': np.float64(4.416), 'std_dev_duration_us': np.float64(0.09621309682158638), 'min_duration_us': np.float64(4.32), 'max_duration_us': np.float64(4.608)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, 4, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 22.144000000000002, 'mean_duration_us': 4.428800000000001, 'median_duration_us': 4.416, 'std_dev_duration_us': 0.09621309682158638, 'min_duration_us': 4.32, 'max_duration_us': 4.608}]</t>
         </is>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFun...', 'stream': 7, 'mean_duration_us': np.float64(4.43)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFun...', 'stream': 7, 'mean_duration_us': 4.43}]</t>
         </is>
       </c>
       <c r="P54" t="n">
@@ -5078,12 +5078,12 @@
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(20.255), 'mean_duration_us': np.float64(4.051), 'median_duration_us': np.float64(4.032), 'std_dev_duration_us': np.float64(0.02550294100687212), 'min_duration_us': np.float64(4.032), 'max_duration_us': np.float64(4.096)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': 20.255, 'mean_duration_us': 4.051, 'median_duration_us': 4.032, 'std_dev_duration_us': 0.02550294100687212, 'min_duration_us': 4.032, 'max_duration_us': 4.096}]</t>
         </is>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(4.05)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 4.05}]</t>
         </is>
       </c>
       <c r="P55" t="n">
@@ -5145,12 +5145,12 @@
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(20.128), 'mean_duration_us': np.float64(4.0256), 'median_duration_us': np.float64(4.0), 'std_dev_duration_us': np.float64(0.13636656481704024), 'min_duration_us': np.float64(3.808), 'max_duration_us': np.float64(4.224)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 20.128, 'mean_duration_us': 4.0256, 'median_duration_us': 4.0, 'std_dev_duration_us': 0.13636656481704024, 'min_duration_us': 3.808, 'max_duration_us': 4.224}]</t>
         </is>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': np.float64(4.03)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': 4.03}]</t>
         </is>
       </c>
       <c r="P56" t="n">
@@ -5212,12 +5212,12 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(18.784), 'mean_duration_us': np.float64(3.7567999999999997), 'median_duration_us': np.float64(3.744), 'std_dev_duration_us': np.float64(0.03263372488699366), 'min_duration_us': np.float64(3.712), 'max_duration_us': np.float64(3.808)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 18.784, 'mean_duration_us': 3.7567999999999997, 'median_duration_us': 3.744, 'std_dev_duration_us': 0.03263372488699366, 'min_duration_us': 3.712, 'max_duration_us': 3.808}]</t>
         </is>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': np.float64(3.76)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': 3.76}]</t>
         </is>
       </c>
       <c r="P57" t="n">
@@ -5279,12 +5279,12 @@
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;int, at::native::ArgMaxOps&lt;int&gt;, unsigned int, long, 4&gt; &gt;(at::native::ReduceOp&lt;int, at::native::ArgMaxOps&lt;int&gt;, unsigned int, long, 4&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(18.527), 'mean_duration_us': np.float64(3.7054), 'median_duration_us': np.float64(3.712), 'std_dev_duration_us': np.float64(0.13307982566865645), 'min_duration_us': np.float64(3.488), 'max_duration_us': np.float64(3.871)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;int, at::native::ArgMaxOps&lt;int&gt;, unsigned int, long, 4&gt; &gt;(at::native::ReduceOp&lt;int, at::native::ArgMaxOps&lt;int&gt;, unsigned int, long, 4&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 18.527, 'mean_duration_us': 3.7054, 'median_duration_us': 3.712, 'std_dev_duration_us': 0.13307982566865645, 'min_duration_us': 3.488, 'max_duration_us': 3.871}]</t>
         </is>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;int,...', 'stream': 7, 'mean_duration_us': np.float64(3.71)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;int,...', 'stream': 7, 'mean_duration_us': 3.71}]</t>
         </is>
       </c>
       <c r="P58" t="n">
@@ -5346,12 +5346,12 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(17.918), 'mean_duration_us': np.float64(3.5835999999999997), 'median_duration_us': np.float64(3.552), 'std_dev_duration_us': np.float64(0.049834124854360604), 'min_duration_us': np.float64(3.551), 'max_duration_us': np.float64(3.68)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 17.918, 'mean_duration_us': 3.5835999999999997, 'median_duration_us': 3.552, 'std_dev_duration_us': 0.049834124854360604, 'min_duration_us': 3.551, 'max_duration_us': 3.68}]</t>
         </is>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': np.float64(3.58)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': 3.58}]</t>
         </is>
       </c>
       <c r="P59" t="n">
@@ -5413,12 +5413,12 @@
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(17.44), 'mean_duration_us': np.float64(1.7440000000000002), 'median_duration_us': np.float64(1.7440000000000002), 'std_dev_duration_us': np.float64(0.9569284194755635), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(2.72)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': 17.44, 'mean_duration_us': 1.7440000000000002, 'median_duration_us': 1.7440000000000002, 'std_dev_duration_us': 0.9569284194755635, 'min_duration_us': 0.768, 'max_duration_us': 2.72}]</t>
         </is>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(1.74)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 1.74}]</t>
         </is>
       </c>
       <c r="P60" t="n">
@@ -5480,12 +5480,12 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt; &gt;(at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(15.936), 'mean_duration_us': np.float64(3.1872), 'median_duration_us': np.float64(3.104), 'std_dev_duration_us': np.float64(0.2268165778773677), 'min_duration_us': np.float64(2.944), 'max_duration_us': np.float64(3.488)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt; &gt;(at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 15.936, 'mean_duration_us': 3.1872, 'median_duration_us': 3.104, 'std_dev_duration_us': 0.2268165778773677, 'min_duration_us': 2.944, 'max_duration_us': 3.488}]</t>
         </is>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10:...', 'stream': 7, 'mean_duration_us': np.float64(3.19)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10:...', 'stream': 7, 'mean_duration_us': 3.19}]</t>
         </is>
       </c>
       <c r="P61" t="n">
@@ -5547,12 +5547,12 @@
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.717999999999998), 'mean_duration_us': np.float64(2.9435999999999996), 'median_duration_us': np.float64(2.944), 'std_dev_duration_us': np.float64(0.0004898979485565817), 'min_duration_us': np.float64(2.943), 'max_duration_us': np.float64(2.944)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 14.717999999999998, 'mean_duration_us': 2.9435999999999996, 'median_duration_us': 2.944, 'std_dev_duration_us': 0.0004898979485565817, 'min_duration_us': 2.943, 'max_duration_us': 2.944}]</t>
         </is>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.94)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.94}]</t>
         </is>
       </c>
       <c r="P62" t="n">
@@ -5614,12 +5614,12 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.657), 'mean_duration_us': np.float64(2.9314), 'median_duration_us': np.float64(2.944), 'std_dev_duration_us': np.float64(0.03232089107682529), 'min_duration_us': np.float64(2.881), 'max_duration_us': np.float64(2.976)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 14.657, 'mean_duration_us': 2.9314, 'median_duration_us': 2.944, 'std_dev_duration_us': 0.03232089107682529, 'min_duration_us': 2.881, 'max_duration_us': 2.976}]</t>
         </is>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.93)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.93}]</t>
         </is>
       </c>
       <c r="P63" t="n">
@@ -5681,12 +5681,12 @@
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.560000000000002), 'mean_duration_us': np.float64(2.9120000000000004), 'median_duration_us': np.float64(3.008), 'std_dev_duration_us': np.float64(0.21891368161903446), 'min_duration_us': np.float64(2.656), 'max_duration_us': np.float64(3.2)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 14.560000000000002, 'mean_duration_us': 2.9120000000000004, 'median_duration_us': 3.008, 'std_dev_duration_us': 0.21891368161903446, 'min_duration_us': 2.656, 'max_duration_us': 3.2}]</t>
         </is>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.91)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.91}]</t>
         </is>
       </c>
       <c r="P64" t="n">
@@ -5748,12 +5748,12 @@
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.495999999999999), 'mean_duration_us': np.float64(2.8991999999999996), 'median_duration_us': np.float64(2.912), 'std_dev_duration_us': np.float64(0.032633724886993856), 'min_duration_us': np.float64(2.848), 'max_duration_us': np.float64(2.944)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 14.495999999999999, 'mean_duration_us': 2.8991999999999996, 'median_duration_us': 2.912, 'std_dev_duration_us': 0.032633724886993856, 'min_duration_us': 2.848, 'max_duration_us': 2.944}]</t>
         </is>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.9)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.9}]</t>
         </is>
       </c>
       <c r="P65" t="n">
@@ -5815,12 +5815,12 @@
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.985), 'mean_duration_us': np.float64(2.7969999999999997), 'median_duration_us': np.float64(2.785), 'std_dev_duration_us': np.float64(0.015517731793016621), 'min_duration_us': np.float64(2.784), 'max_duration_us': np.float64(2.816)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 13.985, 'mean_duration_us': 2.7969999999999997, 'median_duration_us': 2.785, 'std_dev_duration_us': 0.015517731793016621, 'min_duration_us': 2.784, 'max_duration_us': 2.816}]</t>
         </is>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': np.float64(2.8)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': 2.8}]</t>
         </is>
       </c>
       <c r="P66" t="n">
@@ -5882,12 +5882,12 @@
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.472000000000001), 'mean_duration_us': np.float64(2.6944000000000004), 'median_duration_us': np.float64(2.752), 'std_dev_duration_us': np.float64(0.10398769157934018), 'min_duration_us': np.float64(2.528), 'max_duration_us': np.float64(2.816)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 13.472000000000001, 'mean_duration_us': 2.6944000000000004, 'median_duration_us': 2.752, 'std_dev_duration_us': 0.10398769157934018, 'min_duration_us': 2.528, 'max_duration_us': 2.816}]</t>
         </is>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.69)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.69}]</t>
         </is>
       </c>
       <c r="P67" t="n">
@@ -5949,12 +5949,12 @@
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.407000000000002), 'mean_duration_us': np.float64(2.6814000000000004), 'median_duration_us': np.float64(2.656), 'std_dev_duration_us': np.float64(0.07142996570067763), 'min_duration_us': np.float64(2.623), 'max_duration_us': np.float64(2.816)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 13.407000000000002, 'mean_duration_us': 2.6814000000000004, 'median_duration_us': 2.656, 'std_dev_duration_us': 0.07142996570067763, 'min_duration_us': 2.623, 'max_duration_us': 2.816}]</t>
         </is>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.68)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.68}]</t>
         </is>
       </c>
       <c r="P68" t="n">
@@ -6016,12 +6016,12 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.345), 'mean_duration_us': np.float64(2.669), 'median_duration_us': np.float64(2.72), 'std_dev_duration_us': np.float64(0.08978641322605552), 'min_duration_us': np.float64(2.56), 'max_duration_us': np.float64(2.753)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 13.345, 'mean_duration_us': 2.669, 'median_duration_us': 2.72, 'std_dev_duration_us': 0.08978641322605552, 'min_duration_us': 2.56, 'max_duration_us': 2.753}]</t>
         </is>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.67)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.67}]</t>
         </is>
       </c>
       <c r="P69" t="n">
@@ -6083,12 +6083,12 @@
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(12.222999999999999), 'mean_duration_us': np.float64(2.4446), 'median_duration_us': np.float64(2.336), 'std_dev_duration_us': np.float64(0.1469742834648294), 'min_duration_us': np.float64(2.303), 'max_duration_us': np.float64(2.624)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 12.222999999999999, 'mean_duration_us': 2.4446, 'median_duration_us': 2.336, 'std_dev_duration_us': 0.1469742834648294, 'min_duration_us': 2.303, 'max_duration_us': 2.624}]</t>
         </is>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.44)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.44}]</t>
         </is>
       </c>
       <c r="P70" t="n">
@@ -6150,12 +6150,12 @@
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(11.904), 'mean_duration_us': np.float64(2.3808), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.04340691189200176), 'min_duration_us': np.float64(2.336), 'max_duration_us': np.float64(2.464)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 11.904, 'mean_duration_us': 2.3808, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.04340691189200176, 'min_duration_us': 2.336, 'max_duration_us': 2.464}]</t>
         </is>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.38)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.38}]</t>
         </is>
       </c>
       <c r="P71" t="n">
@@ -6217,12 +6217,12 @@
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(11.904), 'mean_duration_us': np.float64(2.3808), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.0478932145507065), 'min_duration_us': np.float64(2.336), 'max_duration_us': np.float64(2.464)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 11.904, 'mean_duration_us': 2.3808, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.0478932145507065, 'min_duration_us': 2.336, 'max_duration_us': 2.464}]</t>
         </is>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.38)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.38}]</t>
         </is>
       </c>
       <c r="P72" t="n">
@@ -6284,12 +6284,12 @@
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; &gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; &gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(10.687), 'mean_duration_us': np.float64(2.1374), 'median_duration_us': np.float64(2.208), 'std_dev_duration_us': np.float64(0.14060953026022097), 'min_duration_us': np.float64(1.952), 'max_duration_us': np.float64(2.272)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; &gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; &gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 10.687, 'mean_duration_us': 2.1374, 'median_duration_us': 2.208, 'std_dev_duration_us': 0.14060953026022097, 'min_duration_us': 1.952, 'max_duration_us': 2.272}]</t>
         </is>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.14)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.14}]</t>
         </is>
       </c>
       <c r="P73" t="n">
@@ -6351,12 +6351,12 @@
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::AUnaryFunctor&lt;long, long, bool, at::native::(anonymous namespace)::CompareEqFunctor&lt;long&gt; &gt;, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::AUnaryFunctor&lt;long, long, bool, at::native::(anonymous namespace)::CompareEqFunctor&lt;long&gt; &gt;, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(10.048), 'mean_duration_us': np.float64(2.0096), 'median_duration_us': np.float64(2.016), 'std_dev_duration_us': np.float64(0.08442179813294667), 'min_duration_us': np.float64(1.856), 'max_duration_us': np.float64(2.112)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::AUnaryFunctor&lt;long, long, bool, at::native::(anonymous namespace)::CompareEqFunctor&lt;long&gt; &gt;, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::AUnaryFunctor&lt;long, long, bool, at::native::(anonymous namespace)::CompareEqFunctor&lt;long&gt; &gt;, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 10.048, 'mean_duration_us': 2.0096, 'median_duration_us': 2.016, 'std_dev_duration_us': 0.08442179813294667, 'min_duration_us': 1.856, 'max_duration_us': 2.112}]</t>
         </is>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::AUnaryF...', 'stream': 7, 'mean_duration_us': np.float64(2.01)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::AUnaryF...', 'stream': 7, 'mean_duration_us': 2.01}]</t>
         </is>
       </c>
       <c r="P74" t="n">
@@ -6418,12 +6418,12 @@
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::compare_scalar_kernel&lt;long&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::OpType, long)::{lambda(long)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::compare_scalar_kernel&lt;long&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::OpType, long)::{lambda(long)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(9.247), 'mean_duration_us': np.float64(1.8494), 'median_duration_us': np.float64(1.888), 'std_dev_duration_us': np.float64(0.12672426760490674), 'min_duration_us': np.float64(1.696), 'max_duration_us': np.float64(2.047)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::compare_scalar_kernel&lt;long&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::OpType, long)::{lambda(long)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::compare_scalar_kernel&lt;long&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::OpType, long)::{lambda(long)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 9.247, 'mean_duration_us': 1.8494, 'median_duration_us': 1.888, 'std_dev_duration_us': 0.12672426760490674, 'min_duration_us': 1.696, 'max_duration_us': 2.047}]</t>
         </is>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::co...', 'stream': 7, 'mean_duration_us': np.float64(1.85)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::co...', 'stream': 7, 'mean_duration_us': 1.85}]</t>
         </is>
       </c>
       <c r="P75" t="n">
@@ -6485,12 +6485,12 @@
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.896), 'mean_duration_us': np.float64(1.7792000000000001), 'median_duration_us': np.float64(1.792), 'std_dev_duration_us': np.float64(0.025600000000000022), 'min_duration_us': np.float64(1.728), 'max_duration_us': np.float64(1.792)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.896, 'mean_duration_us': 1.7792000000000001, 'median_duration_us': 1.792, 'std_dev_duration_us': 0.025600000000000022, 'min_duration_us': 1.728, 'max_duration_us': 1.792}]</t>
         </is>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': np.float64(1.78)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': 1.78}]</t>
         </is>
       </c>
       <c r="P76" t="n">
@@ -6552,12 +6552,12 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.799), 'mean_duration_us': np.float64(1.7597999999999998), 'median_duration_us': np.float64(1.76), 'std_dev_duration_us': np.float64(0.10100376230616363), 'min_duration_us': np.float64(1.632), 'max_duration_us': np.float64(1.888)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.799, 'mean_duration_us': 1.7597999999999998, 'median_duration_us': 1.76, 'std_dev_duration_us': 0.10100376230616363, 'min_duration_us': 1.632, 'max_duration_us': 1.888}]</t>
         </is>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.76)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.76}]</t>
         </is>
       </c>
       <c r="P77" t="n">
@@ -6619,12 +6619,12 @@
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.769), 'mean_duration_us': np.float64(1.7538), 'median_duration_us': np.float64(1.792), 'std_dev_duration_us': np.float64(0.0742762411542211), 'min_duration_us': np.float64(1.664), 'max_duration_us': np.float64(1.825)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.769, 'mean_duration_us': 1.7538, 'median_duration_us': 1.792, 'std_dev_duration_us': 0.0742762411542211, 'min_duration_us': 1.664, 'max_duration_us': 1.825}]</t>
         </is>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': np.float64(1.75)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': 1.75}]</t>
         </is>
       </c>
       <c r="P78" t="n">
@@ -6686,12 +6686,12 @@
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.64), 'mean_duration_us': np.float64(1.7280000000000002), 'median_duration_us': np.float64(1.696), 'std_dev_duration_us': np.float64(0.10516273104099186), 'min_duration_us': np.float64(1.6), 'max_duration_us': np.float64(1.92)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.64, 'mean_duration_us': 1.7280000000000002, 'median_duration_us': 1.696, 'std_dev_duration_us': 0.10516273104099186, 'min_duration_us': 1.6, 'max_duration_us': 1.92}]</t>
         </is>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': np.float64(1.73)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': 1.73}]</t>
         </is>
       </c>
       <c r="P79" t="n">
@@ -6753,12 +6753,12 @@
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(anonymous namespace)::elu_kernel(at::TensorIteratorBase&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::(anonymous namespace)::elu_kernel(at::TensorIteratorBase&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.479), 'mean_duration_us': np.float64(1.6957999999999998), 'median_duration_us': np.float64(1.696), 'std_dev_duration_us': np.float64(0.020556264252047336), 'min_duration_us': np.float64(1.663), 'max_duration_us': np.float64(1.728)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(anonymous namespace)::elu_kernel(at::TensorIteratorBase&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::(anonymous namespace)::elu_kernel(at::TensorIteratorBase&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.479, 'mean_duration_us': 1.6957999999999998, 'median_duration_us': 1.696, 'std_dev_duration_us': 0.020556264252047336, 'min_duration_us': 1.663, 'max_duration_us': 1.728}]</t>
         </is>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(a...', 'stream': 7, 'mean_duration_us': np.float64(1.7)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(a...', 'stream': 7, 'mean_duration_us': 1.7}]</t>
         </is>
       </c>
       <c r="P80" t="n">
@@ -6820,12 +6820,12 @@
       </c>
       <c r="N81" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::exp_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::exp_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.447), 'mean_duration_us': np.float64(1.6893999999999998), 'median_duration_us': np.float64(1.632), 'std_dev_duration_us': np.float64(0.09808486121721335), 'min_duration_us': np.float64(1.599), 'max_duration_us': np.float64(1.824)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::exp_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::exp_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.447, 'mean_duration_us': 1.6893999999999998, 'median_duration_us': 1.632, 'std_dev_duration_us': 0.09808486121721335, 'min_duration_us': 1.599, 'max_duration_us': 1.824}]</t>
         </is>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::ex...', 'stream': 7, 'mean_duration_us': np.float64(1.69)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::ex...', 'stream': 7, 'mean_duration_us': 1.69}]</t>
         </is>
       </c>
       <c r="P81" t="n">
@@ -6887,12 +6887,12 @@
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.030999999999999), 'mean_duration_us': np.float64(1.6061999999999999), 'median_duration_us': np.float64(1.632), 'std_dev_duration_us': np.float64(0.046786322787754936), 'min_duration_us': np.float64(1.536), 'max_duration_us': np.float64(1.663)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.030999999999999, 'mean_duration_us': 1.6061999999999999, 'median_duration_us': 1.632, 'std_dev_duration_us': 0.046786322787754936, 'min_duration_us': 1.536, 'max_duration_us': 1.663}]</t>
         </is>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.61)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.61}]</t>
         </is>
       </c>
       <c r="P82" t="n">
@@ -6954,12 +6954,12 @@
       </c>
       <c r="N83" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(7.968), 'mean_duration_us': np.float64(0.7968), 'median_duration_us': np.float64(0.8), 'std_dev_duration_us': np.float64(0.009600000000000008), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(0.8)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': 7.968, 'mean_duration_us': 0.7968, 'median_duration_us': 0.8, 'std_dev_duration_us': 0.009600000000000008, 'min_duration_us': 0.768, 'max_duration_us': 0.8}]</t>
         </is>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(0.8)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 0.8}]</t>
         </is>
       </c>
       <c r="P83" t="n">
@@ -7021,12 +7021,12 @@
       </c>
       <c r="N84" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.872), 'mean_duration_us': np.float64(1.5744), 'median_duration_us': np.float64(1.568), 'std_dev_duration_us': np.float64(0.02394660727535325), 'min_duration_us': np.float64(1.536), 'max_duration_us': np.float64(1.6)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.872, 'mean_duration_us': 1.5744, 'median_duration_us': 1.568, 'std_dev_duration_us': 0.02394660727535325, 'min_duration_us': 1.536, 'max_duration_us': 1.6}]</t>
         </is>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.57)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.57}]</t>
         </is>
       </c>
       <c r="P84" t="n">
@@ -7088,12 +7088,12 @@
       </c>
       <c r="N85" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.744), 'mean_duration_us': np.float64(1.5488), 'median_duration_us': np.float64(1.6), 'std_dev_duration_us': np.float64(0.09185728060420688), 'min_duration_us': np.float64(1.408), 'max_duration_us': np.float64(1.632)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.744, 'mean_duration_us': 1.5488, 'median_duration_us': 1.6, 'std_dev_duration_us': 0.09185728060420688, 'min_duration_us': 1.408, 'max_duration_us': 1.632}]</t>
         </is>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.55)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.55}]</t>
         </is>
       </c>
       <c r="P85" t="n">
@@ -7155,12 +7155,12 @@
       </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#7}::operator()() const::{lambda(float, bool)#1}, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#7}::operator()() const::{lambda(float, bool)#1}, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.454000000000001), 'mean_duration_us': np.float64(1.4908000000000001), 'median_duration_us': np.float64(1.536), 'std_dev_duration_us': np.float64(0.0797932327957703), 'min_duration_us': np.float64(1.344), 'max_duration_us': np.float64(1.567)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#7}::operator()() const::{lambda(float, bool)#1}, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#7}::operator()() const::{lambda(float, bool)#1}, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.454000000000001, 'mean_duration_us': 1.4908000000000001, 'median_duration_us': 1.536, 'std_dev_duration_us': 0.0797932327957703, 'min_duration_us': 1.344, 'max_duration_us': 1.567}]</t>
         </is>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(a...', 'stream': 7, 'mean_duration_us': np.float64(1.49)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(a...', 'stream': 7, 'mean_duration_us': 1.49}]</t>
         </is>
       </c>
       <c r="P86" t="n">
@@ -7222,12 +7222,12 @@
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.424999999999999), 'mean_duration_us': np.float64(1.4849999999999999), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.025502941006872143), 'min_duration_us': np.float64(1.472), 'max_duration_us': np.float64(1.536)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.424999999999999, 'mean_duration_us': 1.4849999999999999, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.025502941006872143, 'min_duration_us': 1.472, 'max_duration_us': 1.536}]</t>
         </is>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(1.48)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 1.48}]</t>
         </is>
       </c>
       <c r="P87" t="n">
@@ -7289,12 +7289,12 @@
       </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.264999999999999), 'mean_duration_us': np.float64(1.4529999999999998), 'median_duration_us': np.float64(1.441), 'std_dev_duration_us': np.float64(0.015517731793016656), 'min_duration_us': np.float64(1.44), 'max_duration_us': np.float64(1.472)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.264999999999999, 'mean_duration_us': 1.4529999999999998, 'median_duration_us': 1.441, 'std_dev_duration_us': 0.015517731793016656, 'min_duration_us': 1.44, 'max_duration_us': 1.472}]</t>
         </is>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.45)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.45}]</t>
         </is>
       </c>
       <c r="P88" t="n">
@@ -7356,12 +7356,12 @@
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16, bool)#1}, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16, bool)#1}, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.134), 'mean_duration_us': np.float64(1.4268), 'median_duration_us': np.float64(1.375), 'std_dev_duration_us': np.float64(0.08990083425641834), 'min_duration_us': np.float64(1.343), 'max_duration_us': np.float64(1.536)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16, bool)#1}, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16, bool)#1}, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.134, 'mean_duration_us': 1.4268, 'median_duration_us': 1.375, 'std_dev_duration_us': 0.08990083425641834, 'min_duration_us': 1.343, 'max_duration_us': 1.536}]</t>
         </is>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(a...', 'stream': 7, 'mean_duration_us': np.float64(1.43)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(a...', 'stream': 7, 'mean_duration_us': 1.43}]</t>
         </is>
       </c>
       <c r="P89" t="n">
@@ -7423,12 +7423,12 @@
       </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;(int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}, function_traits&lt;at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;::result_type*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.103999999999999), 'mean_duration_us': np.float64(1.4207999999999998), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.16639999999999996), 'min_duration_us': np.float64(1.248), 'max_duration_us': np.float64(1.696)}]</t>
+          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;(int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}, function_traits&lt;at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;::result_type*)', 'stream': 7, 'count': 5, 'total_duration_us': 7.103999999999999, 'mean_duration_us': 1.4207999999999998, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.16639999999999996, 'min_duration_us': 1.248, 'max_duration_us': 1.696}]</t>
         </is>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, a...', 'stream': 7, 'mean_duration_us': np.float64(1.42)}]</t>
+          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, a...', 'stream': 7, 'mean_duration_us': 1.42}]</t>
         </is>
       </c>
       <c r="P90" t="n">
@@ -7490,12 +7490,12 @@
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnOther_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnOther_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.040000000000001), 'mean_duration_us': np.float64(1.4080000000000001), 'median_duration_us': np.float64(1.344), 'std_dev_duration_us': np.float64(0.09706080568385983), 'min_duration_us': np.float64(1.312), 'max_duration_us': np.float64(1.568)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnOther_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnOther_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.040000000000001, 'mean_duration_us': 1.4080000000000001, 'median_duration_us': 1.344, 'std_dev_duration_us': 0.09706080568385983, 'min_duration_us': 1.312, 'max_duration_us': 1.568}]</t>
         </is>
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.41)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.41}]</t>
         </is>
       </c>
       <c r="P91" t="n">
@@ -7557,12 +7557,12 @@
       </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.008999999999999), 'mean_duration_us': np.float64(1.4017999999999997), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.08894132897590411), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.504)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.008999999999999, 'mean_duration_us': 1.4017999999999997, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.08894132897590411, 'min_duration_us': 1.28, 'max_duration_us': 1.504}]</t>
         </is>
       </c>
       <c r="O92" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bf...', 'stream': 7, 'mean_duration_us': np.float64(1.4)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bf...', 'stream': 7, 'mean_duration_us': 1.4}]</t>
         </is>
       </c>
       <c r="P92" t="n">
@@ -7624,12 +7624,12 @@
       </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::FillFunctor&lt;float&gt;, std::array&lt;char*, 1ul&gt; &gt;(int, at::native::FillFunctor&lt;float&gt;, std::array&lt;char*, 1ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.008000000000001), 'mean_duration_us': np.float64(1.4016000000000002), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.09997119585160516), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.504)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::FillFunctor&lt;float&gt;, std::array&lt;char*, 1ul&gt; &gt;(int, at::native::FillFunctor&lt;float&gt;, std::array&lt;char*, 1ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.008000000000001, 'mean_duration_us': 1.4016000000000002, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.09997119585160516, 'min_duration_us': 1.28, 'max_duration_us': 1.504}]</t>
         </is>
       </c>
       <c r="O93" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Fi...', 'stream': 7, 'mean_duration_us': np.float64(1.4)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Fi...', 'stream': 7, 'mean_duration_us': 1.4}]</t>
         </is>
       </c>
       <c r="P93" t="n">
@@ -7691,12 +7691,12 @@
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.007999999999999), 'mean_duration_us': np.float64(1.4015999999999997), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.08914168497397834), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.504)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.007999999999999, 'mean_duration_us': 1.4015999999999997, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.08914168497397834, 'min_duration_us': 1.28, 'max_duration_us': 1.504}]</t>
         </is>
       </c>
       <c r="O94" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(1.4)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 1.4}]</t>
         </is>
       </c>
       <c r="P94" t="n">
@@ -7758,12 +7758,12 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(6.687999999999999), 'mean_duration_us': np.float64(1.3375999999999997), 'median_duration_us': np.float64(1.408), 'std_dev_duration_us': np.float64(0.0868138237840034), 'min_duration_us': np.float64(1.216), 'max_duration_us': np.float64(1.408)}]</t>
+          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': 6.687999999999999, 'mean_duration_us': 1.3375999999999997, 'median_duration_us': 1.408, 'std_dev_duration_us': 0.0868138237840034, 'min_duration_us': 1.216, 'max_duration_us': 1.408}]</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(1.34)}]</t>
+          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'mean_duration_us': 1.34}]</t>
         </is>
       </c>
       <c r="P95" t="n">
@@ -7825,12 +7825,12 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;(int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}, function_traits&lt;at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;::result_type*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(6.176), 'mean_duration_us': np.float64(1.2352), 'median_duration_us': np.float64(1.28), 'std_dev_duration_us': np.float64(0.08245823185104081), 'min_duration_us': np.float64(1.12), 'max_duration_us': np.float64(1.312)}]</t>
+          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;(int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}, function_traits&lt;at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;::result_type*)', 'stream': 7, 'count': 5, 'total_duration_us': 6.176, 'mean_duration_us': 1.2352, 'median_duration_us': 1.28, 'std_dev_duration_us': 0.08245823185104081, 'min_duration_us': 1.12, 'max_duration_us': 1.312}]</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, a...', 'stream': 7, 'mean_duration_us': np.float64(1.24)}]</t>
+          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, a...', 'stream': 7, 'mean_duration_us': 1.24}]</t>
         </is>
       </c>
       <c r="P96" t="n">
@@ -7892,12 +7892,12 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::FillFunctor&lt;c10::BFloat16&gt;, std::array&lt;char*, 1ul&gt; &gt;(int, at::native::FillFunctor&lt;c10::BFloat16&gt;, std::array&lt;char*, 1ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(5.984000000000001), 'mean_duration_us': np.float64(1.1968), 'median_duration_us': np.float64(1.12), 'std_dev_duration_us': np.float64(0.09406040612287402), 'min_duration_us': np.float64(1.12), 'max_duration_us': np.float64(1.312)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::FillFunctor&lt;c10::BFloat16&gt;, std::array&lt;char*, 1ul&gt; &gt;(int, at::native::FillFunctor&lt;c10::BFloat16&gt;, std::array&lt;char*, 1ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 5.984000000000001, 'mean_duration_us': 1.1968, 'median_duration_us': 1.12, 'std_dev_duration_us': 0.09406040612287402, 'min_duration_us': 1.12, 'max_duration_us': 1.312}]</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Fi...', 'stream': 7, 'mean_duration_us': np.float64(1.2)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Fi...', 'stream': 7, 'mean_duration_us': 1.2}]</t>
         </is>
       </c>
       <c r="P97" t="n">
@@ -8185,12 +8185,12 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(130015.7), 'mean_duration_us': np.float64(1083.4641666666666), 'median_duration_us': np.float64(1082.965), 'std_dev_duration_us': np.float64(3.932529614919927), 'min_duration_us': np.float64(1075.574), 'max_duration_us': np.float64(1096.694)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': 130015.7, 'mean_duration_us': 1083.4641666666666, 'median_duration_us': 1082.965, 'std_dev_duration_us': 3.932529614919927, 'min_duration_us': 1075.574, 'max_duration_us': 1096.694}]</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_25...', 'stream': 7, 'mean_duration_us': np.float64(1083.46)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_25...', 'stream': 7, 'mean_duration_us': 1083.46}]</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -8315,12 +8315,12 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(99311.41), 'mean_duration_us': np.float64(827.5950833333334), 'median_duration_us': np.float64(826.9205), 'std_dev_duration_us': np.float64(2.9474507419783706), 'min_duration_us': np.float64(825.432), 'max_duration_us': np.float64(851.8)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': 99311.41, 'mean_duration_us': 827.5950833333334, 'median_duration_us': 826.9205, 'std_dev_duration_us': 2.9474507419783706, 'min_duration_us': 825.432, 'max_duration_us': 851.8}]</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_12...', 'stream': 7, 'mean_duration_us': np.float64(827.6)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_12...', 'stream': 7, 'mean_duration_us': 827.6}]</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
@@ -8445,12 +8445,12 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 480, 'total_duration_us': np.float64(449.6640000000001), 'mean_duration_us': np.float64(0.9368000000000002), 'median_duration_us': np.float64(0.96), 'std_dev_duration_us': np.float64(0.14700191892171566), 'min_duration_us': np.float64(0.767), 'max_duration_us': np.float64(1.408)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 480, 'total_duration_us': np.float64(10035.521), 'mean_duration_us': np.float64(20.90733541666667), 'median_duration_us': np.float64(20.912), 'std_dev_duration_us': np.float64(0.2994497001373127), 'min_duration_us': np.float64(20.256), 'max_duration_us': np.float64(22.015)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 480, 'total_duration_us': 449.6640000000001, 'mean_duration_us': 0.9368000000000002, 'median_duration_us': 0.96, 'std_dev_duration_us': 0.14700191892171566, 'min_duration_us': 0.767, 'max_duration_us': 1.408}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 480, 'total_duration_us': 10035.521, 'mean_duration_us': 20.90733541666667, 'median_duration_us': 20.912, 'std_dev_duration_us': 0.2994497001373127, 'min_duration_us': 20.256, 'max_duration_us': 22.015}]</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.94)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(20.91)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.94}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 20.91}]</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
@@ -8575,12 +8575,12 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(115.61200000000002), 'mean_duration_us': np.float64(0.9634333333333335), 'median_duration_us': np.float64(0.96), 'std_dev_duration_us': np.float64(0.18370559478566667), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(1.6)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(7766.737), 'mean_duration_us': np.float64(64.72280833333333), 'median_duration_us': np.float64(64.639), 'std_dev_duration_us': np.float64(0.5570301951096441), 'min_duration_us': np.float64(63.711), 'max_duration_us': np.float64(65.951)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': 115.61200000000002, 'mean_duration_us': 0.9634333333333335, 'median_duration_us': 0.96, 'std_dev_duration_us': 0.18370559478566667, 'min_duration_us': 0.768, 'max_duration_us': 1.6}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': 7766.737, 'mean_duration_us': 64.72280833333333, 'median_duration_us': 64.639, 'std_dev_duration_us': 0.5570301951096441, 'min_duration_us': 63.711, 'max_duration_us': 65.951}]</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.96)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(64.72)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.96}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 64.72}]</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
@@ -8705,12 +8705,12 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(116.09), 'mean_duration_us': np.float64(0.9674166666666667), 'median_duration_us': np.float64(0.96), 'std_dev_duration_us': np.float64(0.15527371441711854), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(1.568)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(6884.5689999999995), 'mean_duration_us': np.float64(57.37140833333333), 'median_duration_us': np.float64(57.344), 'std_dev_duration_us': np.float64(0.31250691981227396), 'min_duration_us': np.float64(56.639), 'max_duration_us': np.float64(58.048)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': 116.09, 'mean_duration_us': 0.9674166666666667, 'median_duration_us': 0.96, 'std_dev_duration_us': 0.15527371441711854, 'min_duration_us': 0.768, 'max_duration_us': 1.568}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': 6884.5689999999995, 'mean_duration_us': 57.37140833333333, 'median_duration_us': 57.344, 'std_dev_duration_us': 0.31250691981227396, 'min_duration_us': 56.639, 'max_duration_us': 58.048}]</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.97)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(57.37)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.97}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 57.37}]</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
@@ -8835,12 +8835,12 @@
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 240, 'total_duration_us': np.float64(1579.851), 'mean_duration_us': np.float64(6.5827125), 'median_duration_us': np.float64(6.592), 'std_dev_duration_us': np.float64(0.13116311667951205), 'min_duration_us': np.float64(6.303), 'max_duration_us': np.float64(6.975)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 240, 'total_duration_us': 1579.851, 'mean_duration_us': 6.5827125, 'median_duration_us': 6.592, 'std_dev_duration_us': 0.13116311667951205, 'min_duration_us': 6.303, 'max_duration_us': 6.975}]</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': np.float64(6.58)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': 6.58}]</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
@@ -8965,12 +8965,12 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(385.4959999999999), 'mean_duration_us': np.float64(6.424933333333332), 'median_duration_us': np.float64(6.336), 'std_dev_duration_us': np.float64(0.19279919317489072), 'min_duration_us': np.float64(6.239), 'max_duration_us': np.float64(6.912)}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, __nv_bfloat16, float, __nv_bfloat16, true, true, false&gt;(cublasLt::cublasSplitKParams&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, float const*, float const*, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, void*, long, float*, int*)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(140.35000000000002), 'mean_duration_us': np.float64(2.339166666666667), 'median_duration_us': np.float64(2.336), 'std_dev_duration_us': np.float64(0.037292164801142315), 'min_duration_us': np.float64(2.272), 'max_duration_us': np.float64(2.496)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 385.4959999999999, 'mean_duration_us': 6.424933333333332, 'median_duration_us': 6.336, 'std_dev_duration_us': 0.19279919317489072, 'min_duration_us': 6.239, 'max_duration_us': 6.912}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, __nv_bfloat16, float, __nv_bfloat16, true, true, false&gt;(cublasLt::cublasSplitKParams&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, float const*, float const*, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, void*, long, float*, int*)', 'stream': 7, 'count': 60, 'total_duration_us': 140.35000000000002, 'mean_duration_us': 2.339166666666667, 'median_duration_us': 2.336, 'std_dev_duration_us': 0.037292164801142315, 'min_duration_us': 2.272, 'max_duration_us': 2.496}]</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': np.float64(6.42)}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': np.float64(2.34)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': 6.42}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': 2.34}]</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
@@ -9095,12 +9095,12 @@
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 20, 'total_duration_us': np.float64(17.248), 'mean_duration_us': np.float64(0.8624), 'median_duration_us': np.float64(0.8), 'std_dev_duration_us': np.float64(0.13365305832639968), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(1.248)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 20, 'total_duration_us': np.float64(414.7149999999999), 'mean_duration_us': np.float64(20.735749999999996), 'median_duration_us': np.float64(20.768), 'std_dev_duration_us': np.float64(0.42032010123238245), 'min_duration_us': np.float64(19.936), 'max_duration_us': np.float64(21.279)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 20, 'total_duration_us': 17.248, 'mean_duration_us': 0.8624, 'median_duration_us': 0.8, 'std_dev_duration_us': 0.13365305832639968, 'min_duration_us': 0.768, 'max_duration_us': 1.248}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 20, 'total_duration_us': 414.7149999999999, 'mean_duration_us': 20.735749999999996, 'median_duration_us': 20.768, 'std_dev_duration_us': 0.42032010123238245, 'min_duration_us': 19.936, 'max_duration_us': 21.279}]</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.86)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(20.74)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.86}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 20.74}]</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
@@ -9225,12 +9225,12 @@
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(422.845), 'mean_duration_us': np.float64(7.047416666666667), 'median_duration_us': np.float64(6.976), 'std_dev_duration_us': np.float64(0.17790056133194818), 'min_duration_us': np.float64(6.752), 'max_duration_us': np.float64(7.52)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 422.845, 'mean_duration_us': 7.047416666666667, 'median_duration_us': 6.976, 'std_dev_duration_us': 0.17790056133194818, 'min_duration_us': 6.752, 'max_duration_us': 7.52}]</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': np.float64(7.05)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': 7.05}]</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
@@ -9355,12 +9355,12 @@
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(185.69699999999997), 'mean_duration_us': np.float64(3.0949499999999994), 'median_duration_us': np.float64(3.104), 'std_dev_duration_us': np.float64(0.04453478977159322), 'min_duration_us': np.float64(3.008), 'max_duration_us': np.float64(3.168)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 185.69699999999997, 'mean_duration_us': 3.0949499999999994, 'median_duration_us': 3.104, 'std_dev_duration_us': 0.04453478977159322, 'min_duration_us': 3.008, 'max_duration_us': 3.168}]</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': np.float64(3.09)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': 3.09}]</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
@@ -9485,12 +9485,12 @@
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(167.428), 'mean_duration_us': np.float64(2.7904666666666667), 'median_duration_us': np.float64(2.816), 'std_dev_duration_us': np.float64(0.037250264726874344), 'min_duration_us': np.float64(2.72), 'max_duration_us': np.float64(2.88)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 167.428, 'mean_duration_us': 2.7904666666666667, 'median_duration_us': 2.816, 'std_dev_duration_us': 0.037250264726874344, 'min_duration_us': 2.72, 'max_duration_us': 2.88}]</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': np.float64(2.79)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': 2.79}]</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
@@ -9615,12 +9615,12 @@
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 15, 'total_duration_us': np.float64(35.168), 'mean_duration_us': np.float64(2.344533333333333), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.10418372660300108), 'min_duration_us': np.float64(2.176), 'max_duration_us': np.float64(2.56)}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 15, 'total_duration_us': np.float64(83.104), 'mean_duration_us': np.float64(5.540266666666667), 'median_duration_us': np.float64(5.376), 'std_dev_duration_us': np.float64(0.32818683025916123), 'min_duration_us': np.float64(5.152), 'max_duration_us': np.float64(6.176)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 15, 'total_duration_us': 35.168, 'mean_duration_us': 2.344533333333333, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.10418372660300108, 'min_duration_us': 2.176, 'max_duration_us': 2.56}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 15, 'total_duration_us': 83.104, 'mean_duration_us': 5.540266666666667, 'median_duration_us': 5.376, 'std_dev_duration_us': 0.32818683025916123, 'min_duration_us': 5.152, 'max_duration_us': 6.176}]</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.34)}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': np.float64(5.54)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.34}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': 5.54}]</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
@@ -9745,12 +9745,12 @@
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warpgroupsize2x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(86.78200000000001), 'mean_duration_us': np.float64(17.3564), 'median_duration_us': np.float64(17.376), 'std_dev_duration_us': np.float64(0.07209049868047837), 'min_duration_us': np.float64(17.215), 'max_duration_us': np.float64(17.408)}]</t>
+          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warpgroupsize2x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 5, 'total_duration_us': 86.78200000000001, 'mean_duration_us': 17.3564, 'median_duration_us': 17.376, 'std_dev_duration_us': 0.07209049868047837, 'min_duration_us': 17.215, 'max_duration_us': 17.408}]</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(17.36)}]</t>
+          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warp...', 'stream': 7, 'mean_duration_us': 17.36}]</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
@@ -9875,12 +9875,12 @@
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2&gt;(cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2::Params)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(56.54299999999999), 'mean_duration_us': np.float64(11.308599999999998), 'median_duration_us': np.float64(11.296), 'std_dev_duration_us': np.float64(0.10403768547983014), 'min_duration_us': np.float64(11.168), 'max_duration_us': np.float64(11.487)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2&gt;(cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2::Params)', 'stream': 7, 'count': 5, 'total_duration_us': 56.54299999999999, 'mean_duration_us': 11.308599999999998, 'median_duration_us': 11.296, 'std_dev_duration_us': 0.10403768547983014, 'min_duration_us': 11.168, 'max_duration_us': 11.487}]</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': np.float64(11.31)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': 11.31}]</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
@@ -10005,12 +10005,12 @@
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(23.615000000000002), 'mean_duration_us': np.float64(4.723000000000001), 'median_duration_us': np.float64(4.704), 'std_dev_duration_us': np.float64(0.06861486719363401), 'min_duration_us': np.float64(4.64), 'max_duration_us': np.float64(4.831)}]</t>
+          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 5, 'total_duration_us': 23.615000000000002, 'mean_duration_us': 4.723000000000001, 'median_duration_us': 4.704, 'std_dev_duration_us': 0.06861486719363401, 'min_duration_us': 4.64, 'max_duration_us': 4.831}]</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': np.float64(4.72)}]</t>
+          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': 4.72}]</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
@@ -10135,12 +10135,12 @@
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt; &gt;(cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(10.143), 'mean_duration_us': np.float64(2.0286), 'median_duration_us': np.float64(2.047), 'std_dev_duration_us': np.float64(0.02545270123189289), 'min_duration_us': np.float64(1.984), 'max_duration_us': np.float64(2.048)}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStridedBatched&lt;float&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt; &gt;(float const*, float, cublasGemvTensorStridedBatched&lt;float&gt;, int, float const*, float, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, cublasPointerMode_t, cublasLtEpilogue_t, cublasGemvTensorStridedBatched&lt;biasType&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;::value_type, float&gt;::type const&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.183000000000002), 'mean_duration_us': np.float64(2.6366000000000005), 'median_duration_us': np.float64(2.688), 'std_dev_duration_us': np.float64(0.08984341934721768), 'min_duration_us': np.float64(2.527), 'max_duration_us': np.float64(2.72)}]</t>
+          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt; &gt;(cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 10.143, 'mean_duration_us': 2.0286, 'median_duration_us': 2.047, 'std_dev_duration_us': 0.02545270123189289, 'min_duration_us': 1.984, 'max_duration_us': 2.048}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStridedBatched&lt;float&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt; &gt;(float const*, float, cublasGemvTensorStridedBatched&lt;float&gt;, int, float const*, float, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, cublasPointerMode_t, cublasLtEpilogue_t, cublasGemvTensorStridedBatched&lt;biasType&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;::value_type, float&gt;::type const&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 13.183000000000002, 'mean_duration_us': 2.6366000000000005, 'median_duration_us': 2.688, 'std_dev_duration_us': 0.08984341934721768, 'min_duration_us': 2.527, 'max_duration_us': 2.72}]</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorS...', 'stream': 7, 'mean_duration_us': np.float64(2.03)}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStrided...', 'stream': 7, 'mean_duration_us': np.float64(2.64)}]</t>
+          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorS...', 'stream': 7, 'mean_duration_us': 2.03}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStrided...', 'stream': 7, 'mean_duration_us': 2.64}]</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
@@ -10265,12 +10265,12 @@
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(18.784), 'mean_duration_us': np.float64(3.7567999999999997), 'median_duration_us': np.float64(3.744), 'std_dev_duration_us': np.float64(0.03263372488699366), 'min_duration_us': np.float64(3.712), 'max_duration_us': np.float64(3.808)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 18.784, 'mean_duration_us': 3.7567999999999997, 'median_duration_us': 3.744, 'std_dev_duration_us': 0.03263372488699366, 'min_duration_us': 3.712, 'max_duration_us': 3.808}]</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': np.float64(3.76)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': 3.76}]</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
@@ -10395,12 +10395,12 @@
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(17.918), 'mean_duration_us': np.float64(3.5835999999999997), 'median_duration_us': np.float64(3.552), 'std_dev_duration_us': np.float64(0.049834124854360604), 'min_duration_us': np.float64(3.551), 'max_duration_us': np.float64(3.68)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 17.918, 'mean_duration_us': 3.5835999999999997, 'median_duration_us': 3.552, 'std_dev_duration_us': 0.049834124854360604, 'min_duration_us': 3.551, 'max_duration_us': 3.68}]</t>
         </is>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': np.float64(3.58)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': 3.58}]</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
@@ -10780,12 +10780,12 @@
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(28.127000000000002), 'mean_duration_us': np.float64(5.625400000000001), 'median_duration_us': np.float64(5.664), 'std_dev_duration_us': np.float64(0.08941498755801505), 'min_duration_us': np.float64(5.503), 'max_duration_us': np.float64(5.728)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(222.207), 'mean_duration_us': np.float64(44.4414), 'median_duration_us': np.float64(44.384), 'std_dev_duration_us': np.float64(0.1792647204555328), 'min_duration_us': np.float64(44.224), 'max_duration_us': np.float64(44.768)}, {'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(10.85), 'mean_duration_us': np.float64(2.17), 'median_duration_us': np.float64(2.176), 'std_dev_duration_us': np.float64(0.013007690033207267), 'min_duration_us': np.float64(2.144), 'max_duration_us': np.float64(2.177)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(58.303000000000004), 'mean_duration_us': np.float64(11.6606), 'median_duration_us': np.float64(11.679), 'std_dev_duration_us': np.float64(0.15088485676170435), 'min_duration_us': np.float64(11.424), 'max_duration_us': np.float64(11.872)}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8&gt;(cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8::Params)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(982.9660000000001), 'mean_duration_us': np.float64(196.59320000000002), 'median_duration_us': np.float64(196.542), 'std_dev_duration_us': np.float64(0.4292092263686784), 'min_duration_us': np.float64(195.966), 'max_duration_us': np.float64(197.245)}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16, __nv_bfloat16, float, true, false, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nhwc2nchw_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(48.35), 'mean_duration_us': np.float64(9.67), 'median_duration_us': np.float64(9.663), 'std_dev_duration_us': np.float64(0.0547539952880155), 'min_duration_us': np.float64(9.6), 'max_duration_us': np.float64(9.759)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': 28.127000000000002, 'mean_duration_us': 5.625400000000001, 'median_duration_us': 5.664, 'std_dev_duration_us': 0.08941498755801505, 'min_duration_us': 5.503, 'max_duration_us': 5.728}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 222.207, 'mean_duration_us': 44.4414, 'median_duration_us': 44.384, 'std_dev_duration_us': 0.1792647204555328, 'min_duration_us': 44.224, 'max_duration_us': 44.768}, {'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': 10.85, 'mean_duration_us': 2.17, 'median_duration_us': 2.176, 'std_dev_duration_us': 0.013007690033207267, 'min_duration_us': 2.144, 'max_duration_us': 2.177}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 58.303000000000004, 'mean_duration_us': 11.6606, 'median_duration_us': 11.679, 'std_dev_duration_us': 0.15088485676170435, 'min_duration_us': 11.424, 'max_duration_us': 11.872}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8&gt;(cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8::Params)', 'stream': 7, 'count': 5, 'total_duration_us': 982.9660000000001, 'mean_duration_us': 196.59320000000002, 'median_duration_us': 196.542, 'std_dev_duration_us': 0.4292092263686784, 'min_duration_us': 195.966, 'max_duration_us': 197.245}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16, __nv_bfloat16, float, true, false, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nhwc2nchw_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 48.35, 'mean_duration_us': 9.67, 'median_duration_us': 9.663, 'std_dev_duration_us': 0.0547539952880155, 'min_duration_us': 9.6, 'max_duration_us': 9.759}]</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(5.63)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': np.float64(44.44)}, {'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(2.17)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': np.float64(11.66)}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop...', 'stream': 7, 'mean_duration_us': np.float64(196.59)}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': np.float64(9.67)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 5.63}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': 44.44}, {'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 2.17}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': 11.66}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop...', 'stream': 7, 'mean_duration_us': 196.59}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': 9.67}]</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
@@ -11081,12 +11081,12 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8133.554), 'mean_duration_us': np.float64(1626.7108), 'median_duration_us': np.float64(347.196), 'std_dev_duration_us': np.float64(1579.6924965375256), 'min_duration_us': np.float64(325.565), 'max_duration_us': np.float64(3620.445)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 8133.554, 'mean_duration_us': 1626.7108, 'median_duration_us': 347.196, 'std_dev_duration_us': 1579.6924965375256, 'min_duration_us': 325.565, 'max_duration_us': 3620.445}]</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(1626.71)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 1626.71}]</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -11201,12 +11201,12 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 360, 'total_duration_us': np.float64(5038.033), 'mean_duration_us': np.float64(13.994536111111112), 'median_duration_us': np.float64(13.152), 'std_dev_duration_us': np.float64(1.3500063184322875), 'min_duration_us': np.float64(12.736), 'max_duration_us': np.float64(16.288)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 360, 'total_duration_us': 5038.033, 'mean_duration_us': 13.994536111111112, 'median_duration_us': 13.152, 'std_dev_duration_us': 1.3500063184322875, 'min_duration_us': 12.736, 'max_duration_us': 16.288}]</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(13.99)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 13.99}]</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -11317,12 +11317,12 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(3988.498), 'mean_duration_us': np.float64(33.23748333333334), 'median_duration_us': np.float64(33.055), 'std_dev_duration_us': np.float64(0.39268874407375365), 'min_duration_us': np.float64(32.8), 'max_duration_us': np.float64(34.272)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 3988.498, 'mean_duration_us': 33.23748333333334, 'median_duration_us': 33.055, 'std_dev_duration_us': 0.39268874407375365, 'min_duration_us': 32.8, 'max_duration_us': 34.272}]</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': np.float64(33.24)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': 33.24}]</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -11437,12 +11437,12 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(2338.761), 'mean_duration_us': np.float64(467.7522), 'median_duration_us': np.float64(464.252), 'std_dev_duration_us': np.float64(11.281809454161158), 'min_duration_us': np.float64(454.556), 'max_duration_us': np.float64(487.899)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 2338.761, 'mean_duration_us': 467.7522, 'median_duration_us': 464.252, 'std_dev_duration_us': 11.281809454161158, 'min_duration_us': 454.556, 'max_duration_us': 487.899}]</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(467.75)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 467.75}]</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -11557,12 +11557,12 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(2324.394), 'mean_duration_us': np.float64(464.87879999999996), 'median_duration_us': np.float64(472.188), 'std_dev_duration_us': np.float64(19.601893596282974), 'min_duration_us': np.float64(436.444), 'max_duration_us': np.float64(489.34)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 2324.394, 'mean_duration_us': 464.87879999999996, 'median_duration_us': 472.188, 'std_dev_duration_us': 19.601893596282974, 'min_duration_us': 436.444, 'max_duration_us': 489.34}]</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(464.88)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 464.88}]</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -11677,12 +11677,12 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(1873.8329999999999), 'mean_duration_us': np.float64(15.615274999999999), 'median_duration_us': np.float64(15.584), 'std_dev_duration_us': np.float64(0.1854254999768552), 'min_duration_us': np.float64(15.264), 'max_duration_us': np.float64(16.384)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': 1873.8329999999999, 'mean_duration_us': 15.615274999999999, 'median_duration_us': 15.584, 'std_dev_duration_us': 0.1854254999768552, 'min_duration_us': 15.264, 'max_duration_us': 16.384}]</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(15.62)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 15.62}]</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -11797,12 +11797,12 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(1627.952), 'mean_duration_us': np.float64(325.5904), 'median_duration_us': np.float64(333.501), 'std_dev_duration_us': np.float64(11.368233417730304), 'min_duration_us': np.float64(304.989), 'max_duration_us': np.float64(334.205)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': 1627.952, 'mean_duration_us': 325.5904, 'median_duration_us': 333.501, 'std_dev_duration_us': 11.368233417730304, 'min_duration_us': 304.989, 'max_duration_us': 334.205}]</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(325.59)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 325.59}]</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -11917,12 +11917,12 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 180, 'total_duration_us': np.float64(457.9199999999999), 'mean_duration_us': np.float64(2.5439999999999996), 'median_duration_us': np.float64(2.4645), 'std_dev_duration_us': np.float64(0.22104903930525865), 'min_duration_us': np.float64(2.24), 'max_duration_us': np.float64(3.232)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 180, 'total_duration_us': 457.9199999999999, 'mean_duration_us': 2.5439999999999996, 'median_duration_us': 2.4645, 'std_dev_duration_us': 0.22104903930525865, 'min_duration_us': 2.24, 'max_duration_us': 3.232}]</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.54)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.54}]</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -12037,12 +12037,12 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(163.17200000000005), 'mean_duration_us': np.float64(2.719533333333334), 'median_duration_us': np.float64(2.784), 'std_dev_duration_us': np.float64(0.14011381881250043), 'min_duration_us': np.float64(2.527), 'max_duration_us': np.float64(3.008)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 60, 'total_duration_us': 163.17200000000005, 'mean_duration_us': 2.719533333333334, 'median_duration_us': 2.784, 'std_dev_duration_us': 0.14011381881250043, 'min_duration_us': 2.527, 'max_duration_us': 3.008}]</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.72)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.72}]</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -12153,12 +12153,12 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(105.02100000000002), 'mean_duration_us': np.float64(1.7503500000000003), 'median_duration_us': np.float64(1.76), 'std_dev_duration_us': np.float64(0.021235838418422137), 'min_duration_us': np.float64(1.696), 'max_duration_us': np.float64(1.792)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 105.02100000000002, 'mean_duration_us': 1.7503500000000003, 'median_duration_us': 1.76, 'std_dev_duration_us': 0.021235838418422137, 'min_duration_us': 1.696, 'max_duration_us': 1.792}]</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': np.float64(1.75)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': 1.75}]</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
@@ -12273,12 +12273,12 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(20.255), 'mean_duration_us': np.float64(4.051), 'median_duration_us': np.float64(4.032), 'std_dev_duration_us': np.float64(0.02550294100687212), 'min_duration_us': np.float64(4.032), 'max_duration_us': np.float64(4.096)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': 20.255, 'mean_duration_us': 4.051, 'median_duration_us': 4.032, 'std_dev_duration_us': 0.02550294100687212, 'min_duration_us': 4.032, 'max_duration_us': 4.096}]</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(4.05)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 4.05}]</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
@@ -12379,12 +12379,12 @@
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(17.44), 'mean_duration_us': np.float64(1.7440000000000002), 'median_duration_us': np.float64(1.7440000000000002), 'std_dev_duration_us': np.float64(0.9569284194755635), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(2.72)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': 17.44, 'mean_duration_us': 1.7440000000000002, 'median_duration_us': 1.7440000000000002, 'std_dev_duration_us': 0.9569284194755635, 'min_duration_us': 0.768, 'max_duration_us': 2.72}]</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(1.74)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 1.74}]</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
@@ -12499,12 +12499,12 @@
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.717999999999998), 'mean_duration_us': np.float64(2.9435999999999996), 'median_duration_us': np.float64(2.944), 'std_dev_duration_us': np.float64(0.0004898979485565817), 'min_duration_us': np.float64(2.943), 'max_duration_us': np.float64(2.944)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 14.717999999999998, 'mean_duration_us': 2.9435999999999996, 'median_duration_us': 2.944, 'std_dev_duration_us': 0.0004898979485565817, 'min_duration_us': 2.943, 'max_duration_us': 2.944}]</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.94)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.94}]</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
@@ -12619,12 +12619,12 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.495999999999999), 'mean_duration_us': np.float64(2.8991999999999996), 'median_duration_us': np.float64(2.912), 'std_dev_duration_us': np.float64(0.032633724886993856), 'min_duration_us': np.float64(2.848), 'max_duration_us': np.float64(2.944)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 14.495999999999999, 'mean_duration_us': 2.8991999999999996, 'median_duration_us': 2.912, 'std_dev_duration_us': 0.032633724886993856, 'min_duration_us': 2.848, 'max_duration_us': 2.944}]</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.9)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.9}]</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
@@ -12739,12 +12739,12 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.985), 'mean_duration_us': np.float64(2.7969999999999997), 'median_duration_us': np.float64(2.785), 'std_dev_duration_us': np.float64(0.015517731793016621), 'min_duration_us': np.float64(2.784), 'max_duration_us': np.float64(2.816)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 13.985, 'mean_duration_us': 2.7969999999999997, 'median_duration_us': 2.785, 'std_dev_duration_us': 0.015517731793016621, 'min_duration_us': 2.784, 'max_duration_us': 2.816}]</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': np.float64(2.8)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': 2.8}]</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
@@ -12859,12 +12859,12 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.472000000000001), 'mean_duration_us': np.float64(2.6944000000000004), 'median_duration_us': np.float64(2.752), 'std_dev_duration_us': np.float64(0.10398769157934018), 'min_duration_us': np.float64(2.528), 'max_duration_us': np.float64(2.816)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 13.472000000000001, 'mean_duration_us': 2.6944000000000004, 'median_duration_us': 2.752, 'std_dev_duration_us': 0.10398769157934018, 'min_duration_us': 2.528, 'max_duration_us': 2.816}]</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.69)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.69}]</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
@@ -12979,12 +12979,12 @@
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.407000000000002), 'mean_duration_us': np.float64(2.6814000000000004), 'median_duration_us': np.float64(2.656), 'std_dev_duration_us': np.float64(0.07142996570067763), 'min_duration_us': np.float64(2.623), 'max_duration_us': np.float64(2.816)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 13.407000000000002, 'mean_duration_us': 2.6814000000000004, 'median_duration_us': 2.656, 'std_dev_duration_us': 0.07142996570067763, 'min_duration_us': 2.623, 'max_duration_us': 2.816}]</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.68)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.68}]</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
@@ -13099,12 +13099,12 @@
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.345), 'mean_duration_us': np.float64(2.669), 'median_duration_us': np.float64(2.72), 'std_dev_duration_us': np.float64(0.08978641322605552), 'min_duration_us': np.float64(2.56), 'max_duration_us': np.float64(2.753)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 13.345, 'mean_duration_us': 2.669, 'median_duration_us': 2.72, 'std_dev_duration_us': 0.08978641322605552, 'min_duration_us': 2.56, 'max_duration_us': 2.753}]</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.67)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.67}]</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
@@ -13219,12 +13219,12 @@
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(12.222999999999999), 'mean_duration_us': np.float64(2.4446), 'median_duration_us': np.float64(2.336), 'std_dev_duration_us': np.float64(0.1469742834648294), 'min_duration_us': np.float64(2.303), 'max_duration_us': np.float64(2.624)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 12.222999999999999, 'mean_duration_us': 2.4446, 'median_duration_us': 2.336, 'std_dev_duration_us': 0.1469742834648294, 'min_duration_us': 2.303, 'max_duration_us': 2.624}]</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.44)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.44}]</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
@@ -13339,12 +13339,12 @@
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(11.904), 'mean_duration_us': np.float64(2.3808), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.04340691189200176), 'min_duration_us': np.float64(2.336), 'max_duration_us': np.float64(2.464)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 11.904, 'mean_duration_us': 2.3808, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.04340691189200176, 'min_duration_us': 2.336, 'max_duration_us': 2.464}]</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.38)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.38}]</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
@@ -13459,12 +13459,12 @@
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(11.904), 'mean_duration_us': np.float64(2.3808), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.0478932145507065), 'min_duration_us': np.float64(2.336), 'max_duration_us': np.float64(2.464)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 11.904, 'mean_duration_us': 2.3808, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.0478932145507065, 'min_duration_us': 2.336, 'max_duration_us': 2.464}]</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.38)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.38}]</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
@@ -13575,12 +13575,12 @@
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.896), 'mean_duration_us': np.float64(1.7792000000000001), 'median_duration_us': np.float64(1.792), 'std_dev_duration_us': np.float64(0.025600000000000022), 'min_duration_us': np.float64(1.728), 'max_duration_us': np.float64(1.792)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.896, 'mean_duration_us': 1.7792000000000001, 'median_duration_us': 1.792, 'std_dev_duration_us': 0.025600000000000022, 'min_duration_us': 1.728, 'max_duration_us': 1.792}]</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': np.float64(1.78)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': 1.78}]</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
@@ -13681,12 +13681,12 @@
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.769), 'mean_duration_us': np.float64(1.7538), 'median_duration_us': np.float64(1.792), 'std_dev_duration_us': np.float64(0.0742762411542211), 'min_duration_us': np.float64(1.664), 'max_duration_us': np.float64(1.825)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.769, 'mean_duration_us': 1.7538, 'median_duration_us': 1.792, 'std_dev_duration_us': 0.0742762411542211, 'min_duration_us': 1.664, 'max_duration_us': 1.825}]</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': np.float64(1.75)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': 1.75}]</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
@@ -13787,12 +13787,12 @@
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.64), 'mean_duration_us': np.float64(1.7280000000000002), 'median_duration_us': np.float64(1.696), 'std_dev_duration_us': np.float64(0.10516273104099186), 'min_duration_us': np.float64(1.6), 'max_duration_us': np.float64(1.92)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.64, 'mean_duration_us': 1.7280000000000002, 'median_duration_us': 1.696, 'std_dev_duration_us': 0.10516273104099186, 'min_duration_us': 1.6, 'max_duration_us': 1.92}]</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': np.float64(1.73)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': 1.73}]</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
@@ -13907,12 +13907,12 @@
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(7.968), 'mean_duration_us': np.float64(0.7968), 'median_duration_us': np.float64(0.8), 'std_dev_duration_us': np.float64(0.009600000000000008), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(0.8)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': 7.968, 'mean_duration_us': 0.7968, 'median_duration_us': 0.8, 'std_dev_duration_us': 0.009600000000000008, 'min_duration_us': 0.768, 'max_duration_us': 0.8}]</t>
         </is>
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(0.8)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 0.8}]</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
@@ -14027,12 +14027,12 @@
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.008999999999999), 'mean_duration_us': np.float64(1.4017999999999997), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.08894132897590411), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.504)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.008999999999999, 'mean_duration_us': 1.4017999999999997, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.08894132897590411, 'min_duration_us': 1.28, 'max_duration_us': 1.504}]</t>
         </is>
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bf...', 'stream': 7, 'mean_duration_us': np.float64(1.4)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bf...', 'stream': 7, 'mean_duration_us': 1.4}]</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
@@ -14147,12 +14147,12 @@
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(6.687999999999999), 'mean_duration_us': np.float64(1.3375999999999997), 'median_duration_us': np.float64(1.408), 'std_dev_duration_us': np.float64(0.0868138237840034), 'min_duration_us': np.float64(1.216), 'max_duration_us': np.float64(1.408)}]</t>
+          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': 6.687999999999999, 'mean_duration_us': 1.3375999999999997, 'median_duration_us': 1.408, 'std_dev_duration_us': 0.0868138237840034, 'min_duration_us': 1.216, 'max_duration_us': 1.408}]</t>
         </is>
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(1.34)}]</t>
+          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'mean_duration_us': 1.34}]</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
@@ -14208,28 +14208,32 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>(1, 3, 1008, 1008)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>('float', None)</t>
+          <t>('c10::BFloat16', 'float')</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>()</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
+          <t>(3048192, 1016064, 1008, 1)</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>(3048192, 1016064, 1008, 1)</t>
+        </is>
+      </c>
       <c r="F29" t="n">
-        <v>1e-09</v>
+        <v>0.003048192</v>
       </c>
       <c r="G29" t="n">
-        <v>7.62939453125e-06</v>
+        <v>17.44189453125</v>
       </c>
       <c r="H29" t="n">
-        <v>0.125</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
@@ -14249,17 +14253,17 @@
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr">
         <is>
-          <t>[[], [], []]</t>
+          <t>[[1, 3, 1008, 1008], [1, 3, 1008, 1008], []]</t>
         </is>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>['float', 'double', 'Scalar']</t>
+          <t>['c10::BFloat16', 'float', 'Scalar']</t>
         </is>
       </c>
       <c r="W29" t="inlineStr">
         <is>
-          <t>[[], [], []]</t>
+          <t>[[3048192, 1016064, 1008, 1], [3048192, 1016064, 1008, 1], []]</t>
         </is>
       </c>
       <c r="X29" t="inlineStr">
@@ -14289,43 +14293,39 @@
         <v>5</v>
       </c>
       <c r="AF29" t="n">
-        <v>23848</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>aten::copy_</t>
+          <t>aten::sigmoid</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>(1, 3, 1008, 1008)</t>
+          <t>(1, 5184)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>('c10::BFloat16', 'float')</t>
+          <t>('float', None)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>(3048192, 1016064, 1008, 1)</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>(3048192, 1016064, 1008, 1)</t>
-        </is>
-      </c>
+          <t>(5184, 1)</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>0.003048192</v>
+        <v>5.184e-06</v>
       </c>
       <c r="G30" t="n">
-        <v>17.44189453125</v>
+        <v>0.03955078125</v>
       </c>
       <c r="H30" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
@@ -14345,22 +14345,22 @@
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr">
         <is>
-          <t>[[1, 3, 1008, 1008], [1, 3, 1008, 1008], []]</t>
+          <t>[[1, 5184]]</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>['c10::BFloat16', 'float', 'Scalar']</t>
+          <t>['float']</t>
         </is>
       </c>
       <c r="W30" t="inlineStr">
         <is>
-          <t>[[3048192, 1016064, 1008, 1], [3048192, 1016064, 1008, 1], []]</t>
+          <t>[[5184, 1]]</t>
         </is>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>['', '', 'False']</t>
+          <t>['']</t>
         </is>
       </c>
       <c r="Y30" t="n">
@@ -14385,7 +14385,7 @@
         <v>5</v>
       </c>
       <c r="AF30" t="n">
-        <v>22</v>
+        <v>23763</v>
       </c>
     </row>
     <row r="31">
@@ -14396,29 +14396,29 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>(1, 1, 4)</t>
+          <t>()</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>('c10::BFloat16', 'int')</t>
+          <t>('c10::BFloat16', None)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>(4, 4, 1)</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>(4, 4, 1)</t>
-        </is>
-      </c>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
-        <v>4e-09</v>
-      </c>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
+        <v>1e-09</v>
+      </c>
+      <c r="G31" t="n">
+        <v>3.814697265625e-06</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.25</v>
+      </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
@@ -14437,17 +14437,17 @@
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr">
         <is>
-          <t>[[1, 1, 4], [1, 1, 4], []]</t>
+          <t>[[], [], []]</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>['c10::BFloat16', 'int', 'Scalar']</t>
+          <t>['c10::BFloat16', 'double', 'Scalar']</t>
         </is>
       </c>
       <c r="W31" t="inlineStr">
         <is>
-          <t>[[4, 4, 1], [4, 4, 1], []]</t>
+          <t>[[], [], []]</t>
         </is>
       </c>
       <c r="X31" t="inlineStr">
@@ -14474,10 +14474,10 @@
         <v>0</v>
       </c>
       <c r="AE31" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AF31" t="n">
-        <v>23834</v>
+        <v>23777</v>
       </c>
     </row>
     <row r="32">
@@ -14488,29 +14488,29 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>(1, 1, 4)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>('c10::BFloat16', None)</t>
+          <t>('c10::BFloat16', 'int')</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>()</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>(4, 4, 1)</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>(4, 4, 1)</t>
+        </is>
+      </c>
       <c r="F32" t="n">
-        <v>1e-09</v>
-      </c>
-      <c r="G32" t="n">
-        <v>3.814697265625e-06</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0.25</v>
-      </c>
+        <v>4e-09</v>
+      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
@@ -14529,17 +14529,17 @@
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr">
         <is>
-          <t>[[], [], []]</t>
+          <t>[[1, 1, 4], [1, 1, 4], []]</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>['c10::BFloat16', 'double', 'Scalar']</t>
+          <t>['c10::BFloat16', 'int', 'Scalar']</t>
         </is>
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>[[], [], []]</t>
+          <t>[[4, 4, 1], [4, 4, 1], []]</t>
         </is>
       </c>
       <c r="X32" t="inlineStr">
@@ -14566,21 +14566,21 @@
         <v>0</v>
       </c>
       <c r="AE32" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AF32" t="n">
-        <v>23777</v>
+        <v>23834</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>aten::sigmoid</t>
+          <t>aten::copy_</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>(1, 5184)</t>
+          <t>()</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -14590,15 +14590,15 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>(5184, 1)</t>
+          <t>()</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
-        <v>5.184e-06</v>
+        <v>1e-09</v>
       </c>
       <c r="G33" t="n">
-        <v>0.03955078125</v>
+        <v>7.62939453125e-06</v>
       </c>
       <c r="H33" t="n">
         <v>0.125</v>
@@ -14621,22 +14621,22 @@
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr">
         <is>
-          <t>[[1, 5184]]</t>
+          <t>[[], [], []]</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>['float']</t>
+          <t>['float', 'double', 'Scalar']</t>
         </is>
       </c>
       <c r="W33" t="inlineStr">
         <is>
-          <t>[[5184, 1]]</t>
+          <t>[[], [], []]</t>
         </is>
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>['']</t>
+          <t>['', '', 'False']</t>
         </is>
       </c>
       <c r="Y33" t="n">
@@ -14661,7 +14661,7 @@
         <v>5</v>
       </c>
       <c r="AF33" t="n">
-        <v>23763</v>
+        <v>23848</v>
       </c>
     </row>
   </sheetData>
@@ -14928,12 +14928,12 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(5223.73), 'mean_duration_us': np.float64(43.53108333333333), 'median_duration_us': np.float64(43.3595), 'std_dev_duration_us': np.float64(0.6410638629566389), 'min_duration_us': np.float64(42.656), 'max_duration_us': np.float64(44.704)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 5223.73, 'mean_duration_us': 43.53108333333333, 'median_duration_us': 43.3595, 'std_dev_duration_us': 0.6410638629566389, 'min_duration_us': 42.656, 'max_duration_us': 44.704}]</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(43.53)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 43.53}]</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
@@ -15054,12 +15054,12 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(3687.3240000000005), 'mean_duration_us': np.float64(30.727700000000006), 'median_duration_us': np.float64(30.591), 'std_dev_duration_us': np.float64(0.3214868737600341), 'min_duration_us': np.float64(30.336), 'max_duration_us': np.float64(31.711)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 3687.3240000000005, 'mean_duration_us': 30.727700000000006, 'median_duration_us': 30.591, 'std_dev_duration_us': 0.3214868737600341, 'min_duration_us': 30.336, 'max_duration_us': 31.711}]</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(30.73)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 30.73}]</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
@@ -15180,12 +15180,12 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 245, 'total_duration_us': np.float64(2317.353), 'mean_duration_us': np.float64(9.458583673469388), 'median_duration_us': np.float64(9.472), 'std_dev_duration_us': np.float64(0.3348456698101192), 'min_duration_us': np.float64(8.576), 'max_duration_us': np.float64(10.849)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 245, 'total_duration_us': 2317.353, 'mean_duration_us': 9.458583673469388, 'median_duration_us': 9.472, 'std_dev_duration_us': 0.3348456698101192, 'min_duration_us': 8.576, 'max_duration_us': 10.849}]</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(9.46)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 9.46}]</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
@@ -15306,12 +15306,12 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(934.809), 'mean_duration_us': np.float64(7.790075), 'median_duration_us': np.float64(7.776), 'std_dev_duration_us': np.float64(0.06863528763204346), 'min_duration_us': np.float64(7.711), 'max_duration_us': np.float64(8.032)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 934.809, 'mean_duration_us': 7.790075, 'median_duration_us': 7.776, 'std_dev_duration_us': 0.06863528763204346, 'min_duration_us': 7.711, 'max_duration_us': 8.032}]</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(7.79)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 7.79}]</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -15432,12 +15432,12 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(287.13699999999994), 'mean_duration_us': np.float64(2.392808333333333), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.24387456802740948), 'min_duration_us': np.float64(1.984), 'max_duration_us': np.float64(2.913)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': 287.13699999999994, 'mean_duration_us': 2.392808333333333, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.24387456802740948, 'min_duration_us': 1.984, 'max_duration_us': 2.913}]</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.39)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.39}]</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
@@ -15558,12 +15558,12 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 125, 'total_duration_us': np.float64(187.747), 'mean_duration_us': np.float64(1.5019760000000002), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.09206636423797784), 'min_duration_us': np.float64(1.344), 'max_duration_us': np.float64(1.633)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 125, 'total_duration_us': 187.747, 'mean_duration_us': 1.5019760000000002, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.09206636423797784, 'min_duration_us': 1.344, 'max_duration_us': 1.633}]</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.5)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.5}]</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
@@ -15684,12 +15684,12 @@
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(94.07899999999998), 'mean_duration_us': np.float64(1.567983333333333), 'median_duration_us': np.float64(1.568), 'std_dev_duration_us': np.float64(0.02925092116308288), 'min_duration_us': np.float64(1.535), 'max_duration_us': np.float64(1.633)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 94.07899999999998, 'mean_duration_us': 1.567983333333333, 'median_duration_us': 1.568, 'std_dev_duration_us': 0.02925092116308288, 'min_duration_us': 1.535, 'max_duration_us': 1.633}]</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(1.57)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 1.57}]</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -15810,12 +15810,12 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(89.14699999999999), 'mean_duration_us': np.float64(1.4857833333333332), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.016880058912482752), 'min_duration_us': np.float64(1.471), 'max_duration_us': np.float64(1.535)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 89.14699999999999, 'mean_duration_us': 1.4857833333333332, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.016880058912482752, 'min_duration_us': 1.471, 'max_duration_us': 1.535}]</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(1.49)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 1.49}]</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -15936,12 +15936,12 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(86.49500000000002), 'mean_duration_us': np.float64(1.4415833333333337), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.10003121040733015), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.568)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 86.49500000000002, 'mean_duration_us': 1.4415833333333337, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.10003121040733015, 'min_duration_us': 1.28, 'max_duration_us': 1.568}]</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(1.44)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 1.44}]</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
@@ -16062,12 +16062,12 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(65.407), 'mean_duration_us': np.float64(13.081399999999999), 'median_duration_us': np.float64(13.088), 'std_dev_duration_us': np.float64(0.058854396607220374), 'min_duration_us': np.float64(13.023), 'max_duration_us': np.float64(13.184)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 65.407, 'mean_duration_us': 13.081399999999999, 'median_duration_us': 13.088, 'std_dev_duration_us': 0.058854396607220374, 'min_duration_us': 13.023, 'max_duration_us': 13.184}]</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(13.08)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 13.08}]</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
@@ -16188,12 +16188,12 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(57.631), 'mean_duration_us': np.float64(11.5262), 'median_duration_us': np.float64(11.552), 'std_dev_duration_us': np.float64(0.0889413289759043), 'min_duration_us': np.float64(11.392), 'max_duration_us': np.float64(11.616)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 57.631, 'mean_duration_us': 11.5262, 'median_duration_us': 11.552, 'std_dev_duration_us': 0.0889413289759043, 'min_duration_us': 11.392, 'max_duration_us': 11.616}]</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(11.53)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 11.53}]</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
@@ -16314,12 +16314,12 @@
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(26.686999999999998), 'mean_duration_us': np.float64(2.6687), 'median_duration_us': np.float64(2.656), 'std_dev_duration_us': np.float64(0.20862696374150683), 'min_duration_us': np.float64(2.335), 'max_duration_us': np.float64(3.008)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 10, 'total_duration_us': 26.686999999999998, 'mean_duration_us': 2.6687, 'median_duration_us': 2.656, 'std_dev_duration_us': 0.20862696374150683, 'min_duration_us': 2.335, 'max_duration_us': 3.008}]</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.67)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.67}]</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
@@ -16440,12 +16440,12 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, 4, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(22.144000000000002), 'mean_duration_us': np.float64(4.428800000000001), 'median_duration_us': np.float64(4.416), 'std_dev_duration_us': np.float64(0.09621309682158638), 'min_duration_us': np.float64(4.32), 'max_duration_us': np.float64(4.608)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, 4, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 22.144000000000002, 'mean_duration_us': 4.428800000000001, 'median_duration_us': 4.416, 'std_dev_duration_us': 0.09621309682158638, 'min_duration_us': 4.32, 'max_duration_us': 4.608}]</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFun...', 'stream': 7, 'mean_duration_us': np.float64(4.43)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFun...', 'stream': 7, 'mean_duration_us': 4.43}]</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
@@ -16566,12 +16566,12 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.560000000000002), 'mean_duration_us': np.float64(2.9120000000000004), 'median_duration_us': np.float64(3.008), 'std_dev_duration_us': np.float64(0.21891368161903446), 'min_duration_us': np.float64(2.656), 'max_duration_us': np.float64(3.2)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 14.560000000000002, 'mean_duration_us': 2.9120000000000004, 'median_duration_us': 3.008, 'std_dev_duration_us': 0.21891368161903446, 'min_duration_us': 2.656, 'max_duration_us': 3.2}]</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.91)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.91}]</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
@@ -16692,12 +16692,12 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.799), 'mean_duration_us': np.float64(1.7597999999999998), 'median_duration_us': np.float64(1.76), 'std_dev_duration_us': np.float64(0.10100376230616363), 'min_duration_us': np.float64(1.632), 'max_duration_us': np.float64(1.888)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.799, 'mean_duration_us': 1.7597999999999998, 'median_duration_us': 1.76, 'std_dev_duration_us': 0.10100376230616363, 'min_duration_us': 1.632, 'max_duration_us': 1.888}]</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.76)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.76}]</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
@@ -16818,12 +16818,12 @@
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.030999999999999), 'mean_duration_us': np.float64(1.6061999999999999), 'median_duration_us': np.float64(1.632), 'std_dev_duration_us': np.float64(0.046786322787754936), 'min_duration_us': np.float64(1.536), 'max_duration_us': np.float64(1.663)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.030999999999999, 'mean_duration_us': 1.6061999999999999, 'median_duration_us': 1.632, 'std_dev_duration_us': 0.046786322787754936, 'min_duration_us': 1.536, 'max_duration_us': 1.663}]</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.61)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.61}]</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
@@ -16944,12 +16944,12 @@
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.872), 'mean_duration_us': np.float64(1.5744), 'median_duration_us': np.float64(1.568), 'std_dev_duration_us': np.float64(0.02394660727535325), 'min_duration_us': np.float64(1.536), 'max_duration_us': np.float64(1.6)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.872, 'mean_duration_us': 1.5744, 'median_duration_us': 1.568, 'std_dev_duration_us': 0.02394660727535325, 'min_duration_us': 1.536, 'max_duration_us': 1.6}]</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.57)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.57}]</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
@@ -17070,12 +17070,12 @@
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.744), 'mean_duration_us': np.float64(1.5488), 'median_duration_us': np.float64(1.6), 'std_dev_duration_us': np.float64(0.09185728060420688), 'min_duration_us': np.float64(1.408), 'max_duration_us': np.float64(1.632)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.744, 'mean_duration_us': 1.5488, 'median_duration_us': 1.6, 'std_dev_duration_us': 0.09185728060420688, 'min_duration_us': 1.408, 'max_duration_us': 1.632}]</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.55)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.55}]</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
@@ -17196,12 +17196,12 @@
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.424999999999999), 'mean_duration_us': np.float64(1.4849999999999999), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.025502941006872143), 'min_duration_us': np.float64(1.472), 'max_duration_us': np.float64(1.536)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.424999999999999, 'mean_duration_us': 1.4849999999999999, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.025502941006872143, 'min_duration_us': 1.472, 'max_duration_us': 1.536}]</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(1.48)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 1.48}]</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
@@ -17322,12 +17322,12 @@
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.264999999999999), 'mean_duration_us': np.float64(1.4529999999999998), 'median_duration_us': np.float64(1.441), 'std_dev_duration_us': np.float64(0.015517731793016656), 'min_duration_us': np.float64(1.44), 'max_duration_us': np.float64(1.472)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.264999999999999, 'mean_duration_us': 1.4529999999999998, 'median_duration_us': 1.441, 'std_dev_duration_us': 0.015517731793016656, 'min_duration_us': 1.44, 'max_duration_us': 1.472}]</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.45)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.45}]</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
@@ -17448,12 +17448,12 @@
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.007999999999999), 'mean_duration_us': np.float64(1.4015999999999997), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.08914168497397834), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.504)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.007999999999999, 'mean_duration_us': 1.4015999999999997, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.08914168497397834, 'min_duration_us': 1.28, 'max_duration_us': 1.504}]</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(1.4)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 1.4}]</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
@@ -17504,7 +17504,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>aten::add</t>
+          <t>aten::mul</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -17514,12 +17514,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>(1, 5184)</t>
+          <t>()</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>('c10::BFloat16', 'c10::BFloat16', None)</t>
+          <t>('c10::BFloat16', 'double', None)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -17529,7 +17529,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>(5184, 1)</t>
+          <t>()</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -17537,10 +17537,10 @@
         <v>5.184e-06</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0296630859375</v>
+        <v>0.01978302001953125</v>
       </c>
       <c r="J23" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.2499035865792518</v>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
@@ -17560,22 +17560,22 @@
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr">
         <is>
-          <t>[[1, 5184], [1, 5184], []]</t>
+          <t>[[1, 5184], []]</t>
         </is>
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>['c10::BFloat16', 'c10::BFloat16', 'Scalar']</t>
+          <t>['c10::BFloat16', 'double']</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>[[20736, 4], [5184, 1], []]</t>
+          <t>[[20736, 4], []]</t>
         </is>
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>['', '', '1']</t>
+          <t>['', '']</t>
         </is>
       </c>
       <c r="AA23" t="n">
@@ -17597,49 +17597,53 @@
         <v>0</v>
       </c>
       <c r="AG23" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AH23" t="n">
-        <v>23790</v>
+        <v>23773</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>aten::mul</t>
+          <t>aten::add</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>(1, 5184, 4)</t>
+          <t>(1, 5184)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>(1, 1, 4)</t>
+          <t>(1, 5184)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>('c10::BFloat16', 'int', None)</t>
+          <t>('c10::BFloat16', 'c10::BFloat16', None)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>(20736, 4, 1)</t>
+          <t>(20736, 4)</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>(4, 4, 1)</t>
+          <t>(5184, 1)</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
-        <v>2.0736e-05</v>
-      </c>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+        <v>5.184e-06</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.0296630859375</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
@@ -17658,22 +17662,22 @@
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr">
         <is>
-          <t>[[1, 5184, 4], [1, 1, 4]]</t>
+          <t>[[1, 5184], [1, 5184], []]</t>
         </is>
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>['c10::BFloat16', 'int']</t>
+          <t>['c10::BFloat16', 'c10::BFloat16', 'Scalar']</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
         <is>
-          <t>[[20736, 4, 1], [4, 4, 1]]</t>
+          <t>[[20736, 4], [5184, 1], []]</t>
         </is>
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>['', '']</t>
+          <t>['', '', '1']</t>
         </is>
       </c>
       <c r="AA24" t="n">
@@ -17695,10 +17699,10 @@
         <v>0</v>
       </c>
       <c r="AG24" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AH24" t="n">
-        <v>23830</v>
+        <v>23790</v>
       </c>
     </row>
     <row r="25">
@@ -17709,39 +17713,35 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>(1, 5184)</t>
+          <t>(1, 5184, 4)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>(1, 1, 4)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>('c10::BFloat16', 'double', None)</t>
+          <t>('c10::BFloat16', 'int', None)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>(20736, 4)</t>
+          <t>(20736, 4, 1)</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>(4, 4, 1)</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
-        <v>5.184e-06</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0.01978302001953125</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0.2499035865792518</v>
-      </c>
+        <v>2.0736e-05</v>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
@@ -17760,17 +17760,17 @@
       <c r="V25" t="inlineStr"/>
       <c r="W25" t="inlineStr">
         <is>
-          <t>[[1, 5184], []]</t>
+          <t>[[1, 5184, 4], [1, 1, 4]]</t>
         </is>
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>['c10::BFloat16', 'double']</t>
+          <t>['c10::BFloat16', 'int']</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>[[20736, 4], []]</t>
+          <t>[[20736, 4, 1], [4, 4, 1]]</t>
         </is>
       </c>
       <c r="Z25" t="inlineStr">
@@ -17797,10 +17797,10 @@
         <v>0</v>
       </c>
       <c r="AG25" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AH25" t="n">
-        <v>23773</v>
+        <v>23830</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(tests): resolve non-determinism in perf report comparison (#385)
The  test was failing intermittently due to two main issues:

1. The row order in the sheet was not deterministic when multiple
operations had the same total kernel time.
2. The test comparison was too strict, failing on minor floating-point
differences within complex object columns and on type mismatches between
Python floats and NumPy scalars.

This commit resolves these issues by:
- Adding  as a secondary sort key in  to guarantee a stable row order.
- Implementing a recursive comparison function in the test to compare
nested floats with a tolerance.
- Improving the value normalization logic to handle string
representations of NumPy types read from reference Excel files.
</commit_message>
<xml_diff>
--- a/tests/traces/h100/google_owlv2-large-patch14-ensemble__1016001_perf_report.xlsx
+++ b/tests/traces/h100/google_owlv2-large-patch14-ensemble__1016001_perf_report.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="gpu_timeline" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ops_summary_by_category" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="ops_summary" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="ops_unique_args" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="GEMM" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="CONV_fwd" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="UnaryElementwise" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="BinaryElementwise" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gpu_timeline" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ops_summary_by_category" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ops_summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ops_unique_args" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GEMM" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CONV_fwd" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UnaryElementwise" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BinaryElementwise" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1527,12 +1527,12 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::cunn_SoftMaxForward&lt;8, c10::BFloat16, float, c10::BFloat16, at::native::(anonymous namespace)::SoftMaxForwardEpilogue&gt;(c10::BFloat16*, c10::BFloat16 const*, int)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(262422.467), 'mean_duration_us': np.float64(2186.8538916666666), 'median_duration_us': np.float64(2170.955), 'std_dev_duration_us': np.float64(52.45910857528236), 'min_duration_us': np.float64(2146.764), 'max_duration_us': np.float64(2395.817)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::cunn_SoftMaxForward&lt;8, c10::BFloat16, float, c10::BFloat16, at::native::(anonymous namespace)::SoftMaxForwardEpilogue&gt;(c10::BFloat16*, c10::BFloat16 const*, int)', 'stream': 7, 'count': 120, 'total_duration_us': 262422.467, 'mean_duration_us': 2186.8538916666666, 'median_duration_us': 2170.955, 'std_dev_duration_us': 52.45910857528236, 'min_duration_us': 2146.764, 'max_duration_us': 2395.817}]</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::cunn_SoftMaxForward&lt;8, c...', 'stream': 7, 'mean_duration_us': np.float64(2186.85)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::cunn_SoftMaxForward&lt;8, c...', 'stream': 7, 'mean_duration_us': 2186.85}]</t>
         </is>
       </c>
       <c r="P2" t="n">
@@ -1594,12 +1594,12 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(130015.7), 'mean_duration_us': np.float64(1083.4641666666666), 'median_duration_us': np.float64(1082.965), 'std_dev_duration_us': np.float64(3.932529614919927), 'min_duration_us': np.float64(1075.574), 'max_duration_us': np.float64(1096.694)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': 130015.7, 'mean_duration_us': 1083.4641666666666, 'median_duration_us': 1082.965, 'std_dev_duration_us': 3.932529614919927, 'min_duration_us': 1075.574, 'max_duration_us': 1096.694}]</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_25...', 'stream': 7, 'mean_duration_us': np.float64(1083.46)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_25...', 'stream': 7, 'mean_duration_us': 1083.46}]</t>
         </is>
       </c>
       <c r="P3" t="n">
@@ -1661,12 +1661,12 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(99311.41), 'mean_duration_us': np.float64(827.5950833333334), 'median_duration_us': np.float64(826.9205), 'std_dev_duration_us': np.float64(2.9474507419783706), 'min_duration_us': np.float64(825.432), 'max_duration_us': np.float64(851.8)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': 99311.41, 'mean_duration_us': 827.5950833333334, 'median_duration_us': 826.9205, 'std_dev_duration_us': 2.9474507419783706, 'min_duration_us': 825.432, 'max_duration_us': 851.8}]</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_12...', 'stream': 7, 'mean_duration_us': np.float64(827.6)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_12...', 'stream': 7, 'mean_duration_us': 827.6}]</t>
         </is>
       </c>
       <c r="P4" t="n">
@@ -1728,12 +1728,12 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 480, 'total_duration_us': np.float64(449.6640000000001), 'mean_duration_us': np.float64(0.9368000000000002), 'median_duration_us': np.float64(0.96), 'std_dev_duration_us': np.float64(0.14700191892171566), 'min_duration_us': np.float64(0.767), 'max_duration_us': np.float64(1.408)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 480, 'total_duration_us': np.float64(10035.521), 'mean_duration_us': np.float64(20.90733541666667), 'median_duration_us': np.float64(20.912), 'std_dev_duration_us': np.float64(0.2994497001373127), 'min_duration_us': np.float64(20.256), 'max_duration_us': np.float64(22.015)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 480, 'total_duration_us': 449.6640000000001, 'mean_duration_us': 0.9368000000000002, 'median_duration_us': 0.96, 'std_dev_duration_us': 0.14700191892171566, 'min_duration_us': 0.767, 'max_duration_us': 1.408}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 480, 'total_duration_us': 10035.521, 'mean_duration_us': 20.90733541666667, 'median_duration_us': 20.912, 'std_dev_duration_us': 0.2994497001373127, 'min_duration_us': 20.256, 'max_duration_us': 22.015}]</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.94)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(20.91)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.94}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 20.91}]</t>
         </is>
       </c>
       <c r="P5" t="n">
@@ -1795,12 +1795,12 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8133.554), 'mean_duration_us': np.float64(1626.7108), 'median_duration_us': np.float64(347.196), 'std_dev_duration_us': np.float64(1579.6924965375256), 'min_duration_us': np.float64(325.565), 'max_duration_us': np.float64(3620.445)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 8133.554, 'mean_duration_us': 1626.7108, 'median_duration_us': 347.196, 'std_dev_duration_us': 1579.6924965375256, 'min_duration_us': 325.565, 'max_duration_us': 3620.445}]</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(1626.71)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 1626.71}]</t>
         </is>
       </c>
       <c r="P6" t="n">
@@ -1862,12 +1862,12 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(115.61200000000002), 'mean_duration_us': np.float64(0.9634333333333335), 'median_duration_us': np.float64(0.96), 'std_dev_duration_us': np.float64(0.18370559478566667), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(1.6)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(7766.737), 'mean_duration_us': np.float64(64.72280833333333), 'median_duration_us': np.float64(64.639), 'std_dev_duration_us': np.float64(0.5570301951096441), 'min_duration_us': np.float64(63.711), 'max_duration_us': np.float64(65.951)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': 115.61200000000002, 'mean_duration_us': 0.9634333333333335, 'median_duration_us': 0.96, 'std_dev_duration_us': 0.18370559478566667, 'min_duration_us': 0.768, 'max_duration_us': 1.6}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': 7766.737, 'mean_duration_us': 64.72280833333333, 'median_duration_us': 64.639, 'std_dev_duration_us': 0.5570301951096441, 'min_duration_us': 63.711, 'max_duration_us': 65.951}]</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.96)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(64.72)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.96}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 64.72}]</t>
         </is>
       </c>
       <c r="P7" t="n">
@@ -1929,12 +1929,12 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(116.09), 'mean_duration_us': np.float64(0.9674166666666667), 'median_duration_us': np.float64(0.96), 'std_dev_duration_us': np.float64(0.15527371441711854), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(1.568)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(6884.5689999999995), 'mean_duration_us': np.float64(57.37140833333333), 'median_duration_us': np.float64(57.344), 'std_dev_duration_us': np.float64(0.31250691981227396), 'min_duration_us': np.float64(56.639), 'max_duration_us': np.float64(58.048)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': 116.09, 'mean_duration_us': 0.9674166666666667, 'median_duration_us': 0.96, 'std_dev_duration_us': 0.15527371441711854, 'min_duration_us': 0.768, 'max_duration_us': 1.568}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': 6884.5689999999995, 'mean_duration_us': 57.37140833333333, 'median_duration_us': 57.344, 'std_dev_duration_us': 0.31250691981227396, 'min_duration_us': 56.639, 'max_duration_us': 58.048}]</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.97)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(57.37)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.97}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 57.37}]</t>
         </is>
       </c>
       <c r="P8" t="n">
@@ -1996,12 +1996,12 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(5223.73), 'mean_duration_us': np.float64(43.53108333333333), 'median_duration_us': np.float64(43.3595), 'std_dev_duration_us': np.float64(0.6410638629566389), 'min_duration_us': np.float64(42.656), 'max_duration_us': np.float64(44.704)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 5223.73, 'mean_duration_us': 43.53108333333333, 'median_duration_us': 43.3595, 'std_dev_duration_us': 0.6410638629566389, 'min_duration_us': 42.656, 'max_duration_us': 44.704}]</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(43.53)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 43.53}]</t>
         </is>
       </c>
       <c r="P9" t="n">
@@ -2063,12 +2063,12 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 360, 'total_duration_us': np.float64(5038.033), 'mean_duration_us': np.float64(13.994536111111112), 'median_duration_us': np.float64(13.152), 'std_dev_duration_us': np.float64(1.3500063184322875), 'min_duration_us': np.float64(12.736), 'max_duration_us': np.float64(16.288)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 360, 'total_duration_us': 5038.033, 'mean_duration_us': 13.994536111111112, 'median_duration_us': 13.152, 'std_dev_duration_us': 1.3500063184322875, 'min_duration_us': 12.736, 'max_duration_us': 16.288}]</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(13.99)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 13.99}]</t>
         </is>
       </c>
       <c r="P10" t="n">
@@ -2130,12 +2130,12 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(3988.498), 'mean_duration_us': np.float64(33.23748333333334), 'median_duration_us': np.float64(33.055), 'std_dev_duration_us': np.float64(0.39268874407375365), 'min_duration_us': np.float64(32.8), 'max_duration_us': np.float64(34.272)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 3988.498, 'mean_duration_us': 33.23748333333334, 'median_duration_us': 33.055, 'std_dev_duration_us': 0.39268874407375365, 'min_duration_us': 32.8, 'max_duration_us': 34.272}]</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': np.float64(33.24)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': 33.24}]</t>
         </is>
       </c>
       <c r="P11" t="n">
@@ -2197,12 +2197,12 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 250, 'total_duration_us': np.float64(3701.084), 'mean_duration_us': np.float64(14.804336), 'median_duration_us': np.float64(14.56), 'std_dev_duration_us': np.float64(0.5479889406767253), 'min_duration_us': np.float64(13.952), 'max_duration_us': np.float64(15.807)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 250, 'total_duration_us': 3701.084, 'mean_duration_us': 14.804336, 'median_duration_us': 14.56, 'std_dev_duration_us': 0.5479889406767253, 'min_duration_us': 13.952, 'max_duration_us': 15.807}]</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': np.float64(14.8)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': 14.8}]</t>
         </is>
       </c>
       <c r="P12" t="n">
@@ -2264,12 +2264,12 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(3687.3240000000005), 'mean_duration_us': np.float64(30.727700000000006), 'median_duration_us': np.float64(30.591), 'std_dev_duration_us': np.float64(0.3214868737600341), 'min_duration_us': np.float64(30.336), 'max_duration_us': np.float64(31.711)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 3687.3240000000005, 'mean_duration_us': 30.727700000000006, 'median_duration_us': 30.591, 'std_dev_duration_us': 0.3214868737600341, 'min_duration_us': 30.336, 'max_duration_us': 31.711}]</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(30.73)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 30.73}]</t>
         </is>
       </c>
       <c r="P13" t="n">
@@ -2331,12 +2331,12 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(2338.761), 'mean_duration_us': np.float64(467.7522), 'median_duration_us': np.float64(464.252), 'std_dev_duration_us': np.float64(11.281809454161158), 'min_duration_us': np.float64(454.556), 'max_duration_us': np.float64(487.899)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 2338.761, 'mean_duration_us': 467.7522, 'median_duration_us': 464.252, 'std_dev_duration_us': 11.281809454161158, 'min_duration_us': 454.556, 'max_duration_us': 487.899}]</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(467.75)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 467.75}]</t>
         </is>
       </c>
       <c r="P14" t="n">
@@ -2398,12 +2398,12 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(2324.394), 'mean_duration_us': np.float64(464.87879999999996), 'median_duration_us': np.float64(472.188), 'std_dev_duration_us': np.float64(19.601893596282974), 'min_duration_us': np.float64(436.444), 'max_duration_us': np.float64(489.34)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 2324.394, 'mean_duration_us': 464.87879999999996, 'median_duration_us': 472.188, 'std_dev_duration_us': 19.601893596282974, 'min_duration_us': 436.444, 'max_duration_us': 489.34}]</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(464.88)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 464.88}]</t>
         </is>
       </c>
       <c r="P15" t="n">
@@ -2465,12 +2465,12 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 245, 'total_duration_us': np.float64(2317.353), 'mean_duration_us': np.float64(9.458583673469388), 'median_duration_us': np.float64(9.472), 'std_dev_duration_us': np.float64(0.3348456698101192), 'min_duration_us': np.float64(8.576), 'max_duration_us': np.float64(10.849)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 245, 'total_duration_us': 2317.353, 'mean_duration_us': 9.458583673469388, 'median_duration_us': 9.472, 'std_dev_duration_us': 0.3348456698101192, 'min_duration_us': 8.576, 'max_duration_us': 10.849}]</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(9.46)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 9.46}]</t>
         </is>
       </c>
       <c r="P16" t="n">
@@ -2532,12 +2532,12 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(1873.8329999999999), 'mean_duration_us': np.float64(15.615274999999999), 'median_duration_us': np.float64(15.584), 'std_dev_duration_us': np.float64(0.1854254999768552), 'min_duration_us': np.float64(15.264), 'max_duration_us': np.float64(16.384)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': 1873.8329999999999, 'mean_duration_us': 15.615274999999999, 'median_duration_us': 15.584, 'std_dev_duration_us': 0.1854254999768552, 'min_duration_us': 15.264, 'max_duration_us': 16.384}]</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(15.62)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 15.62}]</t>
         </is>
       </c>
       <c r="P17" t="n">
@@ -2599,12 +2599,12 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(1627.952), 'mean_duration_us': np.float64(325.5904), 'median_duration_us': np.float64(333.501), 'std_dev_duration_us': np.float64(11.368233417730304), 'min_duration_us': np.float64(304.989), 'max_duration_us': np.float64(334.205)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': 1627.952, 'mean_duration_us': 325.5904, 'median_duration_us': 333.501, 'std_dev_duration_us': 11.368233417730304, 'min_duration_us': 304.989, 'max_duration_us': 334.205}]</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(325.59)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 325.59}]</t>
         </is>
       </c>
       <c r="P18" t="n">
@@ -2666,12 +2666,12 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 240, 'total_duration_us': np.float64(1579.851), 'mean_duration_us': np.float64(6.5827125), 'median_duration_us': np.float64(6.592), 'std_dev_duration_us': np.float64(0.13116311667951205), 'min_duration_us': np.float64(6.303), 'max_duration_us': np.float64(6.975)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 240, 'total_duration_us': 1579.851, 'mean_duration_us': 6.5827125, 'median_duration_us': 6.592, 'std_dev_duration_us': 0.13116311667951205, 'min_duration_us': 6.303, 'max_duration_us': 6.975}]</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': np.float64(6.58)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': 6.58}]</t>
         </is>
       </c>
       <c r="P19" t="n">
@@ -2733,12 +2733,12 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(28.127000000000002), 'mean_duration_us': np.float64(5.625400000000001), 'median_duration_us': np.float64(5.664), 'std_dev_duration_us': np.float64(0.08941498755801505), 'min_duration_us': np.float64(5.503), 'max_duration_us': np.float64(5.728)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(222.207), 'mean_duration_us': np.float64(44.4414), 'median_duration_us': np.float64(44.384), 'std_dev_duration_us': np.float64(0.1792647204555328), 'min_duration_us': np.float64(44.224), 'max_duration_us': np.float64(44.768)}, {'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(10.85), 'mean_duration_us': np.float64(2.17), 'median_duration_us': np.float64(2.176), 'std_dev_duration_us': np.float64(0.013007690033207267), 'min_duration_us': np.float64(2.144), 'max_duration_us': np.float64(2.177)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(58.303000000000004), 'mean_duration_us': np.float64(11.6606), 'median_duration_us': np.float64(11.679), 'std_dev_duration_us': np.float64(0.15088485676170435), 'min_duration_us': np.float64(11.424), 'max_duration_us': np.float64(11.872)}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8&gt;(cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8::Params)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(982.9660000000001), 'mean_duration_us': np.float64(196.59320000000002), 'median_duration_us': np.float64(196.542), 'std_dev_duration_us': np.float64(0.4292092263686784), 'min_duration_us': np.float64(195.966), 'max_duration_us': np.float64(197.245)}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16, __nv_bfloat16, float, true, false, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nhwc2nchw_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(48.35), 'mean_duration_us': np.float64(9.67), 'median_duration_us': np.float64(9.663), 'std_dev_duration_us': np.float64(0.0547539952880155), 'min_duration_us': np.float64(9.6), 'max_duration_us': np.float64(9.759)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': 28.127000000000002, 'mean_duration_us': 5.625400000000001, 'median_duration_us': 5.664, 'std_dev_duration_us': 0.08941498755801505, 'min_duration_us': 5.503, 'max_duration_us': 5.728}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 222.207, 'mean_duration_us': 44.4414, 'median_duration_us': 44.384, 'std_dev_duration_us': 0.1792647204555328, 'min_duration_us': 44.224, 'max_duration_us': 44.768}, {'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': 10.85, 'mean_duration_us': 2.17, 'median_duration_us': 2.176, 'std_dev_duration_us': 0.013007690033207267, 'min_duration_us': 2.144, 'max_duration_us': 2.177}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 58.303000000000004, 'mean_duration_us': 11.6606, 'median_duration_us': 11.679, 'std_dev_duration_us': 0.15088485676170435, 'min_duration_us': 11.424, 'max_duration_us': 11.872}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8&gt;(cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8::Params)', 'stream': 7, 'count': 5, 'total_duration_us': 982.9660000000001, 'mean_duration_us': 196.59320000000002, 'median_duration_us': 196.542, 'std_dev_duration_us': 0.4292092263686784, 'min_duration_us': 195.966, 'max_duration_us': 197.245}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16, __nv_bfloat16, float, true, false, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nhwc2nchw_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 48.35, 'mean_duration_us': 9.67, 'median_duration_us': 9.663, 'std_dev_duration_us': 0.0547539952880155, 'min_duration_us': 9.6, 'max_duration_us': 9.759}]</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(5.63)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': np.float64(44.44)}, {'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(2.17)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': np.float64(11.66)}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop...', 'stream': 7, 'mean_duration_us': np.float64(196.59)}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': np.float64(9.67)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 5.63}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': 44.44}, {'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 2.17}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': 11.66}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop...', 'stream': 7, 'mean_duration_us': 196.59}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': 9.67}]</t>
         </is>
       </c>
       <c r="P20" t="n">
@@ -2800,12 +2800,12 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(934.809), 'mean_duration_us': np.float64(7.790075), 'median_duration_us': np.float64(7.776), 'std_dev_duration_us': np.float64(0.06863528763204346), 'min_duration_us': np.float64(7.711), 'max_duration_us': np.float64(8.032)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 934.809, 'mean_duration_us': 7.790075, 'median_duration_us': 7.776, 'std_dev_duration_us': 0.06863528763204346, 'min_duration_us': 7.711, 'max_duration_us': 8.032}]</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(7.79)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 7.79}]</t>
         </is>
       </c>
       <c r="P21" t="n">
@@ -2867,12 +2867,12 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(385.4959999999999), 'mean_duration_us': np.float64(6.424933333333332), 'median_duration_us': np.float64(6.336), 'std_dev_duration_us': np.float64(0.19279919317489072), 'min_duration_us': np.float64(6.239), 'max_duration_us': np.float64(6.912)}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, __nv_bfloat16, float, __nv_bfloat16, true, true, false&gt;(cublasLt::cublasSplitKParams&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, float const*, float const*, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, void*, long, float*, int*)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(140.35000000000002), 'mean_duration_us': np.float64(2.339166666666667), 'median_duration_us': np.float64(2.336), 'std_dev_duration_us': np.float64(0.037292164801142315), 'min_duration_us': np.float64(2.272), 'max_duration_us': np.float64(2.496)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 385.4959999999999, 'mean_duration_us': 6.424933333333332, 'median_duration_us': 6.336, 'std_dev_duration_us': 0.19279919317489072, 'min_duration_us': 6.239, 'max_duration_us': 6.912}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, __nv_bfloat16, float, __nv_bfloat16, true, true, false&gt;(cublasLt::cublasSplitKParams&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, float const*, float const*, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, void*, long, float*, int*)', 'stream': 7, 'count': 60, 'total_duration_us': 140.35000000000002, 'mean_duration_us': 2.339166666666667, 'median_duration_us': 2.336, 'std_dev_duration_us': 0.037292164801142315, 'min_duration_us': 2.272, 'max_duration_us': 2.496}]</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': np.float64(6.42)}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': np.float64(2.34)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': 6.42}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': 2.34}]</t>
         </is>
       </c>
       <c r="P22" t="n">
@@ -2934,12 +2934,12 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 180, 'total_duration_us': np.float64(457.9199999999999), 'mean_duration_us': np.float64(2.5439999999999996), 'median_duration_us': np.float64(2.4645), 'std_dev_duration_us': np.float64(0.22104903930525865), 'min_duration_us': np.float64(2.24), 'max_duration_us': np.float64(3.232)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 180, 'total_duration_us': 457.9199999999999, 'mean_duration_us': 2.5439999999999996, 'median_duration_us': 2.4645, 'std_dev_duration_us': 0.22104903930525865, 'min_duration_us': 2.24, 'max_duration_us': 3.232}]</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.54)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.54}]</t>
         </is>
       </c>
       <c r="P23" t="n">
@@ -3001,12 +3001,12 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 125, 'total_duration_us': np.float64(451.14099999999996), 'mean_duration_us': np.float64(3.6091279999999997), 'median_duration_us': np.float64(3.584), 'std_dev_duration_us': np.float64(0.16081094370719926), 'min_duration_us': np.float64(3.328), 'max_duration_us': np.float64(4.096)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 125, 'total_duration_us': 451.14099999999996, 'mean_duration_us': 3.6091279999999997, 'median_duration_us': 3.584, 'std_dev_duration_us': 0.16081094370719926, 'min_duration_us': 3.328, 'max_duration_us': 4.096}]</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': np.float64(3.61)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': 3.61}]</t>
         </is>
       </c>
       <c r="P24" t="n">
@@ -3068,12 +3068,12 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 20, 'total_duration_us': np.float64(17.248), 'mean_duration_us': np.float64(0.8624), 'median_duration_us': np.float64(0.8), 'std_dev_duration_us': np.float64(0.13365305832639968), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(1.248)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 20, 'total_duration_us': np.float64(414.7149999999999), 'mean_duration_us': np.float64(20.735749999999996), 'median_duration_us': np.float64(20.768), 'std_dev_duration_us': np.float64(0.42032010123238245), 'min_duration_us': np.float64(19.936), 'max_duration_us': np.float64(21.279)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 20, 'total_duration_us': 17.248, 'mean_duration_us': 0.8624, 'median_duration_us': 0.8, 'std_dev_duration_us': 0.13365305832639968, 'min_duration_us': 0.768, 'max_duration_us': 1.248}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 20, 'total_duration_us': 414.7149999999999, 'mean_duration_us': 20.735749999999996, 'median_duration_us': 20.768, 'std_dev_duration_us': 0.42032010123238245, 'min_duration_us': 19.936, 'max_duration_us': 21.279}]</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.86)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(20.74)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.86}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 20.74}]</t>
         </is>
       </c>
       <c r="P25" t="n">
@@ -3135,12 +3135,12 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(422.845), 'mean_duration_us': np.float64(7.047416666666667), 'median_duration_us': np.float64(6.976), 'std_dev_duration_us': np.float64(0.17790056133194818), 'min_duration_us': np.float64(6.752), 'max_duration_us': np.float64(7.52)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 422.845, 'mean_duration_us': 7.047416666666667, 'median_duration_us': 6.976, 'std_dev_duration_us': 0.17790056133194818, 'min_duration_us': 6.752, 'max_duration_us': 7.52}]</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': np.float64(7.05)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': 7.05}]</t>
         </is>
       </c>
       <c r="P26" t="n">
@@ -3202,12 +3202,12 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(287.13699999999994), 'mean_duration_us': np.float64(2.392808333333333), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.24387456802740948), 'min_duration_us': np.float64(1.984), 'max_duration_us': np.float64(2.913)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': 287.13699999999994, 'mean_duration_us': 2.392808333333333, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.24387456802740948, 'min_duration_us': 1.984, 'max_duration_us': 2.913}]</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.39)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.39}]</t>
         </is>
       </c>
       <c r="P27" t="n">
@@ -3269,12 +3269,12 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::CatArrayBatchedCopy&lt;at::native::(anonymous namespace)::OpaqueType&lt;2u&gt;, unsigned int, 3, 64, 64&gt;(at::native::(anonymous namespace)::OpaqueType&lt;2u&gt;*, at::native::(anonymous namespace)::CatArrInputTensorMetadata&lt;at::native::(anonymous namespace)::OpaqueType&lt;2u&gt;, unsigned int, 64, 64&gt;, at::native::(anonymous namespace)::TensorSizeStride&lt;unsigned int, 4u&gt;, int, unsigned int)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(219.806), 'mean_duration_us': np.float64(43.961200000000005), 'median_duration_us': np.float64(43.712), 'std_dev_duration_us': np.float64(0.48020553932665044), 'min_duration_us': np.float64(43.551), 'max_duration_us': np.float64(44.799)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::CatArrayBatchedCopy&lt;at::native::(anonymous namespace)::OpaqueType&lt;2u&gt;, unsigned int, 3, 64, 64&gt;(at::native::(anonymous namespace)::OpaqueType&lt;2u&gt;*, at::native::(anonymous namespace)::CatArrInputTensorMetadata&lt;at::native::(anonymous namespace)::OpaqueType&lt;2u&gt;, unsigned int, 64, 64&gt;, at::native::(anonymous namespace)::TensorSizeStride&lt;unsigned int, 4u&gt;, int, unsigned int)', 'stream': 7, 'count': 5, 'total_duration_us': 219.806, 'mean_duration_us': 43.961200000000005, 'median_duration_us': 43.712, 'std_dev_duration_us': 0.48020553932665044, 'min_duration_us': 43.551, 'max_duration_us': 44.799}]</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::CatArrayBatchedCopy&lt;at::...', 'stream': 7, 'mean_duration_us': np.float64(43.96)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::CatArrayBatchedCopy&lt;at::...', 'stream': 7, 'mean_duration_us': 43.96}]</t>
         </is>
       </c>
       <c r="P28" t="n">
@@ -3336,12 +3336,12 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectLargeIndex&lt;c10::BFloat16, long, unsigned int, 2, 2, -2, true&gt;(at::cuda::detail::TensorInfo&lt;c10::BFloat16, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;c10::BFloat16 const, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;long const, unsigned int&gt;, int, int, unsigned int, unsigned int, long)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(195.071), 'mean_duration_us': np.float64(39.0142), 'median_duration_us': np.float64(39.072), 'std_dev_duration_us': np.float64(0.2134070289376613), 'min_duration_us': np.float64(38.624), 'max_duration_us': np.float64(39.231)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectLargeIndex&lt;c10::BFloat16, long, unsigned int, 2, 2, -2, true&gt;(at::cuda::detail::TensorInfo&lt;c10::BFloat16, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;c10::BFloat16 const, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;long const, unsigned int&gt;, int, int, unsigned int, unsigned int, long)', 'stream': 7, 'count': 5, 'total_duration_us': 195.071, 'mean_duration_us': 39.0142, 'median_duration_us': 39.072, 'std_dev_duration_us': 0.2134070289376613, 'min_duration_us': 38.624, 'max_duration_us': 39.231}]</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectLargeIndex&lt;c1...', 'stream': 7, 'mean_duration_us': np.float64(39.01)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectLargeIndex&lt;c1...', 'stream': 7, 'mean_duration_us': 39.01}]</t>
         </is>
       </c>
       <c r="P29" t="n">
@@ -3403,12 +3403,12 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 125, 'total_duration_us': np.float64(187.747), 'mean_duration_us': np.float64(1.5019760000000002), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.09206636423797784), 'min_duration_us': np.float64(1.344), 'max_duration_us': np.float64(1.633)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 125, 'total_duration_us': 187.747, 'mean_duration_us': 1.5019760000000002, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.09206636423797784, 'min_duration_us': 1.344, 'max_duration_us': 1.633}]</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.5)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.5}]</t>
         </is>
       </c>
       <c r="P30" t="n">
@@ -3470,12 +3470,12 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(185.69699999999997), 'mean_duration_us': np.float64(3.0949499999999994), 'median_duration_us': np.float64(3.104), 'std_dev_duration_us': np.float64(0.04453478977159322), 'min_duration_us': np.float64(3.008), 'max_duration_us': np.float64(3.168)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 185.69699999999997, 'mean_duration_us': 3.0949499999999994, 'median_duration_us': 3.104, 'std_dev_duration_us': 0.04453478977159322, 'min_duration_us': 3.008, 'max_duration_us': 3.168}]</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': np.float64(3.09)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': 3.09}]</t>
         </is>
       </c>
       <c r="P31" t="n">
@@ -3537,12 +3537,12 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::GeluCUDAKernelImpl(at::TensorIteratorBase&amp;, at::native::GeluType)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::GeluCUDAKernelImpl(at::TensorIteratorBase&amp;, at::native::GeluType)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 20, 'total_duration_us': np.float64(176.76800000000006), 'mean_duration_us': np.float64(8.838400000000004), 'median_duration_us': np.float64(8.832), 'std_dev_duration_us': np.float64(0.06681796165702758), 'min_duration_us': np.float64(8.704), 'max_duration_us': np.float64(8.992)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::GeluCUDAKernelImpl(at::TensorIteratorBase&amp;, at::native::GeluType)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::GeluCUDAKernelImpl(at::TensorIteratorBase&amp;, at::native::GeluType)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 20, 'total_duration_us': 176.76800000000006, 'mean_duration_us': 8.838400000000004, 'median_duration_us': 8.832, 'std_dev_duration_us': 0.06681796165702758, 'min_duration_us': 8.704, 'max_duration_us': 8.992}]</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Ge...', 'stream': 7, 'mean_duration_us': np.float64(8.84)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Ge...', 'stream': 7, 'mean_duration_us': 8.84}]</t>
         </is>
       </c>
       <c r="P32" t="n">
@@ -3604,12 +3604,12 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(167.428), 'mean_duration_us': np.float64(2.7904666666666667), 'median_duration_us': np.float64(2.816), 'std_dev_duration_us': np.float64(0.037250264726874344), 'min_duration_us': np.float64(2.72), 'max_duration_us': np.float64(2.88)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 167.428, 'mean_duration_us': 2.7904666666666667, 'median_duration_us': 2.816, 'std_dev_duration_us': 0.037250264726874344, 'min_duration_us': 2.72, 'max_duration_us': 2.88}]</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': np.float64(2.79)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': 2.79}]</t>
         </is>
       </c>
       <c r="P33" t="n">
@@ -3671,12 +3671,12 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(163.17200000000005), 'mean_duration_us': np.float64(2.719533333333334), 'median_duration_us': np.float64(2.784), 'std_dev_duration_us': np.float64(0.14011381881250043), 'min_duration_us': np.float64(2.527), 'max_duration_us': np.float64(3.008)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 60, 'total_duration_us': 163.17200000000005, 'mean_duration_us': 2.719533333333334, 'median_duration_us': 2.784, 'std_dev_duration_us': 0.14011381881250043, 'min_duration_us': 2.527, 'max_duration_us': 3.008}]</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.72)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.72}]</t>
         </is>
       </c>
       <c r="P34" t="n">
@@ -3738,12 +3738,12 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 15, 'total_duration_us': np.float64(35.168), 'mean_duration_us': np.float64(2.344533333333333), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.10418372660300108), 'min_duration_us': np.float64(2.176), 'max_duration_us': np.float64(2.56)}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 15, 'total_duration_us': np.float64(83.104), 'mean_duration_us': np.float64(5.540266666666667), 'median_duration_us': np.float64(5.376), 'std_dev_duration_us': np.float64(0.32818683025916123), 'min_duration_us': np.float64(5.152), 'max_duration_us': np.float64(6.176)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 15, 'total_duration_us': 35.168, 'mean_duration_us': 2.344533333333333, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.10418372660300108, 'min_duration_us': 2.176, 'max_duration_us': 2.56}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 15, 'total_duration_us': 83.104, 'mean_duration_us': 5.540266666666667, 'median_duration_us': 5.376, 'std_dev_duration_us': 0.32818683025916123, 'min_duration_us': 5.152, 'max_duration_us': 6.176}]</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.34)}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': np.float64(5.54)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.34}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': 5.54}]</t>
         </is>
       </c>
       <c r="P35" t="n">
@@ -3805,12 +3805,12 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>[{'name': 'void (anonymous namespace)::softmax_warp_forward&lt;c10::BFloat16, c10::BFloat16, float, 3, false, false&gt;(c10::BFloat16*, c10::BFloat16 const*, int, int, int, bool const*, int, bool)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(115.74799999999999), 'mean_duration_us': np.float64(1.9291333333333331), 'median_duration_us': np.float64(1.857), 'std_dev_duration_us': np.float64(0.09073284349610612), 'min_duration_us': np.float64(1.824), 'max_duration_us': np.float64(2.049)}]</t>
+          <t>[{'name': 'void (anonymous namespace)::softmax_warp_forward&lt;c10::BFloat16, c10::BFloat16, float, 3, false, false&gt;(c10::BFloat16*, c10::BFloat16 const*, int, int, int, bool const*, int, bool)', 'stream': 7, 'count': 60, 'total_duration_us': 115.74799999999999, 'mean_duration_us': 1.9291333333333331, 'median_duration_us': 1.857, 'std_dev_duration_us': 0.09073284349610612, 'min_duration_us': 1.824, 'max_duration_us': 2.049}]</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>[{'name': 'void (anonymous namespace)::softmax_warp_forward&lt;c10::BFloat16, ...', 'stream': 7, 'mean_duration_us': np.float64(1.93)}]</t>
+          <t>[{'name': 'void (anonymous namespace)::softmax_warp_forward&lt;c10::BFloat16, ...', 'stream': 7, 'mean_duration_us': 1.93}]</t>
         </is>
       </c>
       <c r="P36" t="n">
@@ -3872,12 +3872,12 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(105.02100000000002), 'mean_duration_us': np.float64(1.7503500000000003), 'median_duration_us': np.float64(1.76), 'std_dev_duration_us': np.float64(0.021235838418422137), 'min_duration_us': np.float64(1.696), 'max_duration_us': np.float64(1.792)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 105.02100000000002, 'mean_duration_us': 1.7503500000000003, 'median_duration_us': 1.76, 'std_dev_duration_us': 0.021235838418422137, 'min_duration_us': 1.696, 'max_duration_us': 1.792}]</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': np.float64(1.75)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': 1.75}]</t>
         </is>
       </c>
       <c r="P37" t="n">
@@ -3939,12 +3939,12 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(94.07899999999998), 'mean_duration_us': np.float64(1.567983333333333), 'median_duration_us': np.float64(1.568), 'std_dev_duration_us': np.float64(0.02925092116308288), 'min_duration_us': np.float64(1.535), 'max_duration_us': np.float64(1.633)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 94.07899999999998, 'mean_duration_us': 1.567983333333333, 'median_duration_us': 1.568, 'std_dev_duration_us': 0.02925092116308288, 'min_duration_us': 1.535, 'max_duration_us': 1.633}]</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(1.57)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 1.57}]</t>
         </is>
       </c>
       <c r="P38" t="n">
@@ -4006,12 +4006,12 @@
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(89.14699999999999), 'mean_duration_us': np.float64(1.4857833333333332), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.016880058912482752), 'min_duration_us': np.float64(1.471), 'max_duration_us': np.float64(1.535)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 89.14699999999999, 'mean_duration_us': 1.4857833333333332, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.016880058912482752, 'min_duration_us': 1.471, 'max_duration_us': 1.535}]</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(1.49)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 1.49}]</t>
         </is>
       </c>
       <c r="P39" t="n">
@@ -4073,12 +4073,12 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warpgroupsize2x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(86.78200000000001), 'mean_duration_us': np.float64(17.3564), 'median_duration_us': np.float64(17.376), 'std_dev_duration_us': np.float64(0.07209049868047837), 'min_duration_us': np.float64(17.215), 'max_duration_us': np.float64(17.408)}]</t>
+          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warpgroupsize2x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 5, 'total_duration_us': 86.78200000000001, 'mean_duration_us': 17.3564, 'median_duration_us': 17.376, 'std_dev_duration_us': 0.07209049868047837, 'min_duration_us': 17.215, 'max_duration_us': 17.408}]</t>
         </is>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(17.36)}]</t>
+          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warp...', 'stream': 7, 'mean_duration_us': 17.36}]</t>
         </is>
       </c>
       <c r="P40" t="n">
@@ -4140,12 +4140,12 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(86.49500000000002), 'mean_duration_us': np.float64(1.4415833333333337), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.10003121040733015), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.568)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 86.49500000000002, 'mean_duration_us': 1.4415833333333337, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.10003121040733015, 'min_duration_us': 1.28, 'max_duration_us': 1.568}]</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(1.44)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 1.44}]</t>
         </is>
       </c>
       <c r="P41" t="n">
@@ -4207,12 +4207,12 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(70.463), 'mean_duration_us': np.float64(14.0926), 'median_duration_us': np.float64(14.079), 'std_dev_duration_us': np.float64(0.1321144957981524), 'min_duration_us': np.float64(13.92), 'max_duration_us': np.float64(14.272)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 70.463, 'mean_duration_us': 14.0926, 'median_duration_us': 14.079, 'std_dev_duration_us': 0.1321144957981524, 'min_duration_us': 13.92, 'max_duration_us': 14.272}]</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': np.float64(14.09)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': 14.09}]</t>
         </is>
       </c>
       <c r="P42" t="n">
@@ -4274,12 +4274,12 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(65.407), 'mean_duration_us': np.float64(13.081399999999999), 'median_duration_us': np.float64(13.088), 'std_dev_duration_us': np.float64(0.058854396607220374), 'min_duration_us': np.float64(13.023), 'max_duration_us': np.float64(13.184)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 65.407, 'mean_duration_us': 13.081399999999999, 'median_duration_us': 13.088, 'std_dev_duration_us': 0.058854396607220374, 'min_duration_us': 13.023, 'max_duration_us': 13.184}]</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(13.08)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 13.08}]</t>
         </is>
       </c>
       <c r="P43" t="n">
@@ -4341,12 +4341,12 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(57.631), 'mean_duration_us': np.float64(11.5262), 'median_duration_us': np.float64(11.552), 'std_dev_duration_us': np.float64(0.0889413289759043), 'min_duration_us': np.float64(11.392), 'max_duration_us': np.float64(11.616)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 57.631, 'mean_duration_us': 11.5262, 'median_duration_us': 11.552, 'std_dev_duration_us': 0.0889413289759043, 'min_duration_us': 11.392, 'max_duration_us': 11.616}]</t>
         </is>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(11.53)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 11.53}]</t>
         </is>
       </c>
       <c r="P44" t="n">
@@ -4408,12 +4408,12 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2&gt;(cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2::Params)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(56.54299999999999), 'mean_duration_us': np.float64(11.308599999999998), 'median_duration_us': np.float64(11.296), 'std_dev_duration_us': np.float64(0.10403768547983014), 'min_duration_us': np.float64(11.168), 'max_duration_us': np.float64(11.487)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2&gt;(cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2::Params)', 'stream': 7, 'count': 5, 'total_duration_us': 56.54299999999999, 'mean_duration_us': 11.308599999999998, 'median_duration_us': 11.296, 'std_dev_duration_us': 0.10403768547983014, 'min_duration_us': 11.168, 'max_duration_us': 11.487}]</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': np.float64(11.31)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': 11.31}]</t>
         </is>
       </c>
       <c r="P45" t="n">
@@ -4475,12 +4475,12 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt; &gt;(at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt;)', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(31.743), 'mean_duration_us': np.float64(3.1742999999999997), 'median_duration_us': np.float64(3.216), 'std_dev_duration_us': np.float64(0.22374005005809758), 'min_duration_us': np.float64(2.848), 'max_duration_us': np.float64(3.551)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt; &gt;(at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt;)', 'stream': 7, 'count': 10, 'total_duration_us': 31.743, 'mean_duration_us': 3.1742999999999997, 'median_duration_us': 3.216, 'std_dev_duration_us': 0.22374005005809758, 'min_duration_us': 2.848, 'max_duration_us': 3.551}]</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10:...', 'stream': 7, 'mean_duration_us': np.float64(3.17)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10:...', 'stream': 7, 'mean_duration_us': 3.17}]</t>
         </is>
       </c>
       <c r="P46" t="n">
@@ -4542,12 +4542,12 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c10::BFloat16, long, unsigned int, 2, 2, -2&gt;(at::cuda::detail::TensorInfo&lt;c10::BFloat16, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;c10::BFloat16 const, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;long const, unsigned int&gt;, int, int, unsigned int, long)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(28.159999999999997), 'mean_duration_us': np.float64(5.632), 'median_duration_us': np.float64(5.792), 'std_dev_duration_us': np.float64(0.2638787600395301), 'min_duration_us': np.float64(5.28), 'max_duration_us': np.float64(5.888)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c10::BFloat16, long, unsigned int, 2, 2, -2&gt;(at::cuda::detail::TensorInfo&lt;c10::BFloat16, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;c10::BFloat16 const, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;long const, unsigned int&gt;, int, int, unsigned int, long)', 'stream': 7, 'count': 5, 'total_duration_us': 28.159999999999997, 'mean_duration_us': 5.632, 'median_duration_us': 5.792, 'std_dev_duration_us': 0.2638787600395301, 'min_duration_us': 5.28, 'max_duration_us': 5.888}]</t>
         </is>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c1...', 'stream': 7, 'mean_duration_us': np.float64(5.63)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c1...', 'stream': 7, 'mean_duration_us': 5.63}]</t>
         </is>
       </c>
       <c r="P47" t="n">
@@ -4609,12 +4609,12 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(26.686999999999998), 'mean_duration_us': np.float64(2.6687), 'median_duration_us': np.float64(2.656), 'std_dev_duration_us': np.float64(0.20862696374150683), 'min_duration_us': np.float64(2.335), 'max_duration_us': np.float64(3.008)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 10, 'total_duration_us': 26.686999999999998, 'mean_duration_us': 2.6687, 'median_duration_us': 2.656, 'std_dev_duration_us': 0.20862696374150683, 'min_duration_us': 2.335, 'max_duration_us': 3.008}]</t>
         </is>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.67)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.67}]</t>
         </is>
       </c>
       <c r="P48" t="n">
@@ -4676,12 +4676,12 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c10::BFloat16, long, unsigned int, 2, 2, -2&gt;(at::cuda::detail::TensorInfo&lt;c10::BFloat16, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;c10::BFloat16 const, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;long const, unsigned int&gt;, int, int, unsigned int, long)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(26.463), 'mean_duration_us': np.float64(5.2926), 'median_duration_us': np.float64(5.216), 'std_dev_duration_us': np.float64(0.19653355947522047), 'min_duration_us': np.float64(5.088), 'max_duration_us': np.float64(5.599)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c10::BFloat16, long, unsigned int, 2, 2, -2&gt;(at::cuda::detail::TensorInfo&lt;c10::BFloat16, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;c10::BFloat16 const, unsigned int&gt;, at::cuda::detail::TensorInfo&lt;long const, unsigned int&gt;, int, int, unsigned int, long)', 'stream': 7, 'count': 5, 'total_duration_us': 26.463, 'mean_duration_us': 5.2926, 'median_duration_us': 5.216, 'std_dev_duration_us': 0.19653355947522047, 'min_duration_us': 5.088, 'max_duration_us': 5.599}]</t>
         </is>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c1...', 'stream': 7, 'mean_duration_us': np.float64(5.29)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::indexSelectSmallIndex&lt;c1...', 'stream': 7, 'mean_duration_us': 5.29}]</t>
         </is>
       </c>
       <c r="P49" t="n">
@@ -4743,12 +4743,12 @@
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt; &gt;(at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(24.704), 'mean_duration_us': np.float64(4.9408), 'median_duration_us': np.float64(4.96), 'std_dev_duration_us': np.float64(0.05935115837117255), 'min_duration_us': np.float64(4.832), 'max_duration_us': np.float64(4.992)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt; &gt;(at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 24.704, 'mean_duration_us': 4.9408, 'median_duration_us': 4.96, 'std_dev_duration_us': 0.05935115837117255, 'min_duration_us': 4.832, 'max_duration_us': 4.992}]</t>
         </is>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10:...', 'stream': 7, 'mean_duration_us': np.float64(4.94)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10:...', 'stream': 7, 'mean_duration_us': 4.94}]</t>
         </is>
       </c>
       <c r="P50" t="n">
@@ -4810,12 +4810,12 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(23.615000000000002), 'mean_duration_us': np.float64(4.723000000000001), 'median_duration_us': np.float64(4.704), 'std_dev_duration_us': np.float64(0.06861486719363401), 'min_duration_us': np.float64(4.64), 'max_duration_us': np.float64(4.831)}]</t>
+          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 5, 'total_duration_us': 23.615000000000002, 'mean_duration_us': 4.723000000000001, 'median_duration_us': 4.704, 'std_dev_duration_us': 0.06861486719363401, 'min_duration_us': 4.64, 'max_duration_us': 4.831}]</t>
         </is>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': np.float64(4.72)}]</t>
+          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': 4.72}]</t>
         </is>
       </c>
       <c r="P51" t="n">
@@ -4877,12 +4877,12 @@
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt; &gt;(cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(10.143), 'mean_duration_us': np.float64(2.0286), 'median_duration_us': np.float64(2.047), 'std_dev_duration_us': np.float64(0.02545270123189289), 'min_duration_us': np.float64(1.984), 'max_duration_us': np.float64(2.048)}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStridedBatched&lt;float&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt; &gt;(float const*, float, cublasGemvTensorStridedBatched&lt;float&gt;, int, float const*, float, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, cublasPointerMode_t, cublasLtEpilogue_t, cublasGemvTensorStridedBatched&lt;biasType&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;::value_type, float&gt;::type const&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.183000000000002), 'mean_duration_us': np.float64(2.6366000000000005), 'median_duration_us': np.float64(2.688), 'std_dev_duration_us': np.float64(0.08984341934721768), 'min_duration_us': np.float64(2.527), 'max_duration_us': np.float64(2.72)}]</t>
+          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt; &gt;(cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 10.143, 'mean_duration_us': 2.0286, 'median_duration_us': 2.047, 'std_dev_duration_us': 0.02545270123189289, 'min_duration_us': 1.984, 'max_duration_us': 2.048}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStridedBatched&lt;float&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt; &gt;(float const*, float, cublasGemvTensorStridedBatched&lt;float&gt;, int, float const*, float, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, cublasPointerMode_t, cublasLtEpilogue_t, cublasGemvTensorStridedBatched&lt;biasType&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;::value_type, float&gt;::type const&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 13.183000000000002, 'mean_duration_us': 2.6366000000000005, 'median_duration_us': 2.688, 'std_dev_duration_us': 0.08984341934721768, 'min_duration_us': 2.527, 'max_duration_us': 2.72}]</t>
         </is>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorS...', 'stream': 7, 'mean_duration_us': np.float64(2.03)}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStrided...', 'stream': 7, 'mean_duration_us': np.float64(2.64)}]</t>
+          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorS...', 'stream': 7, 'mean_duration_us': 2.03}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStrided...', 'stream': 7, 'mean_duration_us': 2.64}]</t>
         </is>
       </c>
       <c r="P52" t="n">
@@ -4944,12 +4944,12 @@
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::index_elementwise_kernel&lt;128, 4, at::native::gpu_index_kernel&lt;at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1}&gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;, at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1} const&amp;)::{lambda(int)#1}&gt;(long, at::native::gpu_index_kernel&lt;at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1}&gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;, at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(22.176000000000002), 'mean_duration_us': np.float64(4.4352), 'median_duration_us': np.float64(4.256), 'std_dev_duration_us': np.float64(0.26400560600108475), 'min_duration_us': np.float64(4.192), 'max_duration_us': np.float64(4.832)}]</t>
+          <t>[{'name': 'void at::native::index_elementwise_kernel&lt;128, 4, at::native::gpu_index_kernel&lt;at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1}&gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;, at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1} const&amp;)::{lambda(int)#1}&gt;(long, at::native::gpu_index_kernel&lt;at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1}&gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;, at::native::index_kernel_impl&lt;at::native::OpaqueType&lt;2&gt; &gt;(at::TensorIteratorBase&amp;, c10::ArrayRef&lt;long&gt;, c10::ArrayRef&lt;long&gt;)::{lambda(char*, char const*, long)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 22.176000000000002, 'mean_duration_us': 4.4352, 'median_duration_us': 4.256, 'std_dev_duration_us': 0.26400560600108475, 'min_duration_us': 4.192, 'max_duration_us': 4.832}]</t>
         </is>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::index_elementwise_kernel&lt;128, 4, at::native::gp...', 'stream': 7, 'mean_duration_us': np.float64(4.44)}]</t>
+          <t>[{'name': 'void at::native::index_elementwise_kernel&lt;128, 4, at::native::gp...', 'stream': 7, 'mean_duration_us': 4.44}]</t>
         </is>
       </c>
       <c r="P53" t="n">
@@ -5011,12 +5011,12 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, 4, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(22.144000000000002), 'mean_duration_us': np.float64(4.428800000000001), 'median_duration_us': np.float64(4.416), 'std_dev_duration_us': np.float64(0.09621309682158638), 'min_duration_us': np.float64(4.32), 'max_duration_us': np.float64(4.608)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, 4, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 22.144000000000002, 'mean_duration_us': 4.428800000000001, 'median_duration_us': 4.416, 'std_dev_duration_us': 0.09621309682158638, 'min_duration_us': 4.32, 'max_duration_us': 4.608}]</t>
         </is>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFun...', 'stream': 7, 'mean_duration_us': np.float64(4.43)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFun...', 'stream': 7, 'mean_duration_us': 4.43}]</t>
         </is>
       </c>
       <c r="P54" t="n">
@@ -5078,12 +5078,12 @@
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(20.255), 'mean_duration_us': np.float64(4.051), 'median_duration_us': np.float64(4.032), 'std_dev_duration_us': np.float64(0.02550294100687212), 'min_duration_us': np.float64(4.032), 'max_duration_us': np.float64(4.096)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': 20.255, 'mean_duration_us': 4.051, 'median_duration_us': 4.032, 'std_dev_duration_us': 0.02550294100687212, 'min_duration_us': 4.032, 'max_duration_us': 4.096}]</t>
         </is>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(4.05)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 4.05}]</t>
         </is>
       </c>
       <c r="P55" t="n">
@@ -5145,12 +5145,12 @@
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(20.128), 'mean_duration_us': np.float64(4.0256), 'median_duration_us': np.float64(4.0), 'std_dev_duration_us': np.float64(0.13636656481704024), 'min_duration_us': np.float64(3.808), 'max_duration_us': np.float64(4.224)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_kernel&lt;c10::BFloat16, float&gt;(int, float, c10::BFloat16 const*, c10::BFloat16 const*, c10::BFloat16 const*, float*, float*, c10::BFloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 20.128, 'mean_duration_us': 4.0256, 'median_duration_us': 4.0, 'std_dev_duration_us': 0.13636656481704024, 'min_duration_us': 3.808, 'max_duration_us': 4.224}]</t>
         </is>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': np.float64(4.03)}]</t>
+          <t>[{'name': 'void at::native::(anonymous namespace)::vectorized_layer_norm_ke...', 'stream': 7, 'mean_duration_us': 4.03}]</t>
         </is>
       </c>
       <c r="P56" t="n">
@@ -5212,12 +5212,12 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(18.784), 'mean_duration_us': np.float64(3.7567999999999997), 'median_duration_us': np.float64(3.744), 'std_dev_duration_us': np.float64(0.03263372488699366), 'min_duration_us': np.float64(3.712), 'max_duration_us': np.float64(3.808)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 18.784, 'mean_duration_us': 3.7567999999999997, 'median_duration_us': 3.744, 'std_dev_duration_us': 0.03263372488699366, 'min_duration_us': 3.712, 'max_duration_us': 3.808}]</t>
         </is>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': np.float64(3.76)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': 3.76}]</t>
         </is>
       </c>
       <c r="P57" t="n">
@@ -5279,12 +5279,12 @@
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;int, at::native::ArgMaxOps&lt;int&gt;, unsigned int, long, 4&gt; &gt;(at::native::ReduceOp&lt;int, at::native::ArgMaxOps&lt;int&gt;, unsigned int, long, 4&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(18.527), 'mean_duration_us': np.float64(3.7054), 'median_duration_us': np.float64(3.712), 'std_dev_duration_us': np.float64(0.13307982566865645), 'min_duration_us': np.float64(3.488), 'max_duration_us': np.float64(3.871)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;int, at::native::ArgMaxOps&lt;int&gt;, unsigned int, long, 4&gt; &gt;(at::native::ReduceOp&lt;int, at::native::ArgMaxOps&lt;int&gt;, unsigned int, long, 4&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 18.527, 'mean_duration_us': 3.7054, 'median_duration_us': 3.712, 'std_dev_duration_us': 0.13307982566865645, 'min_duration_us': 3.488, 'max_duration_us': 3.871}]</t>
         </is>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;int,...', 'stream': 7, 'mean_duration_us': np.float64(3.71)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;int,...', 'stream': 7, 'mean_duration_us': 3.71}]</t>
         </is>
       </c>
       <c r="P58" t="n">
@@ -5346,12 +5346,12 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(17.918), 'mean_duration_us': np.float64(3.5835999999999997), 'median_duration_us': np.float64(3.552), 'std_dev_duration_us': np.float64(0.049834124854360604), 'min_duration_us': np.float64(3.551), 'max_duration_us': np.float64(3.68)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 17.918, 'mean_duration_us': 3.5835999999999997, 'median_duration_us': 3.552, 'std_dev_duration_us': 0.049834124854360604, 'min_duration_us': 3.551, 'max_duration_us': 3.68}]</t>
         </is>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': np.float64(3.58)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': 3.58}]</t>
         </is>
       </c>
       <c r="P59" t="n">
@@ -5413,12 +5413,12 @@
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(17.44), 'mean_duration_us': np.float64(1.7440000000000002), 'median_duration_us': np.float64(1.7440000000000002), 'std_dev_duration_us': np.float64(0.9569284194755635), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(2.72)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': 17.44, 'mean_duration_us': 1.7440000000000002, 'median_duration_us': 1.7440000000000002, 'std_dev_duration_us': 0.9569284194755635, 'min_duration_us': 0.768, 'max_duration_us': 2.72}]</t>
         </is>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(1.74)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 1.74}]</t>
         </is>
       </c>
       <c r="P60" t="n">
@@ -5480,12 +5480,12 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt; &gt;(at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(15.936), 'mean_duration_us': np.float64(3.1872), 'median_duration_us': np.float64(3.104), 'std_dev_duration_us': np.float64(0.2268165778773677), 'min_duration_us': np.float64(2.944), 'max_duration_us': np.float64(3.488)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt; &gt;(at::native::ReduceOp&lt;c10::BFloat16, at::native::NormTwoOps&lt;c10::BFloat16, float, c10::BFloat16&gt;, unsigned int, c10::BFloat16, 4&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 15.936, 'mean_duration_us': 3.1872, 'median_duration_us': 3.104, 'std_dev_duration_us': 0.2268165778773677, 'min_duration_us': 2.944, 'max_duration_us': 3.488}]</t>
         </is>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10:...', 'stream': 7, 'mean_duration_us': np.float64(3.19)}]</t>
+          <t>[{'name': 'void at::native::reduce_kernel&lt;512, 1, at::native::ReduceOp&lt;c10:...', 'stream': 7, 'mean_duration_us': 3.19}]</t>
         </is>
       </c>
       <c r="P61" t="n">
@@ -5547,12 +5547,12 @@
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.717999999999998), 'mean_duration_us': np.float64(2.9435999999999996), 'median_duration_us': np.float64(2.944), 'std_dev_duration_us': np.float64(0.0004898979485565817), 'min_duration_us': np.float64(2.943), 'max_duration_us': np.float64(2.944)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 14.717999999999998, 'mean_duration_us': 2.9435999999999996, 'median_duration_us': 2.944, 'std_dev_duration_us': 0.0004898979485565817, 'min_duration_us': 2.943, 'max_duration_us': 2.944}]</t>
         </is>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.94)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.94}]</t>
         </is>
       </c>
       <c r="P62" t="n">
@@ -5614,12 +5614,12 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.657), 'mean_duration_us': np.float64(2.9314), 'median_duration_us': np.float64(2.944), 'std_dev_duration_us': np.float64(0.03232089107682529), 'min_duration_us': np.float64(2.881), 'max_duration_us': np.float64(2.976)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::where_kernel_impl(at::TensorIterator&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(bool, c10::BFloat16, c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 14.657, 'mean_duration_us': 2.9314, 'median_duration_us': 2.944, 'std_dev_duration_us': 0.03232089107682529, 'min_duration_us': 2.881, 'max_duration_us': 2.976}]</t>
         </is>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.93)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.93}]</t>
         </is>
       </c>
       <c r="P63" t="n">
@@ -5681,12 +5681,12 @@
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.560000000000002), 'mean_duration_us': np.float64(2.9120000000000004), 'median_duration_us': np.float64(3.008), 'std_dev_duration_us': np.float64(0.21891368161903446), 'min_duration_us': np.float64(2.656), 'max_duration_us': np.float64(3.2)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 14.560000000000002, 'mean_duration_us': 2.9120000000000004, 'median_duration_us': 3.008, 'std_dev_duration_us': 0.21891368161903446, 'min_duration_us': 2.656, 'max_duration_us': 3.2}]</t>
         </is>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.91)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.91}]</t>
         </is>
       </c>
       <c r="P64" t="n">
@@ -5748,12 +5748,12 @@
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.495999999999999), 'mean_duration_us': np.float64(2.8991999999999996), 'median_duration_us': np.float64(2.912), 'std_dev_duration_us': np.float64(0.032633724886993856), 'min_duration_us': np.float64(2.848), 'max_duration_us': np.float64(2.944)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 14.495999999999999, 'mean_duration_us': 2.8991999999999996, 'median_duration_us': 2.912, 'std_dev_duration_us': 0.032633724886993856, 'min_duration_us': 2.848, 'max_duration_us': 2.944}]</t>
         </is>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.9)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.9}]</t>
         </is>
       </c>
       <c r="P65" t="n">
@@ -5815,12 +5815,12 @@
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.985), 'mean_duration_us': np.float64(2.7969999999999997), 'median_duration_us': np.float64(2.785), 'std_dev_duration_us': np.float64(0.015517731793016621), 'min_duration_us': np.float64(2.784), 'max_duration_us': np.float64(2.816)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 13.985, 'mean_duration_us': 2.7969999999999997, 'median_duration_us': 2.785, 'std_dev_duration_us': 0.015517731793016621, 'min_duration_us': 2.784, 'max_duration_us': 2.816}]</t>
         </is>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': np.float64(2.8)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': 2.8}]</t>
         </is>
       </c>
       <c r="P66" t="n">
@@ -5882,12 +5882,12 @@
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.472000000000001), 'mean_duration_us': np.float64(2.6944000000000004), 'median_duration_us': np.float64(2.752), 'std_dev_duration_us': np.float64(0.10398769157934018), 'min_duration_us': np.float64(2.528), 'max_duration_us': np.float64(2.816)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 13.472000000000001, 'mean_duration_us': 2.6944000000000004, 'median_duration_us': 2.752, 'std_dev_duration_us': 0.10398769157934018, 'min_duration_us': 2.528, 'max_duration_us': 2.816}]</t>
         </is>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.69)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.69}]</t>
         </is>
       </c>
       <c r="P67" t="n">
@@ -5949,12 +5949,12 @@
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.407000000000002), 'mean_duration_us': np.float64(2.6814000000000004), 'median_duration_us': np.float64(2.656), 'std_dev_duration_us': np.float64(0.07142996570067763), 'min_duration_us': np.float64(2.623), 'max_duration_us': np.float64(2.816)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 13.407000000000002, 'mean_duration_us': 2.6814000000000004, 'median_duration_us': 2.656, 'std_dev_duration_us': 0.07142996570067763, 'min_duration_us': 2.623, 'max_duration_us': 2.816}]</t>
         </is>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.68)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.68}]</t>
         </is>
       </c>
       <c r="P68" t="n">
@@ -6016,12 +6016,12 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.345), 'mean_duration_us': np.float64(2.669), 'median_duration_us': np.float64(2.72), 'std_dev_duration_us': np.float64(0.08978641322605552), 'min_duration_us': np.float64(2.56), 'max_duration_us': np.float64(2.753)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 13.345, 'mean_duration_us': 2.669, 'median_duration_us': 2.72, 'std_dev_duration_us': 0.08978641322605552, 'min_duration_us': 2.56, 'max_duration_us': 2.753}]</t>
         </is>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.67)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.67}]</t>
         </is>
       </c>
       <c r="P69" t="n">
@@ -6083,12 +6083,12 @@
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(12.222999999999999), 'mean_duration_us': np.float64(2.4446), 'median_duration_us': np.float64(2.336), 'std_dev_duration_us': np.float64(0.1469742834648294), 'min_duration_us': np.float64(2.303), 'max_duration_us': np.float64(2.624)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 12.222999999999999, 'mean_duration_us': 2.4446, 'median_duration_us': 2.336, 'std_dev_duration_us': 0.1469742834648294, 'min_duration_us': 2.303, 'max_duration_us': 2.624}]</t>
         </is>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.44)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.44}]</t>
         </is>
       </c>
       <c r="P70" t="n">
@@ -6150,12 +6150,12 @@
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(11.904), 'mean_duration_us': np.float64(2.3808), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.04340691189200176), 'min_duration_us': np.float64(2.336), 'max_duration_us': np.float64(2.464)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 11.904, 'mean_duration_us': 2.3808, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.04340691189200176, 'min_duration_us': 2.336, 'max_duration_us': 2.464}]</t>
         </is>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.38)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.38}]</t>
         </is>
       </c>
       <c r="P71" t="n">
@@ -6217,12 +6217,12 @@
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(11.904), 'mean_duration_us': np.float64(2.3808), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.0478932145507065), 'min_duration_us': np.float64(2.336), 'max_duration_us': np.float64(2.464)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 11.904, 'mean_duration_us': 2.3808, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.0478932145507065, 'min_duration_us': 2.336, 'max_duration_us': 2.464}]</t>
         </is>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.38)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.38}]</t>
         </is>
       </c>
       <c r="P72" t="n">
@@ -6284,12 +6284,12 @@
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; &gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; &gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(10.687), 'mean_duration_us': np.float64(2.1374), 'median_duration_us': np.float64(2.208), 'std_dev_duration_us': np.float64(0.14060953026022097), 'min_duration_us': np.float64(1.952), 'max_duration_us': np.float64(2.272)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; &gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; &gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::CompareFunctor&lt;long&gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 10.687, 'mean_duration_us': 2.1374, 'median_duration_us': 2.208, 'std_dev_duration_us': 0.14060953026022097, 'min_duration_us': 1.952, 'max_duration_us': 2.272}]</t>
         </is>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.14)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.14}]</t>
         </is>
       </c>
       <c r="P73" t="n">
@@ -6351,12 +6351,12 @@
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::AUnaryFunctor&lt;long, long, bool, at::native::(anonymous namespace)::CompareEqFunctor&lt;long&gt; &gt;, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::AUnaryFunctor&lt;long, long, bool, at::native::(anonymous namespace)::CompareEqFunctor&lt;long&gt; &gt;, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(10.048), 'mean_duration_us': np.float64(2.0096), 'median_duration_us': np.float64(2.016), 'std_dev_duration_us': np.float64(0.08442179813294667), 'min_duration_us': np.float64(1.856), 'max_duration_us': np.float64(2.112)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::AUnaryFunctor&lt;long, long, bool, at::native::(anonymous namespace)::CompareEqFunctor&lt;long&gt; &gt;, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::AUnaryFunctor&lt;long, long, bool, at::native::(anonymous namespace)::CompareEqFunctor&lt;long&gt; &gt;, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 10.048, 'mean_duration_us': 2.0096, 'median_duration_us': 2.016, 'std_dev_duration_us': 0.08442179813294667, 'min_duration_us': 1.856, 'max_duration_us': 2.112}]</t>
         </is>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::AUnaryF...', 'stream': 7, 'mean_duration_us': np.float64(2.01)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::AUnaryF...', 'stream': 7, 'mean_duration_us': 2.01}]</t>
         </is>
       </c>
       <c r="P74" t="n">
@@ -6418,12 +6418,12 @@
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::compare_scalar_kernel&lt;long&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::OpType, long)::{lambda(long)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::compare_scalar_kernel&lt;long&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::OpType, long)::{lambda(long)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(9.247), 'mean_duration_us': np.float64(1.8494), 'median_duration_us': np.float64(1.888), 'std_dev_duration_us': np.float64(0.12672426760490674), 'min_duration_us': np.float64(1.696), 'max_duration_us': np.float64(2.047)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::compare_scalar_kernel&lt;long&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::OpType, long)::{lambda(long)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::compare_scalar_kernel&lt;long&gt;(at::TensorIteratorBase&amp;, at::native::(anonymous namespace)::OpType, long)::{lambda(long)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 9.247, 'mean_duration_us': 1.8494, 'median_duration_us': 1.888, 'std_dev_duration_us': 0.12672426760490674, 'min_duration_us': 1.696, 'max_duration_us': 2.047}]</t>
         </is>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::co...', 'stream': 7, 'mean_duration_us': np.float64(1.85)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::co...', 'stream': 7, 'mean_duration_us': 1.85}]</t>
         </is>
       </c>
       <c r="P75" t="n">
@@ -6485,12 +6485,12 @@
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.896), 'mean_duration_us': np.float64(1.7792000000000001), 'median_duration_us': np.float64(1.792), 'std_dev_duration_us': np.float64(0.025600000000000022), 'min_duration_us': np.float64(1.728), 'max_duration_us': np.float64(1.792)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.896, 'mean_duration_us': 1.7792000000000001, 'median_duration_us': 1.792, 'std_dev_duration_us': 0.025600000000000022, 'min_duration_us': 1.728, 'max_duration_us': 1.792}]</t>
         </is>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': np.float64(1.78)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': 1.78}]</t>
         </is>
       </c>
       <c r="P76" t="n">
@@ -6552,12 +6552,12 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.799), 'mean_duration_us': np.float64(1.7597999999999998), 'median_duration_us': np.float64(1.76), 'std_dev_duration_us': np.float64(0.10100376230616363), 'min_duration_us': np.float64(1.632), 'max_duration_us': np.float64(1.888)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.799, 'mean_duration_us': 1.7597999999999998, 'median_duration_us': 1.76, 'std_dev_duration_us': 0.10100376230616363, 'min_duration_us': 1.632, 'max_duration_us': 1.888}]</t>
         </is>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.76)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.76}]</t>
         </is>
       </c>
       <c r="P77" t="n">
@@ -6619,12 +6619,12 @@
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.769), 'mean_duration_us': np.float64(1.7538), 'median_duration_us': np.float64(1.792), 'std_dev_duration_us': np.float64(0.0742762411542211), 'min_duration_us': np.float64(1.664), 'max_duration_us': np.float64(1.825)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.769, 'mean_duration_us': 1.7538, 'median_duration_us': 1.792, 'std_dev_duration_us': 0.0742762411542211, 'min_duration_us': 1.664, 'max_duration_us': 1.825}]</t>
         </is>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': np.float64(1.75)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': 1.75}]</t>
         </is>
       </c>
       <c r="P78" t="n">
@@ -6686,12 +6686,12 @@
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.64), 'mean_duration_us': np.float64(1.7280000000000002), 'median_duration_us': np.float64(1.696), 'std_dev_duration_us': np.float64(0.10516273104099186), 'min_duration_us': np.float64(1.6), 'max_duration_us': np.float64(1.92)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.64, 'mean_duration_us': 1.7280000000000002, 'median_duration_us': 1.696, 'std_dev_duration_us': 0.10516273104099186, 'min_duration_us': 1.6, 'max_duration_us': 1.92}]</t>
         </is>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': np.float64(1.73)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': 1.73}]</t>
         </is>
       </c>
       <c r="P79" t="n">
@@ -6753,12 +6753,12 @@
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(anonymous namespace)::elu_kernel(at::TensorIteratorBase&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::(anonymous namespace)::elu_kernel(at::TensorIteratorBase&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.479), 'mean_duration_us': np.float64(1.6957999999999998), 'median_duration_us': np.float64(1.696), 'std_dev_duration_us': np.float64(0.020556264252047336), 'min_duration_us': np.float64(1.663), 'max_duration_us': np.float64(1.728)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(anonymous namespace)::elu_kernel(at::TensorIteratorBase&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::(anonymous namespace)::elu_kernel(at::TensorIteratorBase&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.479, 'mean_duration_us': 1.6957999999999998, 'median_duration_us': 1.696, 'std_dev_duration_us': 0.020556264252047336, 'min_duration_us': 1.663, 'max_duration_us': 1.728}]</t>
         </is>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(a...', 'stream': 7, 'mean_duration_us': np.float64(1.7)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(a...', 'stream': 7, 'mean_duration_us': 1.7}]</t>
         </is>
       </c>
       <c r="P80" t="n">
@@ -6820,12 +6820,12 @@
       </c>
       <c r="N81" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::exp_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::exp_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.447), 'mean_duration_us': np.float64(1.6893999999999998), 'median_duration_us': np.float64(1.632), 'std_dev_duration_us': np.float64(0.09808486121721335), 'min_duration_us': np.float64(1.599), 'max_duration_us': np.float64(1.824)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::exp_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::exp_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.447, 'mean_duration_us': 1.6893999999999998, 'median_duration_us': 1.632, 'std_dev_duration_us': 0.09808486121721335, 'min_duration_us': 1.599, 'max_duration_us': 1.824}]</t>
         </is>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::ex...', 'stream': 7, 'mean_duration_us': np.float64(1.69)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::ex...', 'stream': 7, 'mean_duration_us': 1.69}]</t>
         </is>
       </c>
       <c r="P81" t="n">
@@ -6887,12 +6887,12 @@
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.030999999999999), 'mean_duration_us': np.float64(1.6061999999999999), 'median_duration_us': np.float64(1.632), 'std_dev_duration_us': np.float64(0.046786322787754936), 'min_duration_us': np.float64(1.536), 'max_duration_us': np.float64(1.663)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.030999999999999, 'mean_duration_us': 1.6061999999999999, 'median_duration_us': 1.632, 'std_dev_duration_us': 0.046786322787754936, 'min_duration_us': 1.536, 'max_duration_us': 1.663}]</t>
         </is>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.61)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.61}]</t>
         </is>
       </c>
       <c r="P82" t="n">
@@ -6954,12 +6954,12 @@
       </c>
       <c r="N83" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(7.968), 'mean_duration_us': np.float64(0.7968), 'median_duration_us': np.float64(0.8), 'std_dev_duration_us': np.float64(0.009600000000000008), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(0.8)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': 7.968, 'mean_duration_us': 0.7968, 'median_duration_us': 0.8, 'std_dev_duration_us': 0.009600000000000008, 'min_duration_us': 0.768, 'max_duration_us': 0.8}]</t>
         </is>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(0.8)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 0.8}]</t>
         </is>
       </c>
       <c r="P83" t="n">
@@ -7021,12 +7021,12 @@
       </c>
       <c r="N84" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.872), 'mean_duration_us': np.float64(1.5744), 'median_duration_us': np.float64(1.568), 'std_dev_duration_us': np.float64(0.02394660727535325), 'min_duration_us': np.float64(1.536), 'max_duration_us': np.float64(1.6)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.872, 'mean_duration_us': 1.5744, 'median_duration_us': 1.568, 'std_dev_duration_us': 0.02394660727535325, 'min_duration_us': 1.536, 'max_duration_us': 1.6}]</t>
         </is>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.57)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.57}]</t>
         </is>
       </c>
       <c r="P84" t="n">
@@ -7088,12 +7088,12 @@
       </c>
       <c r="N85" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.744), 'mean_duration_us': np.float64(1.5488), 'median_duration_us': np.float64(1.6), 'std_dev_duration_us': np.float64(0.09185728060420688), 'min_duration_us': np.float64(1.408), 'max_duration_us': np.float64(1.632)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.744, 'mean_duration_us': 1.5488, 'median_duration_us': 1.6, 'std_dev_duration_us': 0.09185728060420688, 'min_duration_us': 1.408, 'max_duration_us': 1.632}]</t>
         </is>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.55)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.55}]</t>
         </is>
       </c>
       <c r="P85" t="n">
@@ -7155,12 +7155,12 @@
       </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#7}::operator()() const::{lambda(float, bool)#1}, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#7}::operator()() const::{lambda(float, bool)#1}, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.454000000000001), 'mean_duration_us': np.float64(1.4908000000000001), 'median_duration_us': np.float64(1.536), 'std_dev_duration_us': np.float64(0.0797932327957703), 'min_duration_us': np.float64(1.344), 'max_duration_us': np.float64(1.567)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#7}::operator()() const::{lambda(float, bool)#1}, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#7}::operator()() const::{lambda(float, bool)#1}, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.454000000000001, 'mean_duration_us': 1.4908000000000001, 'median_duration_us': 1.536, 'std_dev_duration_us': 0.0797932327957703, 'min_duration_us': 1.344, 'max_duration_us': 1.567}]</t>
         </is>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(a...', 'stream': 7, 'mean_duration_us': np.float64(1.49)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(a...', 'stream': 7, 'mean_duration_us': 1.49}]</t>
         </is>
       </c>
       <c r="P86" t="n">
@@ -7222,12 +7222,12 @@
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.424999999999999), 'mean_duration_us': np.float64(1.4849999999999999), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.025502941006872143), 'min_duration_us': np.float64(1.472), 'max_duration_us': np.float64(1.536)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.424999999999999, 'mean_duration_us': 1.4849999999999999, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.025502941006872143, 'min_duration_us': 1.472, 'max_duration_us': 1.536}]</t>
         </is>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(1.48)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 1.48}]</t>
         </is>
       </c>
       <c r="P87" t="n">
@@ -7289,12 +7289,12 @@
       </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.264999999999999), 'mean_duration_us': np.float64(1.4529999999999998), 'median_duration_us': np.float64(1.441), 'std_dev_duration_us': np.float64(0.015517731793016656), 'min_duration_us': np.float64(1.44), 'max_duration_us': np.float64(1.472)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.264999999999999, 'mean_duration_us': 1.4529999999999998, 'median_duration_us': 1.441, 'std_dev_duration_us': 0.015517731793016656, 'min_duration_us': 1.44, 'max_duration_us': 1.472}]</t>
         </is>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.45)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.45}]</t>
         </is>
       </c>
       <c r="P88" t="n">
@@ -7356,12 +7356,12 @@
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16, bool)#1}, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16, bool)#1}, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.134), 'mean_duration_us': np.float64(1.4268), 'median_duration_us': np.float64(1.375), 'std_dev_duration_us': np.float64(0.08990083425641834), 'min_duration_us': np.float64(1.343), 'max_duration_us': np.float64(1.536)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16, bool)#1}, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::(anonymous namespace)::masked_fill_kernel(at::TensorIterator&amp;, c10::Scalar const&amp;)::{lambda()#1}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16, bool)#1}, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.134, 'mean_duration_us': 1.4268, 'median_duration_us': 1.375, 'std_dev_duration_us': 0.08990083425641834, 'min_duration_us': 1.343, 'max_duration_us': 1.536}]</t>
         </is>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(a...', 'stream': 7, 'mean_duration_us': np.float64(1.43)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::(a...', 'stream': 7, 'mean_duration_us': 1.43}]</t>
         </is>
       </c>
       <c r="P89" t="n">
@@ -7423,12 +7423,12 @@
       </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;(int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}, function_traits&lt;at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;::result_type*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.103999999999999), 'mean_duration_us': np.float64(1.4207999999999998), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.16639999999999996), 'min_duration_us': np.float64(1.248), 'max_duration_us': np.float64(1.696)}]</t>
+          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;(int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}, function_traits&lt;at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;::result_type*)', 'stream': 7, 'count': 5, 'total_duration_us': 7.103999999999999, 'mean_duration_us': 1.4207999999999998, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.16639999999999996, 'min_duration_us': 1.248, 'max_duration_us': 1.696}]</t>
         </is>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, a...', 'stream': 7, 'mean_duration_us': np.float64(1.42)}]</t>
+          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, a...', 'stream': 7, 'mean_duration_us': 1.42}]</t>
         </is>
       </c>
       <c r="P90" t="n">
@@ -7490,12 +7490,12 @@
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnOther_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnOther_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.040000000000001), 'mean_duration_us': np.float64(1.4080000000000001), 'median_duration_us': np.float64(1.344), 'std_dev_duration_us': np.float64(0.09706080568385983), 'min_duration_us': np.float64(1.312), 'max_duration_us': np.float64(1.568)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnOther_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnOther_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.040000000000001, 'mean_duration_us': 1.4080000000000001, 'median_duration_us': 1.344, 'std_dev_duration_us': 0.09706080568385983, 'min_duration_us': 1.312, 'max_duration_us': 1.568}]</t>
         </is>
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.41)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.41}]</t>
         </is>
       </c>
       <c r="P91" t="n">
@@ -7557,12 +7557,12 @@
       </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.008999999999999), 'mean_duration_us': np.float64(1.4017999999999997), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.08894132897590411), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.504)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.008999999999999, 'mean_duration_us': 1.4017999999999997, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.08894132897590411, 'min_duration_us': 1.28, 'max_duration_us': 1.504}]</t>
         </is>
       </c>
       <c r="O92" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bf...', 'stream': 7, 'mean_duration_us': np.float64(1.4)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bf...', 'stream': 7, 'mean_duration_us': 1.4}]</t>
         </is>
       </c>
       <c r="P92" t="n">
@@ -7624,12 +7624,12 @@
       </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::FillFunctor&lt;float&gt;, std::array&lt;char*, 1ul&gt; &gt;(int, at::native::FillFunctor&lt;float&gt;, std::array&lt;char*, 1ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.008000000000001), 'mean_duration_us': np.float64(1.4016000000000002), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.09997119585160516), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.504)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::FillFunctor&lt;float&gt;, std::array&lt;char*, 1ul&gt; &gt;(int, at::native::FillFunctor&lt;float&gt;, std::array&lt;char*, 1ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.008000000000001, 'mean_duration_us': 1.4016000000000002, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.09997119585160516, 'min_duration_us': 1.28, 'max_duration_us': 1.504}]</t>
         </is>
       </c>
       <c r="O93" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Fi...', 'stream': 7, 'mean_duration_us': np.float64(1.4)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Fi...', 'stream': 7, 'mean_duration_us': 1.4}]</t>
         </is>
       </c>
       <c r="P93" t="n">
@@ -7691,12 +7691,12 @@
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.007999999999999), 'mean_duration_us': np.float64(1.4015999999999997), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.08914168497397834), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.504)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.007999999999999, 'mean_duration_us': 1.4015999999999997, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.08914168497397834, 'min_duration_us': 1.28, 'max_duration_us': 1.504}]</t>
         </is>
       </c>
       <c r="O94" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(1.4)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 1.4}]</t>
         </is>
       </c>
       <c r="P94" t="n">
@@ -7758,12 +7758,12 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(6.687999999999999), 'mean_duration_us': np.float64(1.3375999999999997), 'median_duration_us': np.float64(1.408), 'std_dev_duration_us': np.float64(0.0868138237840034), 'min_duration_us': np.float64(1.216), 'max_duration_us': np.float64(1.408)}]</t>
+          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': 6.687999999999999, 'mean_duration_us': 1.3375999999999997, 'median_duration_us': 1.408, 'std_dev_duration_us': 0.0868138237840034, 'min_duration_us': 1.216, 'max_duration_us': 1.408}]</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(1.34)}]</t>
+          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'mean_duration_us': 1.34}]</t>
         </is>
       </c>
       <c r="P95" t="n">
@@ -7825,12 +7825,12 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;(int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}, function_traits&lt;at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;::result_type*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(6.176), 'mean_duration_us': np.float64(1.2352), 'median_duration_us': np.float64(1.28), 'std_dev_duration_us': np.float64(0.08245823185104081), 'min_duration_us': np.float64(1.12), 'max_duration_us': np.float64(1.312)}]</t>
+          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;(int, at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}, function_traits&lt;at::native::arange_cuda_out(c10::Scalar const&amp;, c10::Scalar const&amp;, c10::Scalar const&amp;, at::Tensor&amp;)::{lambda()#1}::operator()() const::{lambda()#4}::operator()() const::{lambda(long)#1}&gt;::result_type*)', 'stream': 7, 'count': 5, 'total_duration_us': 6.176, 'mean_duration_us': 1.2352, 'median_duration_us': 1.28, 'std_dev_duration_us': 0.08245823185104081, 'min_duration_us': 1.12, 'max_duration_us': 1.312}]</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, a...', 'stream': 7, 'mean_duration_us': np.float64(1.24)}]</t>
+          <t>[{'name': 'void (anonymous namespace)::elementwise_kernel_with_index&lt;int, a...', 'stream': 7, 'mean_duration_us': 1.24}]</t>
         </is>
       </c>
       <c r="P96" t="n">
@@ -7892,12 +7892,12 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::FillFunctor&lt;c10::BFloat16&gt;, std::array&lt;char*, 1ul&gt; &gt;(int, at::native::FillFunctor&lt;c10::BFloat16&gt;, std::array&lt;char*, 1ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(5.984000000000001), 'mean_duration_us': np.float64(1.1968), 'median_duration_us': np.float64(1.12), 'std_dev_duration_us': np.float64(0.09406040612287402), 'min_duration_us': np.float64(1.12), 'max_duration_us': np.float64(1.312)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::FillFunctor&lt;c10::BFloat16&gt;, std::array&lt;char*, 1ul&gt; &gt;(int, at::native::FillFunctor&lt;c10::BFloat16&gt;, std::array&lt;char*, 1ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 5.984000000000001, 'mean_duration_us': 1.1968, 'median_duration_us': 1.12, 'std_dev_duration_us': 0.09406040612287402, 'min_duration_us': 1.12, 'max_duration_us': 1.312}]</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Fi...', 'stream': 7, 'mean_duration_us': np.float64(1.2)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Fi...', 'stream': 7, 'mean_duration_us': 1.2}]</t>
         </is>
       </c>
       <c r="P97" t="n">
@@ -8185,12 +8185,12 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(130015.7), 'mean_duration_us': np.float64(1083.4641666666666), 'median_duration_us': np.float64(1082.965), 'std_dev_duration_us': np.float64(3.932529614919927), 'min_duration_us': np.float64(1075.574), 'max_duration_us': np.float64(1096.694)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_256x128_tn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': 130015.7, 'mean_duration_us': 1083.4641666666666, 'median_duration_us': 1082.965, 'std_dev_duration_us': 3.932529614919927, 'min_duration_us': 1075.574, 'max_duration_us': 1096.694}]</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_25...', 'stream': 7, 'mean_duration_us': np.float64(1083.46)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_25...', 'stream': 7, 'mean_duration_us': 1083.46}]</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -8315,12 +8315,12 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(99311.41), 'mean_duration_us': np.float64(827.5950833333334), 'median_duration_us': np.float64(826.9205), 'std_dev_duration_us': np.float64(2.9474507419783706), 'min_duration_us': np.float64(825.432), 'max_duration_us': np.float64(851.8)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1&gt;(cutlass_75_tensorop_bf16_s1688gemm_bf16_128x128_nn_align1::Params)', 'stream': 7, 'count': 120, 'total_duration_us': 99311.41, 'mean_duration_us': 827.5950833333334, 'median_duration_us': 826.9205, 'std_dev_duration_us': 2.9474507419783706, 'min_duration_us': 825.432, 'max_duration_us': 851.8}]</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_12...', 'stream': 7, 'mean_duration_us': np.float64(827.6)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_tensorop_bf16_s1688gemm_bf16_12...', 'stream': 7, 'mean_duration_us': 827.6}]</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
@@ -8445,12 +8445,12 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 480, 'total_duration_us': np.float64(449.6640000000001), 'mean_duration_us': np.float64(0.9368000000000002), 'median_duration_us': np.float64(0.96), 'std_dev_duration_us': np.float64(0.14700191892171566), 'min_duration_us': np.float64(0.767), 'max_duration_us': np.float64(1.408)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 480, 'total_duration_us': np.float64(10035.521), 'mean_duration_us': np.float64(20.90733541666667), 'median_duration_us': np.float64(20.912), 'std_dev_duration_us': np.float64(0.2994497001373127), 'min_duration_us': np.float64(20.256), 'max_duration_us': np.float64(22.015)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 480, 'total_duration_us': 449.6640000000001, 'mean_duration_us': 0.9368000000000002, 'median_duration_us': 0.96, 'std_dev_duration_us': 0.14700191892171566, 'min_duration_us': 0.767, 'max_duration_us': 1.408}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 480, 'total_duration_us': 10035.521, 'mean_duration_us': 20.90733541666667, 'median_duration_us': 20.912, 'std_dev_duration_us': 0.2994497001373127, 'min_duration_us': 20.256, 'max_duration_us': 22.015}]</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.94)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(20.91)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.94}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 20.91}]</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
@@ -8575,12 +8575,12 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(115.61200000000002), 'mean_duration_us': np.float64(0.9634333333333335), 'median_duration_us': np.float64(0.96), 'std_dev_duration_us': np.float64(0.18370559478566667), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(1.6)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(7766.737), 'mean_duration_us': np.float64(64.72280833333333), 'median_duration_us': np.float64(64.639), 'std_dev_duration_us': np.float64(0.5570301951096441), 'min_duration_us': np.float64(63.711), 'max_duration_us': np.float64(65.951)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': 115.61200000000002, 'mean_duration_us': 0.9634333333333335, 'median_duration_us': 0.96, 'std_dev_duration_us': 0.18370559478566667, 'min_duration_us': 0.768, 'max_duration_us': 1.6}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': 7766.737, 'mean_duration_us': 64.72280833333333, 'median_duration_us': 64.639, 'std_dev_duration_us': 0.5570301951096441, 'min_duration_us': 63.711, 'max_duration_us': 65.951}]</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.96)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(64.72)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.96}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 64.72}]</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
@@ -8705,12 +8705,12 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(116.09), 'mean_duration_us': np.float64(0.9674166666666667), 'median_duration_us': np.float64(0.96), 'std_dev_duration_us': np.float64(0.15527371441711854), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(1.568)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(6884.5689999999995), 'mean_duration_us': np.float64(57.37140833333333), 'median_duration_us': np.float64(57.344), 'std_dev_duration_us': np.float64(0.31250691981227396), 'min_duration_us': np.float64(56.639), 'max_duration_us': np.float64(58.048)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 120, 'total_duration_us': 116.09, 'mean_duration_us': 0.9674166666666667, 'median_duration_us': 0.96, 'std_dev_duration_us': 0.15527371441711854, 'min_duration_us': 0.768, 'max_duration_us': 1.568}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 120, 'total_duration_us': 6884.5689999999995, 'mean_duration_us': 57.37140833333333, 'median_duration_us': 57.344, 'std_dev_duration_us': 0.31250691981227396, 'min_duration_us': 56.639, 'max_duration_us': 58.048}]</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.97)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(57.37)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.97}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 57.37}]</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
@@ -8835,12 +8835,12 @@
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 240, 'total_duration_us': np.float64(1579.851), 'mean_duration_us': np.float64(6.5827125), 'median_duration_us': np.float64(6.592), 'std_dev_duration_us': np.float64(0.13116311667951205), 'min_duration_us': np.float64(6.303), 'max_duration_us': np.float64(6.975)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 240, 'total_duration_us': 1579.851, 'mean_duration_us': 6.5827125, 'median_duration_us': 6.592, 'std_dev_duration_us': 0.13116311667951205, 'min_duration_us': 6.303, 'max_duration_us': 6.975}]</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': np.float64(6.58)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': 6.58}]</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
@@ -8965,12 +8965,12 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(385.4959999999999), 'mean_duration_us': np.float64(6.424933333333332), 'median_duration_us': np.float64(6.336), 'std_dev_duration_us': np.float64(0.19279919317489072), 'min_duration_us': np.float64(6.239), 'max_duration_us': np.float64(6.912)}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, __nv_bfloat16, float, __nv_bfloat16, true, true, false&gt;(cublasLt::cublasSplitKParams&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, float const*, float const*, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, void*, long, float*, int*)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(140.35000000000002), 'mean_duration_us': np.float64(2.339166666666667), 'median_duration_us': np.float64(2.336), 'std_dev_duration_us': np.float64(0.037292164801142315), 'min_duration_us': np.float64(2.272), 'max_duration_us': np.float64(2.496)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 385.4959999999999, 'mean_duration_us': 6.424933333333332, 'median_duration_us': 6.336, 'std_dev_duration_us': 0.19279919317489072, 'min_duration_us': 6.239, 'max_duration_us': 6.912}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, __nv_bfloat16, float, __nv_bfloat16, true, true, false&gt;(cublasLt::cublasSplitKParams&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, float const*, float const*, __nv_bfloat16 const*, __nv_bfloat16 const*, __nv_bfloat16*, void*, long, float*, int*)', 'stream': 7, 'count': 60, 'total_duration_us': 140.35000000000002, 'mean_duration_us': 2.339166666666667, 'median_duration_us': 2.336, 'std_dev_duration_us': 0.037292164801142315, 'min_duration_us': 2.272, 'max_duration_us': 2.496}]</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': np.float64(6.42)}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': np.float64(2.34)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': 6.42}, {'name': 'void cublasLt::splitKreduce_kernel&lt;32, 16, int, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': 2.34}]</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
@@ -9095,12 +9095,12 @@
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 20, 'total_duration_us': np.float64(17.248), 'mean_duration_us': np.float64(0.8624), 'median_duration_us': np.float64(0.8), 'std_dev_duration_us': np.float64(0.13365305832639968), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(1.248)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 20, 'total_duration_us': np.float64(414.7149999999999), 'mean_duration_us': np.float64(20.735749999999996), 'median_duration_us': np.float64(20.768), 'std_dev_duration_us': np.float64(0.42032010123238245), 'min_duration_us': np.float64(19.936), 'max_duration_us': np.float64(21.279)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 20, 'total_duration_us': 17.248, 'mean_duration_us': 0.8624, 'median_duration_us': 0.8, 'std_dev_duration_us': 0.13365305832639968, 'min_duration_us': 0.768, 'max_duration_us': 1.248}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warpgroupsize1x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 20, 'total_duration_us': 414.7149999999999, 'mean_duration_us': 20.735749999999996, 'median_duration_us': 20.768, 'std_dev_duration_us': 0.42032010123238245, 'min_duration_us': 19.936, 'max_duration_us': 21.279}]</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(0.86)}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(20.74)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 0.86}, {'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize128x128x64_warp...', 'stream': 7, 'mean_duration_us': 20.74}]</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
@@ -9225,12 +9225,12 @@
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(422.845), 'mean_duration_us': np.float64(7.047416666666667), 'median_duration_us': np.float64(6.976), 'std_dev_duration_us': np.float64(0.17790056133194818), 'min_duration_us': np.float64(6.752), 'max_duration_us': np.float64(7.52)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8&gt;(cutlass_80_tensorop_bf16_s16816gemm_relu_bf16_64x64_64x6_tn_align8::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 422.845, 'mean_duration_us': 7.047416666666667, 'median_duration_us': 6.976, 'std_dev_duration_us': 0.17790056133194818, 'min_duration_us': 6.752, 'max_duration_us': 7.52}]</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': np.float64(7.05)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_tensorop_bf16_s16816gemm_relu_b...', 'stream': 7, 'mean_duration_us': 7.05}]</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
@@ -9355,12 +9355,12 @@
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(185.69699999999997), 'mean_duration_us': np.float64(3.0949499999999994), 'median_duration_us': np.float64(3.104), 'std_dev_duration_us': np.float64(0.04453478977159322), 'min_duration_us': np.float64(3.008), 'max_duration_us': np.float64(3.168)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_tn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 185.69699999999997, 'mean_duration_us': 3.0949499999999994, 'median_duration_us': 3.104, 'std_dev_duration_us': 0.04453478977159322, 'min_duration_us': 3.008, 'max_duration_us': 3.168}]</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': np.float64(3.09)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': 3.09}]</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
@@ -9485,12 +9485,12 @@
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(167.428), 'mean_duration_us': np.float64(2.7904666666666667), 'median_duration_us': np.float64(2.816), 'std_dev_duration_us': np.float64(0.037250264726874344), 'min_duration_us': np.float64(2.72), 'max_duration_us': np.float64(2.88)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1&gt;(cutlass_75_wmma_tensorop_bf16_s161616gemm_bf16_32x32_32x1_nn_align1::Params)', 'stream': 7, 'count': 60, 'total_duration_us': 167.428, 'mean_duration_us': 2.7904666666666667, 'median_duration_us': 2.816, 'std_dev_duration_us': 0.037250264726874344, 'min_duration_us': 2.72, 'max_duration_us': 2.88}]</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': np.float64(2.79)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_75_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': 2.79}]</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
@@ -9615,12 +9615,12 @@
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 15, 'total_duration_us': np.float64(35.168), 'mean_duration_us': np.float64(2.344533333333333), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.10418372660300108), 'min_duration_us': np.float64(2.176), 'max_duration_us': np.float64(2.56)}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 15, 'total_duration_us': np.float64(83.104), 'mean_duration_us': np.float64(5.540266666666667), 'median_duration_us': np.float64(5.376), 'std_dev_duration_us': np.float64(0.32818683025916123), 'min_duration_us': np.float64(5.152), 'max_duration_us': np.float64(6.176)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 15, 'total_duration_us': 35.168, 'mean_duration_us': 2.344533333333333, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.10418372660300108, 'min_duration_us': 2.176, 'max_duration_us': 2.56}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 15, 'total_duration_us': 83.104, 'mean_duration_us': 5.540266666666667, 'median_duration_us': 5.376, 'std_dev_duration_us': 0.32818683025916123, 'min_duration_us': 5.152, 'max_duration_us': 6.176}]</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.34)}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': np.float64(5.54)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.34}, {'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': 5.54}]</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
@@ -9745,12 +9745,12 @@
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warpgroupsize2x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(86.78200000000001), 'mean_duration_us': np.float64(17.3564), 'median_duration_us': np.float64(17.376), 'std_dev_duration_us': np.float64(0.07209049868047837), 'min_duration_us': np.float64(17.215), 'max_duration_us': np.float64(17.408)}]</t>
+          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warpgroupsize2x1x1_execute_segment_k_off_kernel__5x_cublas', 'stream': 7, 'count': 5, 'total_duration_us': 86.78200000000001, 'mean_duration_us': 17.3564, 'median_duration_us': 17.376, 'std_dev_duration_us': 0.07209049868047837, 'min_duration_us': 17.215, 'max_duration_us': 17.408}]</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warp...', 'stream': 7, 'mean_duration_us': np.float64(17.36)}]</t>
+          <t>[{'name': 'sm90_xmma_gemm_bf16bf16_bf16f32_f32_tn_n_tilesize256x128x64_warp...', 'stream': 7, 'mean_duration_us': 17.36}]</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
@@ -9875,12 +9875,12 @@
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2&gt;(cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2::Params)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(56.54299999999999), 'mean_duration_us': np.float64(11.308599999999998), 'median_duration_us': np.float64(11.296), 'std_dev_duration_us': np.float64(0.10403768547983014), 'min_duration_us': np.float64(11.168), 'max_duration_us': np.float64(11.487)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2&gt;(cutlass_80_wmma_tensorop_bf16_s161616gemm_bf16_32x32_128x2_tn_align2::Params)', 'stream': 7, 'count': 5, 'total_duration_us': 56.54299999999999, 'mean_duration_us': 11.308599999999998, 'median_duration_us': 11.296, 'std_dev_duration_us': 0.10403768547983014, 'min_duration_us': 11.168, 'max_duration_us': 11.487}]</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': np.float64(11.31)}]</t>
+          <t>[{'name': 'void cutlass::Kernel2&lt;cutlass_80_wmma_tensorop_bf16_s161616gemm_...', 'stream': 7, 'mean_duration_us': 11.31}]</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
@@ -10005,12 +10005,12 @@
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(23.615000000000002), 'mean_duration_us': np.float64(4.723000000000001), 'median_duration_us': np.float64(4.704), 'std_dev_duration_us': np.float64(0.06861486719363401), 'min_duration_us': np.float64(4.64), 'max_duration_us': np.float64(4.831)}]</t>
+          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, 128, 16, 4, 4, false, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;, float, float)', 'stream': 7, 'count': 5, 'total_duration_us': 23.615000000000002, 'mean_duration_us': 4.723000000000001, 'median_duration_us': 4.704, 'std_dev_duration_us': 0.06861486719363401, 'min_duration_us': 4.64, 'max_duration_us': 4.831}]</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': np.float64(4.72)}]</t>
+          <t>[{'name': 'void gemv2T_kernel_val&lt;int, int, __nv_bfloat16, __nv_bfloat16, _...', 'stream': 7, 'mean_duration_us': 4.72}]</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
@@ -10135,12 +10135,12 @@
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt; &gt;(cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(10.143), 'mean_duration_us': np.float64(2.0286), 'median_duration_us': np.float64(2.047), 'std_dev_duration_us': np.float64(0.02545270123189289), 'min_duration_us': np.float64(1.984), 'max_duration_us': np.float64(2.048)}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStridedBatched&lt;float&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt; &gt;(float const*, float, cublasGemvTensorStridedBatched&lt;float&gt;, int, float const*, float, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, cublasPointerMode_t, cublasLtEpilogue_t, cublasGemvTensorStridedBatched&lt;biasType&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;::value_type, float&gt;::type const&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.183000000000002), 'mean_duration_us': np.float64(2.6366000000000005), 'median_duration_us': np.float64(2.688), 'std_dev_duration_us': np.float64(0.08984341934721768), 'min_duration_us': np.float64(2.527), 'max_duration_us': np.float64(2.72)}]</t>
+          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt; &gt;(cublasDotParams&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;float&gt; &gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 10.143, 'mean_duration_us': 2.0286, 'median_duration_us': 2.047, 'std_dev_duration_us': 0.02545270123189289, 'min_duration_us': 1.984, 'max_duration_us': 2.048}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStridedBatched&lt;float&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt; &gt;(float const*, float, cublasGemvTensorStridedBatched&lt;float&gt;, int, float const*, float, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, cublasPointerMode_t, cublasLtEpilogue_t, cublasGemvTensorStridedBatched&lt;biasType&lt;cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;::value_type, float&gt;::type const&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 13.183000000000002, 'mean_duration_us': 2.6366000000000005, 'median_duration_us': 2.688, 'std_dev_duration_us': 0.08984341934721768, 'min_duration_us': 2.527, 'max_duration_us': 2.72}]</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorS...', 'stream': 7, 'mean_duration_us': np.float64(2.03)}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStrided...', 'stream': 7, 'mean_duration_us': np.float64(2.64)}]</t>
+          <t>[{'name': 'void dot_kernel&lt;float, 128, 0, cublasDotParams&lt;cublasGemvTensorS...', 'stream': 7, 'mean_duration_us': 2.03}, {'name': 'void reduce_1Block_kernel&lt;float, 128, 7, cublasGemvTensorStrided...', 'stream': 7, 'mean_duration_us': 2.64}]</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
@@ -10265,12 +10265,12 @@
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(18.784), 'mean_duration_us': np.float64(3.7567999999999997), 'median_duration_us': np.float64(3.744), 'std_dev_duration_us': np.float64(0.03263372488699366), 'min_duration_us': np.float64(3.712), 'max_duration_us': np.float64(3.808)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 18.784, 'mean_duration_us': 3.7567999999999997, 'median_duration_us': 3.744, 'std_dev_duration_us': 0.03263372488699366, 'min_duration_us': 3.712, 'max_duration_us': 3.808}]</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': np.float64(3.76)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': 3.76}]</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
@@ -10395,12 +10395,12 @@
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(17.918), 'mean_duration_us': np.float64(3.5835999999999997), 'median_duration_us': np.float64(3.552), 'std_dev_duration_us': np.float64(0.049834124854360604), 'min_duration_us': np.float64(3.551), 'max_duration_us': np.float64(3.68)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int, int, __nv_bfloat16, __nv_bfloat16, __nv_bfloat16, float, false, true, true, false, 7, false, cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt; &gt;(cublasGemvParamsEx&lt;int, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16 const&gt;, cublasGemvTensorStridedBatched&lt;__nv_bfloat16&gt;, float&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 17.918, 'mean_duration_us': 3.5835999999999997, 'median_duration_us': 3.552, 'std_dev_duration_us': 0.049834124854360604, 'min_duration_us': 3.551, 'max_duration_us': 3.68}]</t>
         </is>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': np.float64(3.58)}]</t>
+          <t>[{'name': 'std::enable_if&lt;!(false), void&gt;::type internal::gemvx::kernel&lt;int...', 'stream': 7, 'mean_duration_us': 3.58}]</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
@@ -10780,12 +10780,12 @@
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(28.127000000000002), 'mean_duration_us': np.float64(5.625400000000001), 'median_duration_us': np.float64(5.664), 'std_dev_duration_us': np.float64(0.08941498755801505), 'min_duration_us': np.float64(5.503), 'max_duration_us': np.float64(5.728)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(222.207), 'mean_duration_us': np.float64(44.4414), 'median_duration_us': np.float64(44.384), 'std_dev_duration_us': np.float64(0.1792647204555328), 'min_duration_us': np.float64(44.224), 'max_duration_us': np.float64(44.768)}, {'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(10.85), 'mean_duration_us': np.float64(2.17), 'median_duration_us': np.float64(2.176), 'std_dev_duration_us': np.float64(0.013007690033207267), 'min_duration_us': np.float64(2.144), 'max_duration_us': np.float64(2.177)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(58.303000000000004), 'mean_duration_us': np.float64(11.6606), 'median_duration_us': np.float64(11.679), 'std_dev_duration_us': np.float64(0.15088485676170435), 'min_duration_us': np.float64(11.424), 'max_duration_us': np.float64(11.872)}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8&gt;(cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8::Params)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(982.9660000000001), 'mean_duration_us': np.float64(196.59320000000002), 'median_duration_us': np.float64(196.542), 'std_dev_duration_us': np.float64(0.4292092263686784), 'min_duration_us': np.float64(195.966), 'max_duration_us': np.float64(197.245)}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16, __nv_bfloat16, float, true, false, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nhwc2nchw_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(48.35), 'mean_duration_us': np.float64(9.67), 'median_duration_us': np.float64(9.663), 'std_dev_duration_us': np.float64(0.0547539952880155), 'min_duration_us': np.float64(9.6), 'max_duration_us': np.float64(9.759)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': 28.127000000000002, 'mean_duration_us': 5.625400000000001, 'median_duration_us': 5.664, 'std_dev_duration_us': 0.08941498755801505, 'min_duration_us': 5.503, 'max_duration_us': 5.728}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 222.207, 'mean_duration_us': 44.4414, 'median_duration_us': 44.384, 'std_dev_duration_us': 0.1792647204555328, 'min_duration_us': 44.224, 'max_duration_us': 44.768}, {'name': 'Memset (Device)', 'stream': 7, 'count': 5, 'total_duration_us': 10.85, 'mean_duration_us': 2.17, 'median_duration_us': 2.176, 'std_dev_duration_us': 0.013007690033207267, 'min_duration_us': 2.144, 'max_duration_us': 2.177}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16, __nv_bfloat16, float, false, true, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nchw2nhwc_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 58.303000000000004, 'mean_duration_us': 11.6606, 'median_duration_us': 11.679, 'std_dev_duration_us': 0.15088485676170435, 'min_duration_us': 11.424, 'max_duration_us': 11.872}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8&gt;(cutlass_tensorop_bf16_s16816fprop_optimized_bf16_256x64_32x4_nhwc_align8::Params)', 'stream': 7, 'count': 5, 'total_duration_us': 982.9660000000001, 'mean_duration_us': 196.59320000000002, 'median_duration_us': 196.542, 'std_dev_duration_us': 0.4292092263686784, 'min_duration_us': 195.966, 'max_duration_us': 197.245}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16, __nv_bfloat16, float, true, false, (cudnnKernelDataType_t)0&gt;(cudnn::engines_precompiled::nhwc2nchw_params_t&lt;float&gt;, __nv_bfloat16 const*, __nv_bfloat16*)', 'stream': 7, 'count': 5, 'total_duration_us': 48.35, 'mean_duration_us': 9.67, 'median_duration_us': 9.663, 'std_dev_duration_us': 0.0547539952880155, 'min_duration_us': 9.6, 'max_duration_us': 9.759}]</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(5.63)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': np.float64(44.44)}, {'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': np.float64(2.17)}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': np.float64(11.66)}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop...', 'stream': 7, 'mean_duration_us': np.float64(196.59)}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': np.float64(9.67)}]</t>
+          <t>[{'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 5.63}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': 44.44}, {'name': 'Memset (Device)', 'stream': 7, 'mean_duration_us': 2.17}, {'name': 'void cudnn::engines_precompiled::nchwToNhwcKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': 11.66}, {'name': 'void cutlass__5x_cudnn::Kernel&lt;cutlass_tensorop_bf16_s16816fprop...', 'stream': 7, 'mean_duration_us': 196.59}, {'name': 'void cudnn::engines_precompiled::nhwcToNchwKernel&lt;__nv_bfloat16,...', 'stream': 7, 'mean_duration_us': 9.67}]</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
@@ -11081,12 +11081,12 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8133.554), 'mean_duration_us': np.float64(1626.7108), 'median_duration_us': np.float64(347.196), 'std_dev_duration_us': np.float64(1579.6924965375256), 'min_duration_us': np.float64(325.565), 'max_duration_us': np.float64(3620.445)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 8133.554, 'mean_duration_us': 1626.7108, 'median_duration_us': 347.196, 'std_dev_duration_us': 1579.6924965375256, 'min_duration_us': 325.565, 'max_duration_us': 3620.445}]</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(1626.71)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 1626.71}]</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -11201,12 +11201,12 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 360, 'total_duration_us': np.float64(5038.033), 'mean_duration_us': np.float64(13.994536111111112), 'median_duration_us': np.float64(13.152), 'std_dev_duration_us': np.float64(1.3500063184322875), 'min_duration_us': np.float64(12.736), 'max_duration_us': np.float64(16.288)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 360, 'total_duration_us': 5038.033, 'mean_duration_us': 13.994536111111112, 'median_duration_us': 13.152, 'std_dev_duration_us': 1.3500063184322875, 'min_duration_us': 12.736, 'max_duration_us': 16.288}]</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(13.99)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 13.99}]</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -11317,12 +11317,12 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(3988.498), 'mean_duration_us': np.float64(33.23748333333334), 'median_duration_us': np.float64(33.055), 'std_dev_duration_us': np.float64(0.39268874407375365), 'min_duration_us': np.float64(32.8), 'max_duration_us': np.float64(34.272)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 3988.498, 'mean_duration_us': 33.23748333333334, 'median_duration_us': 33.055, 'std_dev_duration_us': 0.39268874407375365, 'min_duration_us': 32.8, 'max_duration_us': 34.272}]</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': np.float64(33.24)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': 33.24}]</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -11437,12 +11437,12 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(2338.761), 'mean_duration_us': np.float64(467.7522), 'median_duration_us': np.float64(464.252), 'std_dev_duration_us': np.float64(11.281809454161158), 'min_duration_us': np.float64(454.556), 'max_duration_us': np.float64(487.899)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 2338.761, 'mean_duration_us': 467.7522, 'median_duration_us': 464.252, 'std_dev_duration_us': 11.281809454161158, 'min_duration_us': 454.556, 'max_duration_us': 487.899}]</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(467.75)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 467.75}]</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -11557,12 +11557,12 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(2324.394), 'mean_duration_us': np.float64(464.87879999999996), 'median_duration_us': np.float64(472.188), 'std_dev_duration_us': np.float64(19.601893596282974), 'min_duration_us': np.float64(436.444), 'max_duration_us': np.float64(489.34)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 2324.394, 'mean_duration_us': 464.87879999999996, 'median_duration_us': 472.188, 'std_dev_duration_us': 19.601893596282974, 'min_duration_us': 436.444, 'max_duration_us': 489.34}]</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(464.88)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 464.88}]</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -11677,12 +11677,12 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(1873.8329999999999), 'mean_duration_us': np.float64(15.615274999999999), 'median_duration_us': np.float64(15.584), 'std_dev_duration_us': np.float64(0.1854254999768552), 'min_duration_us': np.float64(15.264), 'max_duration_us': np.float64(16.384)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': 1873.8329999999999, 'mean_duration_us': 15.615274999999999, 'median_duration_us': 15.584, 'std_dev_duration_us': 0.1854254999768552, 'min_duration_us': 15.264, 'max_duration_us': 16.384}]</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(15.62)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 15.62}]</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -11797,12 +11797,12 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(1627.952), 'mean_duration_us': np.float64(325.5904), 'median_duration_us': np.float64(333.501), 'std_dev_duration_us': np.float64(11.368233417730304), 'min_duration_us': np.float64(304.989), 'max_duration_us': np.float64(334.205)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': 1627.952, 'mean_duration_us': 325.5904, 'median_duration_us': 333.501, 'std_dev_duration_us': 11.368233417730304, 'min_duration_us': 304.989, 'max_duration_us': 334.205}]</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(325.59)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 325.59}]</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -11917,12 +11917,12 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 180, 'total_duration_us': np.float64(457.9199999999999), 'mean_duration_us': np.float64(2.5439999999999996), 'median_duration_us': np.float64(2.4645), 'std_dev_duration_us': np.float64(0.22104903930525865), 'min_duration_us': np.float64(2.24), 'max_duration_us': np.float64(3.232)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 180, 'total_duration_us': 457.9199999999999, 'mean_duration_us': 2.5439999999999996, 'median_duration_us': 2.4645, 'std_dev_duration_us': 0.22104903930525865, 'min_duration_us': 2.24, 'max_duration_us': 3.232}]</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.54)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.54}]</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -12037,12 +12037,12 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(163.17200000000005), 'mean_duration_us': np.float64(2.719533333333334), 'median_duration_us': np.float64(2.784), 'std_dev_duration_us': np.float64(0.14011381881250043), 'min_duration_us': np.float64(2.527), 'max_duration_us': np.float64(3.008)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 60, 'total_duration_us': 163.17200000000005, 'mean_duration_us': 2.719533333333334, 'median_duration_us': 2.784, 'std_dev_duration_us': 0.14011381881250043, 'min_duration_us': 2.527, 'max_duration_us': 3.008}]</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.72)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.72}]</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -12153,12 +12153,12 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(105.02100000000002), 'mean_duration_us': np.float64(1.7503500000000003), 'median_duration_us': np.float64(1.76), 'std_dev_duration_us': np.float64(0.021235838418422137), 'min_duration_us': np.float64(1.696), 'max_duration_us': np.float64(1.792)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 105.02100000000002, 'mean_duration_us': 1.7503500000000003, 'median_duration_us': 1.76, 'std_dev_duration_us': 0.021235838418422137, 'min_duration_us': 1.696, 'max_duration_us': 1.792}]</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': np.float64(1.75)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': 1.75}]</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
@@ -12273,12 +12273,12 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(20.255), 'mean_duration_us': np.float64(4.051), 'median_duration_us': np.float64(4.032), 'std_dev_duration_us': np.float64(0.02550294100687212), 'min_duration_us': np.float64(4.032), 'max_duration_us': np.float64(4.096)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': 20.255, 'mean_duration_us': 4.051, 'median_duration_us': 4.032, 'std_dev_duration_us': 0.02550294100687212, 'min_duration_us': 4.032, 'max_duration_us': 4.096}]</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(4.05)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 4.05}]</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
@@ -12379,12 +12379,12 @@
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(17.44), 'mean_duration_us': np.float64(1.7440000000000002), 'median_duration_us': np.float64(1.7440000000000002), 'std_dev_duration_us': np.float64(0.9569284194755635), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(2.72)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': 17.44, 'mean_duration_us': 1.7440000000000002, 'median_duration_us': 1.7440000000000002, 'std_dev_duration_us': 0.9569284194755635, 'min_duration_us': 0.768, 'max_duration_us': 2.72}]</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(1.74)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 1.74}]</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
@@ -12499,12 +12499,12 @@
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.717999999999998), 'mean_duration_us': np.float64(2.9435999999999996), 'median_duration_us': np.float64(2.944), 'std_dev_duration_us': np.float64(0.0004898979485565817), 'min_duration_us': np.float64(2.943), 'max_duration_us': np.float64(2.944)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 14.717999999999998, 'mean_duration_us': 2.9435999999999996, 'median_duration_us': 2.944, 'std_dev_duration_us': 0.0004898979485565817, 'min_duration_us': 2.943, 'max_duration_us': 2.944}]</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.94)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.94}]</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
@@ -12619,12 +12619,12 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.495999999999999), 'mean_duration_us': np.float64(2.8991999999999996), 'median_duration_us': np.float64(2.912), 'std_dev_duration_us': np.float64(0.032633724886993856), 'min_duration_us': np.float64(2.848), 'max_duration_us': np.float64(2.944)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 14.495999999999999, 'mean_duration_us': 2.8991999999999996, 'median_duration_us': 2.912, 'std_dev_duration_us': 0.032633724886993856, 'min_duration_us': 2.848, 'max_duration_us': 2.944}]</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.9)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.9}]</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
@@ -12739,12 +12739,12 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.985), 'mean_duration_us': np.float64(2.7969999999999997), 'median_duration_us': np.float64(2.785), 'std_dev_duration_us': np.float64(0.015517731793016621), 'min_duration_us': np.float64(2.784), 'max_duration_us': np.float64(2.816)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#7}::operator()() const::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 13.985, 'mean_duration_us': 2.7969999999999997, 'median_duration_us': 2.785, 'std_dev_duration_us': 0.015517731793016621, 'min_duration_us': 2.784, 'max_duration_us': 2.816}]</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': np.float64(2.8)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': 2.8}]</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
@@ -12859,12 +12859,12 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.472000000000001), 'mean_duration_us': np.float64(2.6944000000000004), 'median_duration_us': np.float64(2.752), 'std_dev_duration_us': np.float64(0.10398769157934018), 'min_duration_us': np.float64(2.528), 'max_duration_us': np.float64(2.816)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 13.472000000000001, 'mean_duration_us': 2.6944000000000004, 'median_duration_us': 2.752, 'std_dev_duration_us': 0.10398769157934018, 'min_duration_us': 2.528, 'max_duration_us': 2.816}]</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.69)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.69}]</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
@@ -12979,12 +12979,12 @@
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.407000000000002), 'mean_duration_us': np.float64(2.6814000000000004), 'median_duration_us': np.float64(2.656), 'std_dev_duration_us': np.float64(0.07142996570067763), 'min_duration_us': np.float64(2.623), 'max_duration_us': np.float64(2.816)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 13.407000000000002, 'mean_duration_us': 2.6814000000000004, 'median_duration_us': 2.656, 'std_dev_duration_us': 0.07142996570067763, 'min_duration_us': 2.623, 'max_duration_us': 2.816}]</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.68)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.68}]</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
@@ -13099,12 +13099,12 @@
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(13.345), 'mean_duration_us': np.float64(2.669), 'median_duration_us': np.float64(2.72), 'std_dev_duration_us': np.float64(0.08978641322605552), 'min_duration_us': np.float64(2.56), 'max_duration_us': np.float64(2.753)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 13.345, 'mean_duration_us': 2.669, 'median_duration_us': 2.72, 'std_dev_duration_us': 0.08978641322605552, 'min_duration_us': 2.56, 'max_duration_us': 2.753}]</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.67)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.67}]</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
@@ -13219,12 +13219,12 @@
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(12.222999999999999), 'mean_duration_us': np.float64(2.4446), 'median_duration_us': np.float64(2.336), 'std_dev_duration_us': np.float64(0.1469742834648294), 'min_duration_us': np.float64(2.303), 'max_duration_us': np.float64(2.624)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1}&gt;(at::TensorIteratorBase&amp;, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#12}::operator()() const::{lambda(c10::BFloat16)#1} const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 12.222999999999999, 'mean_duration_us': 2.4446, 'median_duration_us': 2.336, 'std_dev_duration_us': 0.1469742834648294, 'min_duration_us': 2.303, 'max_duration_us': 2.624}]</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.44)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.44}]</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
@@ -13339,12 +13339,12 @@
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(11.904), 'mean_duration_us': np.float64(2.3808), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.04340691189200176), 'min_duration_us': np.float64(2.336), 'max_duration_us': np.float64(2.464)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 11.904, 'mean_duration_us': 2.3808, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.04340691189200176, 'min_duration_us': 2.336, 'max_duration_us': 2.464}]</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.38)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.38}]</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
@@ -13459,12 +13459,12 @@
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(11.904), 'mean_duration_us': np.float64(2.3808), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.0478932145507065), 'min_duration_us': np.float64(2.336), 'max_duration_us': np.float64(2.464)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'count': 5, 'total_duration_us': 11.904, 'mean_duration_us': 2.3808, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.0478932145507065, 'min_duration_us': 2.336, 'max_duration_us': 2.464}]</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': np.float64(2.38)}]</t>
+          <t>[{'name': 'Memcpy DtoH (Device -&gt; Pageable)', 'stream': 7, 'mean_duration_us': 2.38}]</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
@@ -13575,12 +13575,12 @@
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.896), 'mean_duration_us': np.float64(1.7792000000000001), 'median_duration_us': np.float64(1.792), 'std_dev_duration_us': np.float64(0.025600000000000022), 'min_duration_us': np.float64(1.728), 'max_duration_us': np.float64(1.792)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::sigmoid_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#2}::operator()() const::{lambda()#4}::operator()() const::{lambda(c10::BFloat16)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.896, 'mean_duration_us': 1.7792000000000001, 'median_duration_us': 1.792, 'std_dev_duration_us': 0.025600000000000022, 'min_duration_us': 1.728, 'max_duration_us': 1.792}]</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': np.float64(1.78)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::si...', 'stream': 7, 'mean_duration_us': 1.78}]</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
@@ -13681,12 +13681,12 @@
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.769), 'mean_duration_us': np.float64(1.7538), 'median_duration_us': np.float64(1.792), 'std_dev_duration_us': np.float64(0.0742762411542211), 'min_duration_us': np.float64(1.664), 'max_duration_us': np.float64(1.825)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#11}::operator()() const::{lambda(bool)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.769, 'mean_duration_us': 1.7538, 'median_duration_us': 1.792, 'std_dev_duration_us': 0.0742762411542211, 'min_duration_us': 1.664, 'max_duration_us': 1.825}]</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': np.float64(1.75)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': 1.75}]</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
@@ -13787,12 +13787,12 @@
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.64), 'mean_duration_us': np.float64(1.7280000000000002), 'median_duration_us': np.float64(1.696), 'std_dev_duration_us': np.float64(0.10516273104099186), 'min_duration_us': np.float64(1.6), 'max_duration_us': np.float64(1.92)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, 4, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::direct_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda()#3}::operator()() const::{lambda()#3}::operator()() const::{lambda(int)#1}, std::array&lt;char*, 2ul&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;1&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.64, 'mean_duration_us': 1.7280000000000002, 'median_duration_us': 1.696, 'std_dev_duration_us': 0.10516273104099186, 'min_duration_us': 1.6, 'max_duration_us': 1.92}]</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': np.float64(1.73)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::direct_...', 'stream': 7, 'mean_duration_us': 1.73}]</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
@@ -13907,12 +13907,12 @@
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(7.968), 'mean_duration_us': np.float64(0.7968), 'median_duration_us': np.float64(0.8), 'std_dev_duration_us': np.float64(0.009600000000000008), 'min_duration_us': np.float64(0.768), 'max_duration_us': np.float64(0.8)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'count': 10, 'total_duration_us': 7.968, 'mean_duration_us': 0.7968, 'median_duration_us': 0.8, 'std_dev_duration_us': 0.009600000000000008, 'min_duration_us': 0.768, 'max_duration_us': 0.8}]</t>
         </is>
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(0.8)}]</t>
+          <t>[{'name': 'Memcpy HtoD (Pageable -&gt; Device)', 'stream': 7, 'mean_duration_us': 0.8}]</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
@@ -14027,12 +14027,12 @@
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.008999999999999), 'mean_duration_us': np.float64(1.4017999999999997), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.08894132897590411), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.504)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::bfloat16_copy_kernel_cuda(at::TensorIteratorBase&amp;)::{lambda(float)#1}, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.008999999999999, 'mean_duration_us': 1.4017999999999997, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.08894132897590411, 'min_duration_us': 1.28, 'max_duration_us': 1.504}]</t>
         </is>
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bf...', 'stream': 7, 'mean_duration_us': np.float64(1.4)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::bf...', 'stream': 7, 'mean_duration_us': 1.4}]</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
@@ -14147,12 +14147,12 @@
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(6.687999999999999), 'mean_duration_us': np.float64(1.3375999999999997), 'median_duration_us': np.float64(1.408), 'std_dev_duration_us': np.float64(0.0868138237840034), 'min_duration_us': np.float64(1.216), 'max_duration_us': np.float64(1.408)}]</t>
+          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'count': 5, 'total_duration_us': 6.687999999999999, 'mean_duration_us': 1.3375999999999997, 'median_duration_us': 1.408, 'std_dev_duration_us': 0.0868138237840034, 'min_duration_us': 1.216, 'max_duration_us': 1.408}]</t>
         </is>
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'mean_duration_us': np.float64(1.34)}]</t>
+          <t>[{'name': 'Memcpy DtoD (Device -&gt; Device)', 'stream': 7, 'mean_duration_us': 1.34}]</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
@@ -14208,28 +14208,32 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>(1, 3, 1008, 1008)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>('float', None)</t>
+          <t>('c10::BFloat16', 'float')</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>()</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
+          <t>(3048192, 1016064, 1008, 1)</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>(3048192, 1016064, 1008, 1)</t>
+        </is>
+      </c>
       <c r="F29" t="n">
-        <v>1e-09</v>
+        <v>0.003048192</v>
       </c>
       <c r="G29" t="n">
-        <v>7.62939453125e-06</v>
+        <v>17.44189453125</v>
       </c>
       <c r="H29" t="n">
-        <v>0.125</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
@@ -14249,17 +14253,17 @@
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr">
         <is>
-          <t>[[], [], []]</t>
+          <t>[[1, 3, 1008, 1008], [1, 3, 1008, 1008], []]</t>
         </is>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>['float', 'double', 'Scalar']</t>
+          <t>['c10::BFloat16', 'float', 'Scalar']</t>
         </is>
       </c>
       <c r="W29" t="inlineStr">
         <is>
-          <t>[[], [], []]</t>
+          <t>[[3048192, 1016064, 1008, 1], [3048192, 1016064, 1008, 1], []]</t>
         </is>
       </c>
       <c r="X29" t="inlineStr">
@@ -14289,43 +14293,39 @@
         <v>5</v>
       </c>
       <c r="AF29" t="n">
-        <v>23848</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>aten::copy_</t>
+          <t>aten::sigmoid</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>(1, 3, 1008, 1008)</t>
+          <t>(1, 5184)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>('c10::BFloat16', 'float')</t>
+          <t>('float', None)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>(3048192, 1016064, 1008, 1)</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>(3048192, 1016064, 1008, 1)</t>
-        </is>
-      </c>
+          <t>(5184, 1)</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>0.003048192</v>
+        <v>5.184e-06</v>
       </c>
       <c r="G30" t="n">
-        <v>17.44189453125</v>
+        <v>0.03955078125</v>
       </c>
       <c r="H30" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
@@ -14345,22 +14345,22 @@
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr">
         <is>
-          <t>[[1, 3, 1008, 1008], [1, 3, 1008, 1008], []]</t>
+          <t>[[1, 5184]]</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>['c10::BFloat16', 'float', 'Scalar']</t>
+          <t>['float']</t>
         </is>
       </c>
       <c r="W30" t="inlineStr">
         <is>
-          <t>[[3048192, 1016064, 1008, 1], [3048192, 1016064, 1008, 1], []]</t>
+          <t>[[5184, 1]]</t>
         </is>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>['', '', 'False']</t>
+          <t>['']</t>
         </is>
       </c>
       <c r="Y30" t="n">
@@ -14385,7 +14385,7 @@
         <v>5</v>
       </c>
       <c r="AF30" t="n">
-        <v>22</v>
+        <v>23763</v>
       </c>
     </row>
     <row r="31">
@@ -14396,29 +14396,29 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>(1, 1, 4)</t>
+          <t>()</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>('c10::BFloat16', 'int')</t>
+          <t>('c10::BFloat16', None)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>(4, 4, 1)</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>(4, 4, 1)</t>
-        </is>
-      </c>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
-        <v>4e-09</v>
-      </c>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
+        <v>1e-09</v>
+      </c>
+      <c r="G31" t="n">
+        <v>3.814697265625e-06</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.25</v>
+      </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
@@ -14437,17 +14437,17 @@
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr">
         <is>
-          <t>[[1, 1, 4], [1, 1, 4], []]</t>
+          <t>[[], [], []]</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>['c10::BFloat16', 'int', 'Scalar']</t>
+          <t>['c10::BFloat16', 'double', 'Scalar']</t>
         </is>
       </c>
       <c r="W31" t="inlineStr">
         <is>
-          <t>[[4, 4, 1], [4, 4, 1], []]</t>
+          <t>[[], [], []]</t>
         </is>
       </c>
       <c r="X31" t="inlineStr">
@@ -14474,10 +14474,10 @@
         <v>0</v>
       </c>
       <c r="AE31" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AF31" t="n">
-        <v>23834</v>
+        <v>23777</v>
       </c>
     </row>
     <row r="32">
@@ -14488,29 +14488,29 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>(1, 1, 4)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>('c10::BFloat16', None)</t>
+          <t>('c10::BFloat16', 'int')</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>()</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>(4, 4, 1)</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>(4, 4, 1)</t>
+        </is>
+      </c>
       <c r="F32" t="n">
-        <v>1e-09</v>
-      </c>
-      <c r="G32" t="n">
-        <v>3.814697265625e-06</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0.25</v>
-      </c>
+        <v>4e-09</v>
+      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
@@ -14529,17 +14529,17 @@
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr">
         <is>
-          <t>[[], [], []]</t>
+          <t>[[1, 1, 4], [1, 1, 4], []]</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>['c10::BFloat16', 'double', 'Scalar']</t>
+          <t>['c10::BFloat16', 'int', 'Scalar']</t>
         </is>
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>[[], [], []]</t>
+          <t>[[4, 4, 1], [4, 4, 1], []]</t>
         </is>
       </c>
       <c r="X32" t="inlineStr">
@@ -14566,21 +14566,21 @@
         <v>0</v>
       </c>
       <c r="AE32" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AF32" t="n">
-        <v>23777</v>
+        <v>23834</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>aten::sigmoid</t>
+          <t>aten::copy_</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>(1, 5184)</t>
+          <t>()</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -14590,15 +14590,15 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>(5184, 1)</t>
+          <t>()</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
-        <v>5.184e-06</v>
+        <v>1e-09</v>
       </c>
       <c r="G33" t="n">
-        <v>0.03955078125</v>
+        <v>7.62939453125e-06</v>
       </c>
       <c r="H33" t="n">
         <v>0.125</v>
@@ -14621,22 +14621,22 @@
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr">
         <is>
-          <t>[[1, 5184]]</t>
+          <t>[[], [], []]</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>['float']</t>
+          <t>['float', 'double', 'Scalar']</t>
         </is>
       </c>
       <c r="W33" t="inlineStr">
         <is>
-          <t>[[5184, 1]]</t>
+          <t>[[], [], []]</t>
         </is>
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>['']</t>
+          <t>['', '', 'False']</t>
         </is>
       </c>
       <c r="Y33" t="n">
@@ -14661,7 +14661,7 @@
         <v>5</v>
       </c>
       <c r="AF33" t="n">
-        <v>23763</v>
+        <v>23848</v>
       </c>
     </row>
   </sheetData>
@@ -14928,12 +14928,12 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(5223.73), 'mean_duration_us': np.float64(43.53108333333333), 'median_duration_us': np.float64(43.3595), 'std_dev_duration_us': np.float64(0.6410638629566389), 'min_duration_us': np.float64(42.656), 'max_duration_us': np.float64(44.704)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 5223.73, 'mean_duration_us': 43.53108333333333, 'median_duration_us': 43.3595, 'std_dev_duration_us': 0.6410638629566389, 'min_duration_us': 42.656, 'max_duration_us': 44.704}]</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(43.53)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 43.53}]</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
@@ -15054,12 +15054,12 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(3687.3240000000005), 'mean_duration_us': np.float64(30.727700000000006), 'median_duration_us': np.float64(30.591), 'std_dev_duration_us': np.float64(0.3214868737600341), 'min_duration_us': np.float64(30.336), 'max_duration_us': np.float64(31.711)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 3687.3240000000005, 'mean_duration_us': 30.727700000000006, 'median_duration_us': 30.591, 'std_dev_duration_us': 0.3214868737600341, 'min_duration_us': 30.336, 'max_duration_us': 31.711}]</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(30.73)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 30.73}]</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
@@ -15180,12 +15180,12 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 245, 'total_duration_us': np.float64(2317.353), 'mean_duration_us': np.float64(9.458583673469388), 'median_duration_us': np.float64(9.472), 'std_dev_duration_us': np.float64(0.3348456698101192), 'min_duration_us': np.float64(8.576), 'max_duration_us': np.float64(10.849)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 245, 'total_duration_us': 2317.353, 'mean_duration_us': 9.458583673469388, 'median_duration_us': 9.472, 'std_dev_duration_us': 0.3348456698101192, 'min_duration_us': 8.576, 'max_duration_us': 10.849}]</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(9.46)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 9.46}]</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
@@ -15306,12 +15306,12 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(934.809), 'mean_duration_us': np.float64(7.790075), 'median_duration_us': np.float64(7.776), 'std_dev_duration_us': np.float64(0.06863528763204346), 'min_duration_us': np.float64(7.711), 'max_duration_us': np.float64(8.032)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 120, 'total_duration_us': 934.809, 'mean_duration_us': 7.790075, 'median_duration_us': 7.776, 'std_dev_duration_us': 0.06863528763204346, 'min_duration_us': 7.711, 'max_duration_us': 8.032}]</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(7.79)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 7.79}]</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -15432,12 +15432,12 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': np.float64(287.13699999999994), 'mean_duration_us': np.float64(2.392808333333333), 'median_duration_us': np.float64(2.368), 'std_dev_duration_us': np.float64(0.24387456802740948), 'min_duration_us': np.float64(1.984), 'max_duration_us': np.float64(2.913)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; &gt;(at::TensorIteratorBase&amp;, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 120, 'total_duration_us': 287.13699999999994, 'mean_duration_us': 2.392808333333333, 'median_duration_us': 2.368, 'std_dev_duration_us': 0.24387456802740948, 'min_duration_us': 1.984, 'max_duration_us': 2.913}]</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.39)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.39}]</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
@@ -15558,12 +15558,12 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 125, 'total_duration_us': np.float64(187.747), 'mean_duration_us': np.float64(1.5019760000000002), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.09206636423797784), 'min_duration_us': np.float64(1.344), 'max_duration_us': np.float64(1.633)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 125, 'total_duration_us': 187.747, 'mean_duration_us': 1.5019760000000002, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.09206636423797784, 'min_duration_us': 1.344, 'max_duration_us': 1.633}]</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.5)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.5}]</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
@@ -15684,12 +15684,12 @@
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(94.07899999999998), 'mean_duration_us': np.float64(1.567983333333333), 'median_duration_us': np.float64(1.568), 'std_dev_duration_us': np.float64(0.02925092116308288), 'min_duration_us': np.float64(1.535), 'max_duration_us': np.float64(1.633)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 94.07899999999998, 'mean_duration_us': 1.567983333333333, 'median_duration_us': 1.568, 'std_dev_duration_us': 0.02925092116308288, 'min_duration_us': 1.535, 'max_duration_us': 1.633}]</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(1.57)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 1.57}]</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -15810,12 +15810,12 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(89.14699999999999), 'mean_duration_us': np.float64(1.4857833333333332), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.016880058912482752), 'min_duration_us': np.float64(1.471), 'max_duration_us': np.float64(1.535)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 89.14699999999999, 'mean_duration_us': 1.4857833333333332, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.016880058912482752, 'min_duration_us': 1.471, 'max_duration_us': 1.535}]</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(1.49)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 1.49}]</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -15936,12 +15936,12 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': np.float64(86.49500000000002), 'mean_duration_us': np.float64(1.4415833333333337), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.10003121040733015), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.568)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::AUnaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 60, 'total_duration_us': 86.49500000000002, 'mean_duration_us': 1.4415833333333337, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.10003121040733015, 'min_duration_us': 1.28, 'max_duration_us': 1.568}]</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': np.float64(1.44)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::AU...', 'stream': 7, 'mean_duration_us': 1.44}]</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
@@ -16062,12 +16062,12 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(65.407), 'mean_duration_us': np.float64(13.081399999999999), 'median_duration_us': np.float64(13.088), 'std_dev_duration_us': np.float64(0.058854396607220374), 'min_duration_us': np.float64(13.023), 'max_duration_us': np.float64(13.184)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 65.407, 'mean_duration_us': 13.081399999999999, 'median_duration_us': 13.088, 'std_dev_duration_us': 0.058854396607220374, 'min_duration_us': 13.023, 'max_duration_us': 13.184}]</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(13.08)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 13.08}]</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
@@ -16188,12 +16188,12 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(57.631), 'mean_duration_us': np.float64(11.5262), 'median_duration_us': np.float64(11.552), 'std_dev_duration_us': np.float64(0.0889413289759043), 'min_duration_us': np.float64(11.392), 'max_duration_us': np.float64(11.616)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 57.631, 'mean_duration_us': 11.5262, 'median_duration_us': 11.552, 'std_dev_duration_us': 0.0889413289759043, 'min_duration_us': 11.392, 'max_duration_us': 11.616}]</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(11.53)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 11.53}]</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
@@ -16314,12 +16314,12 @@
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 10, 'total_duration_us': np.float64(26.686999999999998), 'mean_duration_us': np.float64(2.6687), 'median_duration_us': np.float64(2.656), 'std_dev_duration_us': np.float64(0.20862696374150683), 'min_duration_us': np.float64(2.335), 'max_duration_us': np.float64(3.008)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 10, 'total_duration_us': 26.686999999999998, 'mean_duration_us': 2.6687, 'median_duration_us': 2.656, 'std_dev_duration_us': 0.20862696374150683, 'min_duration_us': 2.335, 'max_duration_us': 3.008}]</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.67)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.67}]</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
@@ -16440,12 +16440,12 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, 4, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(22.144000000000002), 'mean_duration_us': np.float64(4.428800000000001), 'median_duration_us': np.float64(4.416), 'std_dev_duration_us': np.float64(0.09621309682158638), 'min_duration_us': np.float64(4.32), 'max_duration_us': np.float64(4.608)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, 4, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt; &gt;(int, at::native::CUDAFunctor_add&lt;float&gt;, std::array&lt;char*, 3ul&gt;, TrivialOffsetCalculator&lt;2, unsigned int&gt;, TrivialOffsetCalculator&lt;1, unsigned int&gt;, at::native::memory::LoadWithCast&lt;2&gt;, at::native::memory::StoreWithCast&lt;1&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 22.144000000000002, 'mean_duration_us': 4.428800000000001, 'median_duration_us': 4.416, 'std_dev_duration_us': 0.09621309682158638, 'min_duration_us': 4.32, 'max_duration_us': 4.608}]</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFun...', 'stream': 7, 'mean_duration_us': np.float64(4.43)}]</t>
+          <t>[{'name': 'void at::native::unrolled_elementwise_kernel&lt;at::native::CUDAFun...', 'stream': 7, 'mean_duration_us': 4.43}]</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
@@ -16566,12 +16566,12 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(14.560000000000002), 'mean_duration_us': np.float64(2.9120000000000004), 'median_duration_us': np.float64(3.008), 'std_dev_duration_us': np.float64(0.21891368161903446), 'min_duration_us': np.float64(2.656), 'max_duration_us': np.float64(3.2)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1}&gt;(int, at::native::gpu_kernel_impl_nocast&lt;at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; &gt;(at::TensorIteratorBase&amp;, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::DivFunctor&lt;c10::BFloat16&gt; &gt; const&amp;)::{lambda(int)#1})', 'stream': 7, 'count': 5, 'total_duration_us': 14.560000000000002, 'mean_duration_us': 2.9120000000000004, 'median_duration_us': 3.008, 'std_dev_duration_us': 0.21891368161903446, 'min_duration_us': 2.656, 'max_duration_us': 3.2}]</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': np.float64(2.91)}]</t>
+          <t>[{'name': 'void at::native::elementwise_kernel&lt;128, 4, at::native::gpu_kern...', 'stream': 7, 'mean_duration_us': 2.91}]</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
@@ -16692,12 +16692,12 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.799), 'mean_duration_us': np.float64(1.7597999999999998), 'median_duration_us': np.float64(1.76), 'std_dev_duration_us': np.float64(0.10100376230616363), 'min_duration_us': np.float64(1.632), 'max_duration_us': np.float64(1.888)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.799, 'mean_duration_us': 1.7597999999999998, 'median_duration_us': 1.76, 'std_dev_duration_us': 0.10100376230616363, 'min_duration_us': 1.632, 'max_duration_us': 1.888}]</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.76)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.76}]</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
@@ -16818,12 +16818,12 @@
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(8.030999999999999), 'mean_duration_us': np.float64(1.6061999999999999), 'median_duration_us': np.float64(1.632), 'std_dev_duration_us': np.float64(0.046786322787754936), 'min_duration_us': np.float64(1.536), 'max_duration_us': np.float64(1.663)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 8.030999999999999, 'mean_duration_us': 1.6061999999999999, 'median_duration_us': 1.632, 'std_dev_duration_us': 0.046786322787754936, 'min_duration_us': 1.536, 'max_duration_us': 1.663}]</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.61)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.61}]</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
@@ -16944,12 +16944,12 @@
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.872), 'mean_duration_us': np.float64(1.5744), 'median_duration_us': np.float64(1.568), 'std_dev_duration_us': np.float64(0.02394660727535325), 'min_duration_us': np.float64(1.536), 'max_duration_us': np.float64(1.6)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::CUDAFunctor_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.872, 'mean_duration_us': 1.5744, 'median_duration_us': 1.568, 'std_dev_duration_us': 0.02394660727535325, 'min_duration_us': 1.536, 'max_duration_us': 1.6}]</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.57)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.57}]</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
@@ -17070,12 +17070,12 @@
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.744), 'mean_duration_us': np.float64(1.5488), 'median_duration_us': np.float64(1.6), 'std_dev_duration_us': np.float64(0.09185728060420688), 'min_duration_us': np.float64(1.408), 'max_duration_us': np.float64(1.632)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;long&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.744, 'mean_duration_us': 1.5488, 'median_duration_us': 1.6, 'std_dev_duration_us': 0.09185728060420688, 'min_duration_us': 1.408, 'max_duration_us': 1.632}]</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.55)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.55}]</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
@@ -17196,12 +17196,12 @@
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.424999999999999), 'mean_duration_us': np.float64(1.4849999999999999), 'median_duration_us': np.float64(1.472), 'std_dev_duration_us': np.float64(0.025502941006872143), 'min_duration_us': np.float64(1.472), 'max_duration_us': np.float64(1.536)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.424999999999999, 'mean_duration_us': 1.4849999999999999, 'median_duration_us': 1.472, 'std_dev_duration_us': 0.025502941006872143, 'min_duration_us': 1.472, 'max_duration_us': 1.536}]</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(1.48)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 1.48}]</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
@@ -17322,12 +17322,12 @@
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.264999999999999), 'mean_duration_us': np.float64(1.4529999999999998), 'median_duration_us': np.float64(1.441), 'std_dev_duration_us': np.float64(0.015517731793016656), 'min_duration_us': np.float64(1.44), 'max_duration_us': np.float64(1.472)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt; &gt;(int, at::native::CUDAFunctorOnSelf_add&lt;c10::BFloat16&gt;, std::array&lt;char*, 2ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.264999999999999, 'mean_duration_us': 1.4529999999999998, 'median_duration_us': 1.441, 'std_dev_duration_us': 0.015517731793016656, 'min_duration_us': 1.44, 'max_duration_us': 1.472}]</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': np.float64(1.45)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::CU...', 'stream': 7, 'mean_duration_us': 1.45}]</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
@@ -17448,12 +17448,12 @@
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': np.float64(7.007999999999999), 'mean_duration_us': np.float64(1.4015999999999997), 'median_duration_us': np.float64(1.44), 'std_dev_duration_us': np.float64(0.08914168497397834), 'min_duration_us': np.float64(1.28), 'max_duration_us': np.float64(1.504)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt; &gt;(int, at::native::BinaryFunctor&lt;c10::BFloat16, c10::BFloat16, c10::BFloat16, at::native::binary_internal::MulFunctor&lt;float&gt; &gt;, std::array&lt;char*, 3ul&gt;)', 'stream': 7, 'count': 5, 'total_duration_us': 7.007999999999999, 'mean_duration_us': 1.4015999999999997, 'median_duration_us': 1.44, 'std_dev_duration_us': 0.08914168497397834, 'min_duration_us': 1.28, 'max_duration_us': 1.504}]</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': np.float64(1.4)}]</t>
+          <t>[{'name': 'void at::native::vectorized_elementwise_kernel&lt;4, at::native::Bi...', 'stream': 7, 'mean_duration_us': 1.4}]</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
@@ -17504,7 +17504,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>aten::add</t>
+          <t>aten::mul</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -17514,12 +17514,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>(1, 5184)</t>
+          <t>()</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>('c10::BFloat16', 'c10::BFloat16', None)</t>
+          <t>('c10::BFloat16', 'double', None)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -17529,7 +17529,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>(5184, 1)</t>
+          <t>()</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -17537,10 +17537,10 @@
         <v>5.184e-06</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0296630859375</v>
+        <v>0.01978302001953125</v>
       </c>
       <c r="J23" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.2499035865792518</v>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
@@ -17560,22 +17560,22 @@
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr">
         <is>
-          <t>[[1, 5184], [1, 5184], []]</t>
+          <t>[[1, 5184], []]</t>
         </is>
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>['c10::BFloat16', 'c10::BFloat16', 'Scalar']</t>
+          <t>['c10::BFloat16', 'double']</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>[[20736, 4], [5184, 1], []]</t>
+          <t>[[20736, 4], []]</t>
         </is>
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>['', '', '1']</t>
+          <t>['', '']</t>
         </is>
       </c>
       <c r="AA23" t="n">
@@ -17597,49 +17597,53 @@
         <v>0</v>
       </c>
       <c r="AG23" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AH23" t="n">
-        <v>23790</v>
+        <v>23773</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>aten::mul</t>
+          <t>aten::add</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>(1, 5184, 4)</t>
+          <t>(1, 5184)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>(1, 1, 4)</t>
+          <t>(1, 5184)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>('c10::BFloat16', 'int', None)</t>
+          <t>('c10::BFloat16', 'c10::BFloat16', None)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>(20736, 4, 1)</t>
+          <t>(20736, 4)</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>(4, 4, 1)</t>
+          <t>(5184, 1)</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
-        <v>2.0736e-05</v>
-      </c>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+        <v>5.184e-06</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.0296630859375</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
@@ -17658,22 +17662,22 @@
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr">
         <is>
-          <t>[[1, 5184, 4], [1, 1, 4]]</t>
+          <t>[[1, 5184], [1, 5184], []]</t>
         </is>
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>['c10::BFloat16', 'int']</t>
+          <t>['c10::BFloat16', 'c10::BFloat16', 'Scalar']</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
         <is>
-          <t>[[20736, 4, 1], [4, 4, 1]]</t>
+          <t>[[20736, 4], [5184, 1], []]</t>
         </is>
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>['', '']</t>
+          <t>['', '', '1']</t>
         </is>
       </c>
       <c r="AA24" t="n">
@@ -17695,10 +17699,10 @@
         <v>0</v>
       </c>
       <c r="AG24" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AH24" t="n">
-        <v>23830</v>
+        <v>23790</v>
       </c>
     </row>
     <row r="25">
@@ -17709,39 +17713,35 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>(1, 5184)</t>
+          <t>(1, 5184, 4)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>(1, 1, 4)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>('c10::BFloat16', 'double', None)</t>
+          <t>('c10::BFloat16', 'int', None)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>(20736, 4)</t>
+          <t>(20736, 4, 1)</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>(4, 4, 1)</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
-        <v>5.184e-06</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0.01978302001953125</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0.2499035865792518</v>
-      </c>
+        <v>2.0736e-05</v>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
@@ -17760,17 +17760,17 @@
       <c r="V25" t="inlineStr"/>
       <c r="W25" t="inlineStr">
         <is>
-          <t>[[1, 5184], []]</t>
+          <t>[[1, 5184, 4], [1, 1, 4]]</t>
         </is>
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>['c10::BFloat16', 'double']</t>
+          <t>['c10::BFloat16', 'int']</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>[[20736, 4], []]</t>
+          <t>[[20736, 4, 1], [4, 4, 1]]</t>
         </is>
       </c>
       <c r="Z25" t="inlineStr">
@@ -17797,10 +17797,10 @@
         <v>0</v>
       </c>
       <c r="AG25" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AH25" t="n">
-        <v>23773</v>
+        <v>23830</v>
       </c>
     </row>
   </sheetData>

</xml_diff>